<commit_message>
Delete unnecessary files and update table formatting
</commit_message>
<xml_diff>
--- a/Lab 1 - Pumps/data_and_analysis.xlsx
+++ b/Lab 1 - Pumps/data_and_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdiep\OneDrive\Documents\LaTeX\MEC-E-403\Lab 1 - Pumps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\LaTeX\MEC-E-403\Lab 1 - Pumps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4A8B0F-3F76-48BB-8380-9D826890B19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F23CAD1-CBFB-4646-9A70-983795235ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="seans analysis" sheetId="6" state="hidden" r:id="rId1"/>
@@ -343,7 +343,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -354,6 +354,7 @@
     <numFmt numFmtId="171" formatCode="#,##0.0000;\-#,##0.0000;\-"/>
     <numFmt numFmtId="172" formatCode="#,##0.00000;\-#,##0.00000;\-"/>
     <numFmt numFmtId="173" formatCode="#,##0.000000;\-#,##0.000000;\-"/>
+    <numFmt numFmtId="176" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -404,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -489,6 +490,12 @@
     <xf numFmtId="172" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -497,6 +504,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,43 +729,43 @@
       <selection activeCell="B14" sqref="B14:AI27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="9" width="7.1796875" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" style="15" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" style="3" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="8.1796875" style="3" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16.54296875" style="3" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="3" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="9" width="7.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="15" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="8.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" style="3" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="3" hidden="1" customWidth="1"/>
-    <col min="16" max="17" width="5.81640625" style="3" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1796875" style="3" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="8.81640625" style="3" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" style="3"/>
-    <col min="21" max="21" width="13.26953125" style="3" hidden="1" customWidth="1"/>
-    <col min="22" max="23" width="10.81640625" style="3"/>
-    <col min="24" max="25" width="12.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="21.54296875" style="3" hidden="1" customWidth="1"/>
-    <col min="28" max="29" width="22.81640625" style="3" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.7265625" style="3" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="16.7265625" style="3" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="5.81640625" style="3" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="13.7265625" style="3" customWidth="1"/>
-    <col min="35" max="35" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="5.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" style="3"/>
+    <col min="21" max="21" width="13.28515625" style="3" hidden="1" customWidth="1"/>
+    <col min="22" max="23" width="10.85546875" style="3"/>
+    <col min="24" max="25" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="21.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="28" max="29" width="22.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="5.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="13.7109375" style="3" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.81640625" style="3"/>
-    <col min="40" max="16384" width="10.81640625" style="2"/>
+    <col min="37" max="37" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.85546875" style="3"/>
+    <col min="40" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -766,7 +776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -777,7 +787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -794,7 +804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -805,7 +815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -817,7 +827,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -829,7 +839,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -844,7 +854,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -856,7 +866,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -867,7 +877,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -875,11 +885,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -890,44 +900,44 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="30" t="s">
+    <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="G13" s="31" t="s">
+      <c r="E13" s="32"/>
+      <c r="G13" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="L13" s="30" t="s">
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="L13" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="30"/>
+      <c r="M13" s="32"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="31" t="s">
+      <c r="Z13" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="31"/>
-      <c r="AB13" s="31" t="s">
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="31"/>
-      <c r="AD13" s="31" t="s">
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="31"/>
-      <c r="AF13" s="31" t="s">
+      <c r="AE13" s="33"/>
+      <c r="AF13" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="31"/>
-    </row>
-    <row r="14" spans="1:39" s="16" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="AG13" s="33"/>
+    </row>
+    <row r="14" spans="1:39" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>62</v>
       </c>
@@ -946,11 +956,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -1042,7 +1052,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
         <v>19</v>
@@ -1142,7 +1152,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>63</v>
       </c>
@@ -1285,7 +1295,7 @@
         <v>1.1386694065108405E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -1428,7 +1438,7 @@
         <v>1.4656802692797793E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>63</v>
       </c>
@@ -1571,7 +1581,7 @@
         <v>2.08923219219989E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>63</v>
       </c>
@@ -1713,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -1856,7 +1866,7 @@
         <v>1.0885097083115679E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1999,7 +2009,7 @@
         <v>5.621711746058875E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -2142,7 +2152,7 @@
         <v>2.018123697163367E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>63</v>
       </c>
@@ -2284,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -2427,7 +2437,7 @@
         <v>6.6059364133894301E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -2570,7 +2580,7 @@
         <v>7.1265663822810228E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -2713,7 +2723,7 @@
         <v>3.8699281683984957E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>63</v>
       </c>
@@ -2855,7 +2865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>64</v>
       </c>
@@ -2998,7 +3008,7 @@
         <v>5.36705638526906E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>64</v>
       </c>
@@ -3141,7 +3151,7 @@
         <v>3.8267632171597936E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>64</v>
       </c>
@@ -3284,7 +3294,7 @@
         <v>6.2844409454881163E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>64</v>
       </c>
@@ -3426,7 +3436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>78</v>
       </c>
@@ -3569,7 +3579,7 @@
         <v>2.217152366422431E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
@@ -3712,7 +3722,7 @@
         <v>4.2659741283684249E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
@@ -3855,7 +3865,7 @@
         <v>1.0008544761487808E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>78</v>
       </c>
@@ -3997,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>63</v>
       </c>
@@ -4137,7 +4147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>63</v>
       </c>
@@ -4277,7 +4287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>63</v>
       </c>
@@ -4417,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>63</v>
       </c>
@@ -4557,7 +4567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>63</v>
       </c>
@@ -4697,7 +4707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>63</v>
       </c>
@@ -4837,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>63</v>
       </c>
@@ -4977,7 +4987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>63</v>
       </c>
@@ -5117,7 +5127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>63</v>
       </c>
@@ -5257,7 +5267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>63</v>
       </c>
@@ -5397,7 +5407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>63</v>
       </c>
@@ -5537,7 +5547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>63</v>
       </c>
@@ -5677,7 +5687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
@@ -5817,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>63</v>
       </c>
@@ -5957,7 +5967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="6"/>
@@ -5966,12 +5976,12 @@
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="33"/>
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="6"/>
@@ -5983,7 +5993,7 @@
       <c r="M51" s="8"/>
       <c r="N51" s="8"/>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="6"/>
@@ -5992,24 +6002,24 @@
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
-      <c r="K52" s="31"/>
-      <c r="L52" s="31"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="33"/>
       <c r="M52" s="8"/>
       <c r="N52" s="8"/>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M53" s="8"/>
       <c r="N53" s="8"/>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M54" s="8"/>
       <c r="N54" s="8"/>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M55" s="8"/>
       <c r="N55" s="8"/>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>79</v>
       </c>
@@ -6020,7 +6030,7 @@
       <c r="M56" s="8"/>
       <c r="N56" s="8"/>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57" s="2" t="s">
         <v>80</v>
@@ -6032,61 +6042,61 @@
       <c r="M57" s="8"/>
       <c r="N57" s="8"/>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58"/>
       <c r="C58" s="26"/>
       <c r="M58" s="8"/>
       <c r="N58" s="8"/>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A59" s="30"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
+    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A59" s="32"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="30"/>
-      <c r="K59" s="31"/>
-      <c r="L59" s="31"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="K59" s="33"/>
+      <c r="L59" s="33"/>
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A60" s="30"/>
-      <c r="B60" s="31"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
+    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A60" s="32"/>
+      <c r="B60" s="33"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
       <c r="M60" s="8"/>
       <c r="N60" s="8"/>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A61" s="30"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="31"/>
-      <c r="H61" s="31"/>
-      <c r="K61" s="31"/>
-      <c r="L61" s="31"/>
+    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A61" s="32"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="33"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="33"/>
       <c r="M61" s="8"/>
       <c r="N61" s="8"/>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M62" s="8"/>
       <c r="N62" s="8"/>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M63" s="8"/>
       <c r="N63" s="8"/>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M64" s="8"/>
       <c r="N64" s="8"/>
     </row>
-    <row r="65" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M65" s="8"/>
       <c r="N65" s="8"/>
     </row>
@@ -6120,50 +6130,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B530A311-2D6F-44F7-871F-14AF58E6CD82}">
   <dimension ref="A1:AO106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H103" sqref="H103"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AO41" sqref="AO16:AO41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.08984375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="32.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="21.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="32.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.81640625" style="3"/>
-    <col min="40" max="16384" width="10.81640625" style="2"/>
+    <col min="38" max="38" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.85546875" style="3"/>
+    <col min="40" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6174,7 +6184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -6185,7 +6195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -6202,7 +6212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6213,7 +6223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -6225,7 +6235,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -6237,7 +6247,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -6252,7 +6262,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -6264,7 +6274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -6275,7 +6285,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -6284,11 +6294,11 @@
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -6299,47 +6309,47 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D13" s="30" t="s">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="D13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="G13" s="31" t="s">
+      <c r="E13" s="32"/>
+      <c r="G13" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="L13" s="30" t="s">
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="L13" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="30"/>
+      <c r="M13" s="32"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="31" t="s">
+      <c r="Z13" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="31"/>
-      <c r="AB13" s="31" t="s">
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="31"/>
-      <c r="AD13" s="31" t="s">
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="31"/>
-      <c r="AF13" s="31" t="s">
+      <c r="AE13" s="33"/>
+      <c r="AF13" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="31"/>
+      <c r="AG13" s="33"/>
       <c r="AO13" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:41" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>62</v>
       </c>
@@ -6358,11 +6368,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -6460,7 +6470,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
         <v>19</v>
@@ -6567,7 +6577,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>63</v>
       </c>
@@ -6718,7 +6728,7 @@
         <v>37.010451746090069</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -6869,7 +6879,7 @@
         <v>39.406990455603598</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>63</v>
       </c>
@@ -7020,7 +7030,7 @@
         <v>36.959072152593905</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>63</v>
       </c>
@@ -7170,7 +7180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -7321,7 +7331,7 @@
         <v>40.916592886771006</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -7472,7 +7482,7 @@
         <v>42.673982331632686</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -7623,7 +7633,7 @@
         <v>49.917307149111032</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>63</v>
       </c>
@@ -7773,7 +7783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -7924,7 +7934,7 @@
         <v>41.834907330788297</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -8075,7 +8085,7 @@
         <v>46.567659646009965</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -8226,7 +8236,7 @@
         <v>44.898280449625048</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>63</v>
       </c>
@@ -8376,7 +8386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
@@ -8515,8 +8525,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="AO28" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>63</v>
       </c>
@@ -8655,8 +8668,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="AO29" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>63</v>
       </c>
@@ -8795,8 +8811,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="AO30" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -8935,8 +8954,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="AO31" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -9075,8 +9097,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO32" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -9215,8 +9240,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO33" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -9355,8 +9383,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO34" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>63</v>
       </c>
@@ -9495,8 +9526,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO35" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>63</v>
       </c>
@@ -9635,8 +9669,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO36" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>63</v>
       </c>
@@ -9775,8 +9812,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO37" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>63</v>
       </c>
@@ -9915,8 +9955,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO38" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>63</v>
       </c>
@@ -10055,8 +10098,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO39" s="3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>63</v>
       </c>
@@ -10195,8 +10241,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO40" s="6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>63</v>
       </c>
@@ -10335,8 +10384,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AO41" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>64</v>
       </c>
@@ -10479,7 +10531,7 @@
         <v>9.5838558336299937E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>64</v>
       </c>
@@ -10622,7 +10674,7 @@
         <v>2.3832863165935709E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>64</v>
       </c>
@@ -10765,7 +10817,7 @@
         <v>2.885476835244572E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>64</v>
       </c>
@@ -10907,7 +10959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>78</v>
       </c>
@@ -11050,7 +11102,7 @@
         <v>6.8838316713215981E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>78</v>
       </c>
@@ -11193,7 +11245,7 @@
         <v>2.4457004676063047E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>78</v>
       </c>
@@ -11336,7 +11388,7 @@
         <v>1.4174356021315262E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>78</v>
       </c>
@@ -11478,7 +11530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>79</v>
       </c>
@@ -11487,28 +11539,28 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="22">
+      <c r="B52" s="35">
         <f>_xlfn.COT(RADIANS(B51))</f>
         <v>1.5398649638145827</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="C54" s="31" t="s">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C54" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31" t="s">
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-    </row>
-    <row r="55" spans="1:39" ht="31" x14ac:dyDescent="0.35">
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+    </row>
+    <row r="55" spans="1:39" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">
         <v>22</v>
       </c>
@@ -11528,7 +11580,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>64</v>
       </c>
@@ -11560,7 +11612,7 @@
         <v>7.8117123467137377</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -11592,7 +11644,7 @@
         <v>8.1227188682608311</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>64</v>
       </c>
@@ -11624,7 +11676,7 @@
         <v>11.261066993909452</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
@@ -11656,7 +11708,7 @@
         <v>12.394593059717804</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>78</v>
       </c>
@@ -11688,7 +11740,7 @@
         <v>11.196055013314581</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>78</v>
       </c>
@@ -11720,7 +11772,7 @@
         <v>12.013256797832247</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>78</v>
       </c>
@@ -11752,7 +11804,7 @@
         <v>20.931795524684208</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>78</v>
       </c>
@@ -11784,11 +11836,11 @@
         <v>24.789186119435609</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
     </row>
-    <row r="65" spans="1:14" ht="62" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>90</v>
       </c>
@@ -11826,7 +11878,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C66" s="3" t="s">
         <v>29</v>
       </c>
@@ -11852,14 +11904,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B67" s="3">
         <v>0.108</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="22">
         <f>$B$8</f>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -11867,87 +11919,87 @@
         <f>$B$9</f>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E67" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F67" s="3">
         <v>3600</v>
       </c>
-      <c r="G67" s="3">
+      <c r="G67" s="8">
         <v>10.3</v>
       </c>
       <c r="H67" s="3">
         <v>52</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I67" s="8">
         <f>B67/2*F67*2*PI()/60</f>
         <v>20.357520395261862</v>
       </c>
-      <c r="J67" s="15">
+      <c r="J67" s="14">
         <f>E67/(C67*(2*PI()*B67/2-$B$10*D67))</f>
         <v>2.9949893162848213</v>
       </c>
-      <c r="K67" s="3">
+      <c r="K67" s="7">
         <f>G67*9.81/I67^2</f>
         <v>0.24381278479778079</v>
       </c>
-      <c r="L67" s="3">
+      <c r="L67" s="7">
         <f>J67/I67</f>
         <v>0.14711955376362507</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B68" s="3">
         <v>0.108</v>
       </c>
-      <c r="C68" s="3">
-        <f t="shared" ref="C68:C91" si="64">$B$8</f>
+      <c r="C68" s="22">
+        <f t="shared" ref="C68:C86" si="64">$B$8</f>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D68" s="3">
-        <f t="shared" ref="D68:D91" si="65">$B$9</f>
+        <f t="shared" ref="D68:D86" si="65">$B$9</f>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E68" s="10">
         <v>6.7000000000000002E-3</v>
       </c>
       <c r="F68" s="3">
         <v>3600</v>
       </c>
-      <c r="G68" s="3">
+      <c r="G68" s="8">
         <v>16.100000000000001</v>
       </c>
       <c r="H68" s="3">
         <v>71</v>
       </c>
-      <c r="I68" s="3">
+      <c r="I68" s="8">
         <f t="shared" ref="I68:I106" si="66">B68/2*F68*2*PI()/60</f>
         <v>20.357520395261862</v>
       </c>
-      <c r="J68" s="15">
+      <c r="J68" s="14">
         <f t="shared" ref="J68:J106" si="67">E68/(C68*(2*PI()*B68/2-$B$10*D68))</f>
         <v>2.5083035523885377</v>
       </c>
-      <c r="K68" s="3">
+      <c r="K68" s="7">
         <f t="shared" ref="K68:K106" si="68">G68*9.81/I68^2</f>
         <v>0.38110542089750205</v>
       </c>
-      <c r="L68" s="3">
+      <c r="L68" s="7">
         <f t="shared" ref="L68:L106" si="69">J68/I68</f>
         <v>0.123212626277036</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B69" s="3">
         <v>0.108</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -11955,45 +12007,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E69" s="3">
+      <c r="E69" s="10">
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="F69" s="3">
         <v>3600</v>
       </c>
-      <c r="G69" s="3">
+      <c r="G69" s="8">
         <v>19.399999999999999</v>
       </c>
       <c r="H69" s="3">
         <v>73</v>
       </c>
-      <c r="I69" s="3">
+      <c r="I69" s="8">
         <f t="shared" si="66"/>
         <v>20.357520395261862</v>
       </c>
-      <c r="J69" s="15">
+      <c r="J69" s="14">
         <f t="shared" si="67"/>
         <v>2.0216177884922546</v>
       </c>
-      <c r="K69" s="3">
+      <c r="K69" s="7">
         <f t="shared" si="68"/>
         <v>0.45922019660941232</v>
       </c>
-      <c r="L69" s="3">
+      <c r="L69" s="7">
         <f t="shared" si="69"/>
         <v>9.9305698790446928E-2</v>
       </c>
       <c r="M69" s="8"/>
       <c r="N69" s="8"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B70" s="3">
         <v>0.108</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12001,45 +12053,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E70" s="6">
+      <c r="E70" s="30">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F70" s="3">
         <v>3600</v>
       </c>
-      <c r="G70" s="6">
+      <c r="G70" s="31">
         <v>21.6</v>
       </c>
       <c r="H70" s="6">
         <v>69</v>
       </c>
-      <c r="I70" s="3">
+      <c r="I70" s="8">
         <f t="shared" si="66"/>
         <v>20.357520395261862</v>
       </c>
-      <c r="J70" s="15">
+      <c r="J70" s="14">
         <f t="shared" si="67"/>
         <v>1.4974946581424107</v>
       </c>
-      <c r="K70" s="3">
+      <c r="K70" s="7">
         <f t="shared" si="68"/>
         <v>0.51129671375068597</v>
       </c>
-      <c r="L70" s="3">
+      <c r="L70" s="7">
         <f t="shared" si="69"/>
         <v>7.3559776881812533E-2</v>
       </c>
       <c r="M70" s="8"/>
       <c r="N70" s="8"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B71" s="6">
         <v>0.108</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12047,45 +12099,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E71" s="6">
+      <c r="E71" s="30">
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="F71" s="6">
         <v>3600</v>
       </c>
-      <c r="G71" s="3">
+      <c r="G71" s="8">
         <v>22.8</v>
       </c>
       <c r="H71" s="3">
         <v>59</v>
       </c>
-      <c r="I71" s="3">
+      <c r="I71" s="8">
         <f t="shared" si="66"/>
         <v>20.357520395261862</v>
       </c>
-      <c r="J71" s="15">
+      <c r="J71" s="14">
         <f t="shared" si="67"/>
         <v>1.0108088942461273</v>
       </c>
-      <c r="K71" s="3">
+      <c r="K71" s="7">
         <f t="shared" si="68"/>
         <v>0.53970208673683517</v>
       </c>
-      <c r="L71" s="3">
+      <c r="L71" s="7">
         <f t="shared" si="69"/>
         <v>4.9652849395223464E-2</v>
       </c>
       <c r="M71" s="8"/>
       <c r="N71" s="8"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B72" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12093,45 +12145,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E72" s="3">
+      <c r="E72" s="10">
         <v>7.6E-3</v>
       </c>
       <c r="F72" s="3">
         <v>3600</v>
       </c>
-      <c r="G72" s="3">
+      <c r="G72" s="8">
         <v>7.9</v>
       </c>
       <c r="H72" s="3">
         <v>47</v>
       </c>
-      <c r="I72" s="3">
+      <c r="I72" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J72" s="15">
+      <c r="J72" s="14">
         <f t="shared" si="67"/>
         <v>3.0381988876492994</v>
       </c>
-      <c r="K72" s="3">
+      <c r="K72" s="7">
         <f t="shared" si="68"/>
         <v>0.2096493445655927</v>
       </c>
-      <c r="L72" s="3">
+      <c r="L72" s="7">
         <f t="shared" si="69"/>
         <v>0.15802103629597514</v>
       </c>
       <c r="M72" s="8"/>
       <c r="N72" s="8"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B73" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12139,45 +12191,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E73" s="3">
+      <c r="E73" s="10">
         <v>6.3E-3</v>
       </c>
       <c r="F73" s="3">
         <v>3600</v>
       </c>
-      <c r="G73" s="3">
+      <c r="G73" s="8">
         <v>13</v>
       </c>
       <c r="H73" s="3">
         <v>66</v>
       </c>
-      <c r="I73" s="3">
+      <c r="I73" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J73" s="15">
+      <c r="J73" s="14">
         <f t="shared" si="67"/>
         <v>2.518506972656656</v>
       </c>
-      <c r="K73" s="3">
+      <c r="K73" s="7">
         <f t="shared" si="68"/>
         <v>0.34499259232312718</v>
       </c>
-      <c r="L73" s="3">
+      <c r="L73" s="7">
         <f t="shared" si="69"/>
         <v>0.13099112219271625</v>
       </c>
       <c r="M73" s="8"/>
       <c r="N73" s="8"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B74" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12185,45 +12237,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E74" s="3">
+      <c r="E74" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F74" s="3">
         <v>3600</v>
       </c>
-      <c r="G74" s="3">
+      <c r="G74" s="8">
         <v>16.3</v>
       </c>
       <c r="H74" s="3">
         <v>69</v>
       </c>
-      <c r="I74" s="3">
+      <c r="I74" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J74" s="15">
+      <c r="J74" s="14">
         <f t="shared" si="67"/>
         <v>1.9988150576640129</v>
       </c>
-      <c r="K74" s="3">
+      <c r="K74" s="7">
         <f t="shared" si="68"/>
         <v>0.43256763498976725</v>
       </c>
-      <c r="L74" s="3">
+      <c r="L74" s="7">
         <f t="shared" si="69"/>
         <v>0.10396120808945734</v>
       </c>
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B75" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12231,45 +12283,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E75" s="3">
+      <c r="E75" s="10">
         <v>3.8E-3</v>
       </c>
       <c r="F75" s="3">
         <v>3600</v>
       </c>
-      <c r="G75" s="3">
+      <c r="G75" s="8">
         <v>18</v>
       </c>
       <c r="H75" s="3">
         <v>64</v>
       </c>
-      <c r="I75" s="3">
+      <c r="I75" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J75" s="15">
+      <c r="J75" s="14">
         <f t="shared" si="67"/>
         <v>1.5190994438246497</v>
       </c>
-      <c r="K75" s="3">
+      <c r="K75" s="7">
         <f t="shared" si="68"/>
         <v>0.47768205090894539</v>
       </c>
-      <c r="L75" s="3">
+      <c r="L75" s="7">
         <f t="shared" si="69"/>
         <v>7.9010518147987568E-2</v>
       </c>
       <c r="M75" s="8"/>
       <c r="N75" s="8"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B76" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12277,45 +12329,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E76" s="3">
+      <c r="E76" s="10">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F76" s="6">
         <v>3600</v>
       </c>
-      <c r="G76" s="3">
+      <c r="G76" s="8">
         <v>19.2</v>
       </c>
       <c r="H76" s="3">
         <v>54</v>
       </c>
-      <c r="I76" s="3">
+      <c r="I76" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J76" s="15">
+      <c r="J76" s="14">
         <f t="shared" si="67"/>
         <v>0.99940752883200645</v>
       </c>
-      <c r="K76" s="3">
+      <c r="K76" s="7">
         <f t="shared" si="68"/>
         <v>0.50952752096954168</v>
       </c>
-      <c r="L76" s="3">
+      <c r="L76" s="7">
         <f t="shared" si="69"/>
         <v>5.1980604044728672E-2</v>
       </c>
       <c r="M76" s="8"/>
       <c r="N76" s="8"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B77" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12323,45 +12375,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E77" s="3">
+      <c r="E77" s="10">
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="F77" s="3">
         <v>3600</v>
       </c>
-      <c r="G77" s="3">
+      <c r="G77" s="8">
         <v>6.65</v>
       </c>
       <c r="H77" s="3">
         <v>45</v>
       </c>
-      <c r="I77" s="3">
+      <c r="I77" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J77" s="15">
+      <c r="J77" s="14">
         <f t="shared" si="67"/>
         <v>3.0448109727843837</v>
       </c>
-      <c r="K77" s="3">
+      <c r="K77" s="7">
         <f t="shared" si="68"/>
         <v>0.19922596561183958</v>
       </c>
-      <c r="L77" s="3">
+      <c r="L77" s="7">
         <f t="shared" si="69"/>
         <v>0.16826274899273511</v>
       </c>
       <c r="M77" s="8"/>
       <c r="N77" s="8"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B78" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12369,45 +12421,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E78" s="3">
+      <c r="E78" s="10">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="F78" s="3">
         <v>3600</v>
       </c>
-      <c r="G78" s="3">
+      <c r="G78" s="8">
         <v>11</v>
       </c>
       <c r="H78" s="3">
         <v>62</v>
       </c>
-      <c r="I78" s="3">
+      <c r="I78" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J78" s="15">
+      <c r="J78" s="14">
         <f t="shared" si="67"/>
         <v>2.5301950337222343</v>
       </c>
-      <c r="K78" s="3">
+      <c r="K78" s="7">
         <f t="shared" si="68"/>
         <v>0.32954671003462188</v>
       </c>
-      <c r="L78" s="3">
+      <c r="L78" s="7">
         <f t="shared" si="69"/>
         <v>0.13982397451508971</v>
       </c>
       <c r="M78" s="8"/>
       <c r="N78" s="8"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B79" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12415,45 +12467,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E79" s="30">
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="F79" s="3">
         <v>3600</v>
       </c>
-      <c r="G79" s="6">
+      <c r="G79" s="31">
         <v>13.9</v>
       </c>
       <c r="H79" s="6">
         <v>65</v>
       </c>
-      <c r="I79" s="3">
+      <c r="I79" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J79" s="15">
+      <c r="J79" s="14">
         <f t="shared" si="67"/>
         <v>2.0155790946600849</v>
       </c>
-      <c r="K79" s="3">
+      <c r="K79" s="7">
         <f t="shared" si="68"/>
         <v>0.41642720631647673</v>
       </c>
-      <c r="L79" s="3">
+      <c r="L79" s="7">
         <f t="shared" si="69"/>
         <v>0.11138520003744436</v>
       </c>
       <c r="M79" s="8"/>
       <c r="N79" s="8"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B80" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12461,45 +12513,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E80" s="3">
+      <c r="E80" s="10">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="F80" s="3">
         <v>3600</v>
       </c>
-      <c r="G80" s="6">
+      <c r="G80" s="31">
         <v>15.8</v>
       </c>
       <c r="H80" s="6">
         <v>60</v>
       </c>
-      <c r="I80" s="3">
+      <c r="I80" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J80" s="15">
+      <c r="J80" s="14">
         <f t="shared" si="67"/>
         <v>1.5009631555979355</v>
       </c>
-      <c r="K80" s="3">
+      <c r="K80" s="7">
         <f t="shared" si="68"/>
         <v>0.47334891077700236</v>
       </c>
-      <c r="L80" s="3">
+      <c r="L80" s="7">
         <f t="shared" si="69"/>
         <v>8.2946425559798975E-2</v>
       </c>
       <c r="M80" s="8"/>
       <c r="N80" s="8"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B81" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12507,45 +12559,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E81" s="3">
+      <c r="E81" s="10">
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="F81" s="3">
         <v>3600</v>
       </c>
-      <c r="G81" s="3">
+      <c r="G81" s="8">
         <v>16.8</v>
       </c>
       <c r="H81" s="3">
         <v>52</v>
       </c>
-      <c r="I81" s="3">
+      <c r="I81" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J81" s="15">
+      <c r="J81" s="14">
         <f t="shared" si="67"/>
         <v>1.0292318781242986</v>
       </c>
-      <c r="K81" s="3">
+      <c r="K81" s="7">
         <f t="shared" si="68"/>
         <v>0.50330770259833157</v>
       </c>
-      <c r="L81" s="3">
+      <c r="L81" s="7">
         <f t="shared" si="69"/>
         <v>5.6877548955290728E-2</v>
       </c>
       <c r="M81" s="8"/>
       <c r="N81" s="8"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B82" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12553,45 +12605,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E82" s="3">
+      <c r="E82" s="10">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="F82" s="3">
         <v>3600</v>
       </c>
-      <c r="G82" s="3">
+      <c r="G82" s="8">
         <v>2.57</v>
       </c>
       <c r="H82" s="3">
         <v>24</v>
       </c>
-      <c r="I82" s="3">
+      <c r="I82" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J82" s="15">
+      <c r="J82" s="14">
         <f t="shared" si="67"/>
         <v>3.0036608329602066</v>
       </c>
-      <c r="K82" s="3">
+      <c r="K82" s="7">
         <f t="shared" si="68"/>
         <v>0.10300153568634084</v>
       </c>
-      <c r="L82" s="3">
+      <c r="L82" s="7">
         <f t="shared" si="69"/>
         <v>0.19198693531611913</v>
       </c>
       <c r="M82" s="8"/>
       <c r="N82" s="8"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B83" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12599,45 +12651,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E83" s="3">
+      <c r="E83" s="10">
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="F83" s="3">
         <v>3600</v>
       </c>
-      <c r="G83" s="3">
+      <c r="G83" s="8">
         <v>5.95</v>
       </c>
       <c r="H83" s="3">
         <v>43</v>
       </c>
-      <c r="I83" s="3">
+      <c r="I83" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J83" s="15">
+      <c r="J83" s="14">
         <f t="shared" si="67"/>
         <v>2.4945657765262732</v>
       </c>
-      <c r="K83" s="3">
+      <c r="K83" s="7">
         <f t="shared" si="68"/>
         <v>0.23846659040222878</v>
       </c>
-      <c r="L83" s="3">
+      <c r="L83" s="7">
         <f t="shared" si="69"/>
         <v>0.15944677678796335</v>
       </c>
       <c r="M83" s="8"/>
       <c r="N83" s="8"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B84" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12645,45 +12697,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E84" s="3">
+      <c r="E84" s="10">
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="F84" s="3">
         <v>3600</v>
       </c>
-      <c r="G84" s="3">
+      <c r="G84" s="8">
         <v>8.41</v>
       </c>
       <c r="H84" s="3">
         <v>53</v>
       </c>
-      <c r="I84" s="3">
+      <c r="I84" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J84" s="15">
+      <c r="J84" s="14">
         <f t="shared" si="67"/>
         <v>1.98547072009234</v>
       </c>
-      <c r="K84" s="3">
+      <c r="K84" s="7">
         <f t="shared" si="68"/>
         <v>0.33705950004752</v>
       </c>
-      <c r="L84" s="3">
+      <c r="L84" s="7">
         <f t="shared" si="69"/>
         <v>0.12690661825980756</v>
       </c>
       <c r="M84" s="8"/>
       <c r="N84" s="8"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B85" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12691,45 +12743,45 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E85" s="3">
+      <c r="E85" s="10">
         <v>2.8999999999999998E-3</v>
       </c>
       <c r="F85" s="3">
         <v>3600</v>
       </c>
-      <c r="G85" s="3">
+      <c r="G85" s="8">
         <v>9.91</v>
       </c>
       <c r="H85" s="3">
         <v>51</v>
       </c>
-      <c r="I85" s="3">
+      <c r="I85" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J85" s="15">
+      <c r="J85" s="14">
         <f t="shared" si="67"/>
         <v>1.4763756636584067</v>
       </c>
-      <c r="K85" s="3">
+      <c r="K85" s="7">
         <f t="shared" si="68"/>
         <v>0.39717712788001464</v>
       </c>
-      <c r="L85" s="3">
+      <c r="L85" s="7">
         <f t="shared" si="69"/>
         <v>9.4366459731651781E-2</v>
       </c>
       <c r="M85" s="8"/>
       <c r="N85" s="8"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B86" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="22">
         <f t="shared" si="64"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12737,43 +12789,43 @@
         <f t="shared" si="65"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E86" s="3">
+      <c r="E86" s="10">
         <v>2E-3</v>
       </c>
       <c r="F86" s="3">
         <v>3600</v>
       </c>
-      <c r="G86" s="3">
+      <c r="G86" s="8">
         <v>10.5</v>
       </c>
       <c r="H86" s="3">
         <v>38</v>
       </c>
-      <c r="I86" s="3">
+      <c r="I86" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J86" s="15">
+      <c r="J86" s="14">
         <f t="shared" si="67"/>
         <v>1.0181901128678668</v>
       </c>
-      <c r="K86" s="3">
+      <c r="K86" s="7">
         <f t="shared" si="68"/>
         <v>0.42082339482746262</v>
       </c>
-      <c r="L86" s="3">
+      <c r="L86" s="7">
         <f t="shared" si="69"/>
         <v>6.5080317056311579E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B87" s="3">
         <v>0.108</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="22">
         <f>$B$8*B87/$B$7</f>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12781,43 +12833,43 @@
         <f>$B$9*B87/$B$7</f>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E87" s="3">
+      <c r="E87" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F87" s="3">
         <v>3600</v>
       </c>
-      <c r="G87" s="3">
+      <c r="G87" s="8">
         <v>10.3</v>
       </c>
       <c r="H87" s="3">
         <v>52</v>
       </c>
-      <c r="I87" s="3">
+      <c r="I87" s="8">
         <f t="shared" si="66"/>
         <v>20.357520395261862</v>
       </c>
-      <c r="J87" s="15">
+      <c r="J87" s="14">
         <f t="shared" si="67"/>
         <v>2.9949893162848213</v>
       </c>
-      <c r="K87" s="3">
+      <c r="K87" s="7">
         <f t="shared" si="68"/>
         <v>0.24381278479778079</v>
       </c>
-      <c r="L87" s="3">
+      <c r="L87" s="7">
         <f t="shared" si="69"/>
         <v>0.14711955376362507</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B88" s="3">
         <v>0.108</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="22">
         <f t="shared" ref="C88:C106" si="70">$B$8*B88/$B$7</f>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12825,43 +12877,43 @@
         <f t="shared" ref="D88:D91" si="71">$B$9*B88/$B$7</f>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E88" s="3">
+      <c r="E88" s="10">
         <v>6.7000000000000002E-3</v>
       </c>
       <c r="F88" s="3">
         <v>3600</v>
       </c>
-      <c r="G88" s="3">
+      <c r="G88" s="8">
         <v>16.100000000000001</v>
       </c>
       <c r="H88" s="3">
         <v>71</v>
       </c>
-      <c r="I88" s="3">
+      <c r="I88" s="8">
         <f t="shared" si="66"/>
         <v>20.357520395261862</v>
       </c>
-      <c r="J88" s="15">
+      <c r="J88" s="14">
         <f t="shared" si="67"/>
         <v>2.5083035523885377</v>
       </c>
-      <c r="K88" s="3">
+      <c r="K88" s="7">
         <f t="shared" si="68"/>
         <v>0.38110542089750205</v>
       </c>
-      <c r="L88" s="3">
+      <c r="L88" s="7">
         <f t="shared" si="69"/>
         <v>0.123212626277036</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B89" s="3">
         <v>0.108</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89" s="22">
         <f t="shared" si="70"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12869,43 +12921,43 @@
         <f t="shared" si="71"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E89" s="3">
+      <c r="E89" s="10">
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="F89" s="3">
         <v>3600</v>
       </c>
-      <c r="G89" s="3">
+      <c r="G89" s="8">
         <v>19.399999999999999</v>
       </c>
       <c r="H89" s="3">
         <v>73</v>
       </c>
-      <c r="I89" s="3">
+      <c r="I89" s="8">
         <f t="shared" si="66"/>
         <v>20.357520395261862</v>
       </c>
-      <c r="J89" s="15">
+      <c r="J89" s="14">
         <f t="shared" si="67"/>
         <v>2.0216177884922546</v>
       </c>
-      <c r="K89" s="3">
+      <c r="K89" s="7">
         <f t="shared" si="68"/>
         <v>0.45922019660941232</v>
       </c>
-      <c r="L89" s="3">
+      <c r="L89" s="7">
         <f t="shared" si="69"/>
         <v>9.9305698790446928E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B90" s="3">
         <v>0.108</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C90" s="22">
         <f t="shared" si="70"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12913,43 +12965,43 @@
         <f t="shared" si="71"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E90" s="6">
+      <c r="E90" s="30">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F90" s="3">
         <v>3600</v>
       </c>
-      <c r="G90" s="6">
+      <c r="G90" s="31">
         <v>21.6</v>
       </c>
       <c r="H90" s="6">
         <v>69</v>
       </c>
-      <c r="I90" s="3">
-        <f t="shared" si="66"/>
+      <c r="I90" s="8">
+        <f>B90/2*F90*2*PI()/60</f>
         <v>20.357520395261862</v>
       </c>
-      <c r="J90" s="15">
+      <c r="J90" s="14">
         <f t="shared" si="67"/>
         <v>1.4974946581424107</v>
       </c>
-      <c r="K90" s="3">
+      <c r="K90" s="7">
         <f t="shared" si="68"/>
         <v>0.51129671375068597</v>
       </c>
-      <c r="L90" s="3">
+      <c r="L90" s="7">
         <f t="shared" si="69"/>
         <v>7.3559776881812533E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B91" s="6">
         <v>0.108</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C91" s="22">
         <f t="shared" si="70"/>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -12957,43 +13009,43 @@
         <f t="shared" si="71"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E91" s="6">
+      <c r="E91" s="30">
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="F91" s="6">
         <v>3600</v>
       </c>
-      <c r="G91" s="3">
+      <c r="G91" s="8">
         <v>22.8</v>
       </c>
       <c r="H91" s="3">
         <v>59</v>
       </c>
-      <c r="I91" s="3">
+      <c r="I91" s="8">
         <f t="shared" si="66"/>
         <v>20.357520395261862</v>
       </c>
-      <c r="J91" s="15">
+      <c r="J91" s="14">
         <f t="shared" si="67"/>
         <v>1.0108088942461273</v>
       </c>
-      <c r="K91" s="3">
+      <c r="K91" s="7">
         <f t="shared" si="68"/>
         <v>0.53970208673683517</v>
       </c>
-      <c r="L91" s="3">
+      <c r="L91" s="7">
         <f t="shared" si="69"/>
         <v>4.9652849395223464E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B92" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C92" s="3">
+      <c r="C92" s="22">
         <f t="shared" si="70"/>
         <v>8.5000000000000006E-3</v>
       </c>
@@ -13001,43 +13053,43 @@
         <f t="shared" ref="D92:D106" si="72">$B$9*B92/$B$7</f>
         <v>8.0277777777777778E-3</v>
       </c>
-      <c r="E92" s="3">
+      <c r="E92" s="10">
         <v>7.6E-3</v>
       </c>
       <c r="F92" s="3">
         <v>3600</v>
       </c>
-      <c r="G92" s="3">
+      <c r="G92" s="8">
         <v>7.9</v>
       </c>
       <c r="H92" s="3">
         <v>47</v>
       </c>
-      <c r="I92" s="3">
+      <c r="I92" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J92" s="15">
+      <c r="J92" s="14">
         <f t="shared" si="67"/>
         <v>3.1898190711158065</v>
       </c>
-      <c r="K92" s="3">
+      <c r="K92" s="7">
         <f t="shared" si="68"/>
         <v>0.2096493445655927</v>
       </c>
-      <c r="L92" s="3">
+      <c r="L92" s="7">
         <f t="shared" si="69"/>
         <v>0.16590701723427406</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B93" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C93" s="3">
+      <c r="C93" s="22">
         <f t="shared" si="70"/>
         <v>8.5000000000000006E-3</v>
       </c>
@@ -13045,43 +13097,43 @@
         <f t="shared" si="72"/>
         <v>8.0277777777777778E-3</v>
       </c>
-      <c r="E93" s="3">
+      <c r="E93" s="10">
         <v>6.3E-3</v>
       </c>
       <c r="F93" s="3">
         <v>3600</v>
       </c>
-      <c r="G93" s="3">
+      <c r="G93" s="8">
         <v>13</v>
       </c>
       <c r="H93" s="3">
         <v>66</v>
       </c>
-      <c r="I93" s="3">
+      <c r="I93" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J93" s="15">
+      <c r="J93" s="14">
         <f t="shared" si="67"/>
         <v>2.6441921247407345</v>
       </c>
-      <c r="K93" s="3">
+      <c r="K93" s="7">
         <f t="shared" si="68"/>
         <v>0.34499259232312718</v>
       </c>
-      <c r="L93" s="3">
+      <c r="L93" s="7">
         <f t="shared" si="69"/>
         <v>0.13752818533893771</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B94" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C94" s="3">
+      <c r="C94" s="22">
         <f t="shared" si="70"/>
         <v>8.5000000000000006E-3</v>
       </c>
@@ -13089,43 +13141,43 @@
         <f t="shared" si="72"/>
         <v>8.0277777777777778E-3</v>
       </c>
-      <c r="E94" s="3">
+      <c r="E94" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F94" s="3">
         <v>3600</v>
       </c>
-      <c r="G94" s="3">
+      <c r="G94" s="8">
         <v>16.3</v>
       </c>
       <c r="H94" s="3">
         <v>69</v>
       </c>
-      <c r="I94" s="3">
+      <c r="I94" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J94" s="15">
+      <c r="J94" s="14">
         <f t="shared" si="67"/>
         <v>2.0985651783656625</v>
       </c>
-      <c r="K94" s="3">
+      <c r="K94" s="7">
         <f t="shared" si="68"/>
         <v>0.43256763498976725</v>
       </c>
-      <c r="L94" s="3">
+      <c r="L94" s="7">
         <f t="shared" si="69"/>
         <v>0.10914935344360137</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B95" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C95" s="22">
         <f t="shared" si="70"/>
         <v>8.5000000000000006E-3</v>
       </c>
@@ -13133,43 +13185,43 @@
         <f t="shared" si="72"/>
         <v>8.0277777777777778E-3</v>
       </c>
-      <c r="E95" s="3">
+      <c r="E95" s="10">
         <v>3.8E-3</v>
       </c>
       <c r="F95" s="3">
         <v>3600</v>
       </c>
-      <c r="G95" s="3">
+      <c r="G95" s="8">
         <v>18</v>
       </c>
       <c r="H95" s="3">
         <v>64</v>
       </c>
-      <c r="I95" s="3">
+      <c r="I95" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J95" s="15">
+      <c r="J95" s="14">
         <f t="shared" si="67"/>
         <v>1.5949095355579033</v>
       </c>
-      <c r="K95" s="3">
+      <c r="K95" s="7">
         <f t="shared" si="68"/>
         <v>0.47768205090894539</v>
       </c>
-      <c r="L95" s="3">
+      <c r="L95" s="7">
         <f t="shared" si="69"/>
         <v>8.2953508617137031E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B96" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C96" s="3">
+      <c r="C96" s="22">
         <f t="shared" si="70"/>
         <v>8.5000000000000006E-3</v>
       </c>
@@ -13177,43 +13229,43 @@
         <f t="shared" si="72"/>
         <v>8.0277777777777778E-3</v>
       </c>
-      <c r="E96" s="3">
+      <c r="E96" s="10">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F96" s="6">
         <v>3600</v>
       </c>
-      <c r="G96" s="3">
+      <c r="G96" s="8">
         <v>19.2</v>
       </c>
       <c r="H96" s="3">
         <v>54</v>
       </c>
-      <c r="I96" s="3">
+      <c r="I96" s="8">
         <f t="shared" si="66"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J96" s="15">
+      <c r="J96" s="14">
         <f t="shared" si="67"/>
         <v>1.0492825891828312</v>
       </c>
-      <c r="K96" s="3">
+      <c r="K96" s="7">
         <f t="shared" si="68"/>
         <v>0.50952752096954168</v>
       </c>
-      <c r="L96" s="3">
+      <c r="L96" s="7">
         <f t="shared" si="69"/>
         <v>5.4574676721800684E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B97" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C97" s="3">
+      <c r="C97" s="22">
         <f t="shared" si="70"/>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -13221,43 +13273,43 @@
         <f t="shared" si="72"/>
         <v>7.5555555555555567E-3</v>
       </c>
-      <c r="E97" s="3">
+      <c r="E97" s="10">
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="F97" s="3">
         <v>3600</v>
       </c>
-      <c r="G97" s="3">
+      <c r="G97" s="8">
         <v>6.65</v>
       </c>
       <c r="H97" s="3">
         <v>45</v>
       </c>
-      <c r="I97" s="3">
+      <c r="I97" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J97" s="15">
+      <c r="J97" s="14">
         <f t="shared" si="67"/>
         <v>3.3640983511628928</v>
       </c>
-      <c r="K97" s="3">
+      <c r="K97" s="7">
         <f t="shared" si="68"/>
         <v>0.19922596561183958</v>
       </c>
-      <c r="L97" s="3">
+      <c r="L97" s="7">
         <f t="shared" si="69"/>
         <v>0.18590725056766289</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B98" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C98" s="22">
         <f t="shared" si="70"/>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -13265,43 +13317,43 @@
         <f t="shared" si="72"/>
         <v>7.5555555555555567E-3</v>
       </c>
-      <c r="E98" s="3">
+      <c r="E98" s="10">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="F98" s="3">
         <v>3600</v>
       </c>
-      <c r="G98" s="3">
+      <c r="G98" s="8">
         <v>11</v>
       </c>
       <c r="H98" s="3">
         <v>62</v>
       </c>
-      <c r="I98" s="3">
+      <c r="I98" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J98" s="15">
+      <c r="J98" s="14">
         <f t="shared" si="67"/>
         <v>2.7955183481494461</v>
       </c>
-      <c r="K98" s="3">
+      <c r="K98" s="7">
         <f t="shared" si="68"/>
         <v>0.32954671003462188</v>
       </c>
-      <c r="L98" s="3">
+      <c r="L98" s="7">
         <f t="shared" si="69"/>
         <v>0.15448630680974804</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B99" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C99" s="22">
         <f t="shared" si="70"/>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -13309,43 +13361,43 @@
         <f t="shared" si="72"/>
         <v>7.5555555555555567E-3</v>
       </c>
-      <c r="E99" s="6">
+      <c r="E99" s="30">
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="F99" s="3">
         <v>3600</v>
       </c>
-      <c r="G99" s="6">
+      <c r="G99" s="31">
         <v>13.9</v>
       </c>
       <c r="H99" s="6">
         <v>65</v>
       </c>
-      <c r="I99" s="3">
+      <c r="I99" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J99" s="15">
+      <c r="J99" s="14">
         <f t="shared" si="67"/>
         <v>2.2269383451359994</v>
       </c>
-      <c r="K99" s="3">
+      <c r="K99" s="7">
         <f t="shared" si="68"/>
         <v>0.41642720631647673</v>
       </c>
-      <c r="L99" s="3">
+      <c r="L99" s="7">
         <f t="shared" si="69"/>
         <v>0.12306536305183319</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B100" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C100" s="22">
         <f t="shared" si="70"/>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -13353,43 +13405,43 @@
         <f t="shared" si="72"/>
         <v>7.5555555555555567E-3</v>
       </c>
-      <c r="E100" s="3">
+      <c r="E100" s="10">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="F100" s="3">
         <v>3600</v>
       </c>
-      <c r="G100" s="6">
+      <c r="G100" s="31">
         <v>15.8</v>
       </c>
       <c r="H100" s="6">
         <v>60</v>
       </c>
-      <c r="I100" s="3">
+      <c r="I100" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J100" s="15">
+      <c r="J100" s="14">
         <f t="shared" si="67"/>
         <v>1.6583583421225527</v>
       </c>
-      <c r="K100" s="3">
+      <c r="K100" s="7">
         <f t="shared" si="68"/>
         <v>0.47334891077700236</v>
       </c>
-      <c r="L100" s="3">
+      <c r="L100" s="7">
         <f t="shared" si="69"/>
         <v>9.1644419293918325E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B101" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C101" s="22">
         <f t="shared" si="70"/>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -13397,43 +13449,43 @@
         <f t="shared" si="72"/>
         <v>7.5555555555555567E-3</v>
       </c>
-      <c r="E101" s="3">
+      <c r="E101" s="10">
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="F101" s="3">
         <v>3600</v>
       </c>
-      <c r="G101" s="3">
+      <c r="G101" s="8">
         <v>16.8</v>
       </c>
       <c r="H101" s="3">
         <v>52</v>
       </c>
-      <c r="I101" s="3">
+      <c r="I101" s="8">
         <f t="shared" si="66"/>
         <v>18.095573684677209</v>
       </c>
-      <c r="J101" s="15">
+      <c r="J101" s="14">
         <f t="shared" si="67"/>
         <v>1.1371600060268932</v>
       </c>
-      <c r="K101" s="3">
+      <c r="K101" s="7">
         <f t="shared" si="68"/>
         <v>0.50330770259833157</v>
       </c>
-      <c r="L101" s="3">
+      <c r="L101" s="7">
         <f t="shared" si="69"/>
         <v>6.2841887515829697E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B102" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C102" s="22">
         <f t="shared" si="70"/>
         <v>6.9166666666666682E-3</v>
       </c>
@@ -13441,43 +13493,43 @@
         <f t="shared" si="72"/>
         <v>6.5324074074074078E-3</v>
       </c>
-      <c r="E102" s="3">
+      <c r="E102" s="10">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="F102" s="3">
         <v>3600</v>
       </c>
-      <c r="G102" s="3">
+      <c r="G102" s="8">
         <v>2.57</v>
       </c>
       <c r="H102" s="3">
         <v>24</v>
       </c>
-      <c r="I102" s="3">
+      <c r="I102" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J102" s="15">
+      <c r="J102" s="14">
         <f t="shared" si="67"/>
         <v>3.7398021623668587</v>
       </c>
-      <c r="K102" s="3">
+      <c r="K102" s="7">
         <f t="shared" si="68"/>
         <v>0.10300153568634084</v>
       </c>
-      <c r="L102" s="3">
+      <c r="L102" s="7">
         <f t="shared" si="69"/>
         <v>0.23903935756082109</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B103" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C103" s="3">
+      <c r="C103" s="22">
         <f t="shared" si="70"/>
         <v>6.9166666666666682E-3</v>
       </c>
@@ -13485,43 +13537,43 @@
         <f t="shared" si="72"/>
         <v>6.5324074074074078E-3</v>
       </c>
-      <c r="E103" s="3">
+      <c r="E103" s="10">
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="F103" s="3">
         <v>3600</v>
       </c>
-      <c r="G103" s="3">
+      <c r="G103" s="8">
         <v>5.95</v>
       </c>
       <c r="H103" s="3">
         <v>43</v>
       </c>
-      <c r="I103" s="3">
+      <c r="I103" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J103" s="15">
+      <c r="J103" s="14">
         <f t="shared" si="67"/>
         <v>3.1059373890843402</v>
       </c>
-      <c r="K103" s="3">
+      <c r="K103" s="7">
         <f t="shared" si="68"/>
         <v>0.23846659040222878</v>
       </c>
-      <c r="L103" s="3">
+      <c r="L103" s="7">
         <f t="shared" si="69"/>
         <v>0.19852421221152938</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B104" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C104" s="3">
+      <c r="C104" s="22">
         <f t="shared" si="70"/>
         <v>6.9166666666666682E-3</v>
       </c>
@@ -13529,43 +13581,43 @@
         <f t="shared" si="72"/>
         <v>6.5324074074074078E-3</v>
       </c>
-      <c r="E104" s="3">
+      <c r="E104" s="10">
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="F104" s="3">
         <v>3600</v>
       </c>
-      <c r="G104" s="3">
+      <c r="G104" s="8">
         <v>8.41</v>
       </c>
       <c r="H104" s="3">
         <v>53</v>
       </c>
-      <c r="I104" s="3">
+      <c r="I104" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J104" s="15">
+      <c r="J104" s="14">
         <f t="shared" si="67"/>
         <v>2.4720726158018218</v>
       </c>
-      <c r="K104" s="3">
+      <c r="K104" s="7">
         <f t="shared" si="68"/>
         <v>0.33705950004752</v>
       </c>
-      <c r="L104" s="3">
+      <c r="L104" s="7">
         <f t="shared" si="69"/>
         <v>0.15800906686223767</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B105" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C105" s="3">
+      <c r="C105" s="22">
         <f t="shared" si="70"/>
         <v>6.9166666666666682E-3</v>
       </c>
@@ -13573,43 +13625,43 @@
         <f t="shared" si="72"/>
         <v>6.5324074074074078E-3</v>
       </c>
-      <c r="E105" s="3">
+      <c r="E105" s="10">
         <v>2.8999999999999998E-3</v>
       </c>
       <c r="F105" s="3">
         <v>3600</v>
       </c>
-      <c r="G105" s="3">
+      <c r="G105" s="8">
         <v>9.91</v>
       </c>
       <c r="H105" s="3">
         <v>51</v>
       </c>
-      <c r="I105" s="3">
+      <c r="I105" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J105" s="15">
+      <c r="J105" s="14">
         <f t="shared" si="67"/>
         <v>1.8382078425193034</v>
       </c>
-      <c r="K105" s="3">
+      <c r="K105" s="7">
         <f t="shared" si="68"/>
         <v>0.39717712788001464</v>
       </c>
-      <c r="L105" s="3">
+      <c r="L105" s="7">
         <f t="shared" si="69"/>
         <v>0.11749392151294595</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B106" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C106" s="3">
+      <c r="C106" s="22">
         <f t="shared" si="70"/>
         <v>6.9166666666666682E-3</v>
       </c>
@@ -13617,37 +13669,40 @@
         <f t="shared" si="72"/>
         <v>6.5324074074074078E-3</v>
       </c>
-      <c r="E106" s="3">
+      <c r="E106" s="10">
         <v>2E-3</v>
       </c>
       <c r="F106" s="3">
         <v>3600</v>
       </c>
-      <c r="G106" s="3">
+      <c r="G106" s="8">
         <v>10.5</v>
       </c>
       <c r="H106" s="3">
         <v>38</v>
       </c>
-      <c r="I106" s="3">
+      <c r="I106" s="8">
         <f t="shared" si="66"/>
         <v>15.64513141487717</v>
       </c>
-      <c r="J106" s="15">
+      <c r="J106" s="14">
         <f t="shared" si="67"/>
         <v>1.2677295465650369</v>
       </c>
-      <c r="K106" s="3">
+      <c r="K106" s="7">
         <f t="shared" si="68"/>
         <v>0.42082339482746262</v>
       </c>
-      <c r="L106" s="3">
+      <c r="L106" s="7">
         <f t="shared" si="69"/>
         <v>8.1030290698583418E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="F54:H54"/>
     <mergeCell ref="AD13:AE13"/>
     <mergeCell ref="AF13:AG13"/>
     <mergeCell ref="D13:E13"/>
@@ -13655,9 +13710,6 @@
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
     <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="F54:H54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated pump analysis and appendix files
</commit_message>
<xml_diff>
--- a/Lab 1 - Pumps/data_and_analysis.xlsx
+++ b/Lab 1 - Pumps/data_and_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\LaTeX\MEC-E-403\Lab 1 - Pumps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F23CAD1-CBFB-4646-9A70-983795235ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3335AF95-68D8-4057-811D-78D0A5047CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38385" windowHeight="21000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="seans analysis" sheetId="6" state="hidden" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="103">
   <si>
     <t>(V)</t>
   </si>
@@ -338,6 +338,15 @@
   <si>
     <t>Flow Coefficient, $\Phi$</t>
   </si>
+  <si>
+    <t>ideal shutoff head</t>
+  </si>
+  <si>
+    <t>thumb</t>
+  </si>
+  <si>
+    <t>actual shutoff head</t>
+  </si>
 </sst>
 </file>
 
@@ -354,7 +363,7 @@
     <numFmt numFmtId="171" formatCode="#,##0.0000;\-#,##0.0000;\-"/>
     <numFmt numFmtId="172" formatCode="#,##0.00000;\-#,##0.00000;\-"/>
     <numFmt numFmtId="173" formatCode="#,##0.000000;\-#,##0.000000;\-"/>
-    <numFmt numFmtId="176" formatCode="0.00000000"/>
+    <numFmt numFmtId="174" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -405,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -496,8 +505,8 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -505,9 +514,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,19 +911,19 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="32"/>
+      <c r="E13" s="35"/>
       <c r="G13" s="33" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="33"/>
       <c r="I13" s="33"/>
-      <c r="L13" s="32" t="s">
+      <c r="L13" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="32"/>
+      <c r="M13" s="35"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
@@ -6050,30 +6060,30 @@
       <c r="N58" s="8"/>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A59" s="32"/>
+      <c r="A59" s="35"/>
       <c r="B59" s="33"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="35"/>
       <c r="K59" s="33"/>
       <c r="L59" s="33"/>
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+      <c r="A60" s="35"/>
       <c r="B60" s="33"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="35"/>
+      <c r="H60" s="35"/>
       <c r="M60" s="8"/>
       <c r="N60" s="8"/>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A61" s="32"/>
+      <c r="A61" s="35"/>
       <c r="C61" s="33"/>
       <c r="D61" s="33"/>
       <c r="F61" s="33"/>
@@ -6102,6 +6112,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="F59:H60"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="K61:L61"/>
     <mergeCell ref="AF13:AG13"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="K50:L50"/>
@@ -6112,14 +6130,6 @@
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
     <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="F59:H60"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="K61:L61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6128,10 +6138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B530A311-2D6F-44F7-871F-14AF58E6CD82}">
-  <dimension ref="A1:AO106"/>
+  <dimension ref="A1:AO111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AO41" sqref="AO16:AO41"/>
+    <sheetView tabSelected="1" topLeftCell="Y8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AO16" sqref="AO16:AO18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6139,19 +6149,19 @@
     <col min="1" max="1" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="15" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="3" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" style="3" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -6310,19 +6320,19 @@
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="32"/>
+      <c r="E13" s="35"/>
       <c r="G13" s="33" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="33"/>
       <c r="I13" s="33"/>
-      <c r="L13" s="32" t="s">
+      <c r="L13" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="32"/>
+      <c r="M13" s="35"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
@@ -11007,7 +11017,7 @@
         <f>L46+M46</f>
         <v>8.3100112559471651</v>
       </c>
-      <c r="O46" s="8">
+      <c r="O46" s="7">
         <f t="shared" si="28"/>
         <v>9.1456936498984369</v>
       </c>
@@ -11543,7 +11553,7 @@
       <c r="A52" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B52" s="35">
+      <c r="B52" s="32">
         <f>_xlfn.COT(RADIANS(B51))</f>
         <v>1.5398649638145827</v>
       </c>
@@ -13696,6 +13706,33 @@
       <c r="L106" s="7">
         <f t="shared" si="69"/>
         <v>8.1030290698583418E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B109" s="36">
+        <f>I67^2/9.81</f>
+        <v>42.245528709837174</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B110" s="36">
+        <f>B109/2</f>
+        <v>21.122764354918587</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B111" s="36">
+        <f>N27</f>
+        <v>21.760961678709098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update pump efficiency plot and abstract
</commit_message>
<xml_diff>
--- a/Lab 1 - Pumps/data_and_analysis.xlsx
+++ b/Lab 1 - Pumps/data_and_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\LaTeX\MEC-E-403\Lab 1 - Pumps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3335AF95-68D8-4057-811D-78D0A5047CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73DA49B-7616-4D33-A38E-20070E2BDF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38385" windowHeight="21000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="seans analysis" sheetId="6" state="hidden" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="106">
   <si>
     <t>(V)</t>
   </si>
@@ -347,6 +347,15 @@
   <si>
     <t>actual shutoff head</t>
   </si>
+  <si>
+    <t>$\delta_{eff}$</t>
+  </si>
+  <si>
+    <t>(\%)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
@@ -414,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -508,16 +517,28 @@
     <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -911,41 +932,41 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="G13" s="33" t="s">
+      <c r="E13" s="34"/>
+      <c r="G13" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="L13" s="35" t="s">
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="L13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="35"/>
+      <c r="M13" s="34"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="33" t="s">
+      <c r="Z13" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="33"/>
-      <c r="AB13" s="33" t="s">
+      <c r="AA13" s="35"/>
+      <c r="AB13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="33"/>
-      <c r="AD13" s="33" t="s">
+      <c r="AC13" s="35"/>
+      <c r="AD13" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="33"/>
-      <c r="AF13" s="33" t="s">
+      <c r="AE13" s="35"/>
+      <c r="AF13" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="33"/>
+      <c r="AG13" s="35"/>
     </row>
     <row r="14" spans="1:39" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -966,11 +987,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -5986,8 +6007,8 @@
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
-      <c r="K50" s="33"/>
-      <c r="L50" s="33"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="35"/>
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
     </row>
@@ -6012,8 +6033,8 @@
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
-      <c r="K52" s="33"/>
-      <c r="L52" s="33"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
       <c r="M52" s="8"/>
       <c r="N52" s="8"/>
     </row>
@@ -6060,37 +6081,37 @@
       <c r="N58" s="8"/>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A59" s="35"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="33"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="34"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
-      <c r="B60" s="33"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="35"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="35"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="34"/>
       <c r="M60" s="8"/>
       <c r="N60" s="8"/>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
-      <c r="K61" s="33"/>
-      <c r="L61" s="33"/>
+      <c r="A61" s="34"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="35"/>
+      <c r="H61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="35"/>
       <c r="M61" s="8"/>
       <c r="N61" s="8"/>
     </row>
@@ -6112,14 +6133,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="F59:H60"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="K61:L61"/>
     <mergeCell ref="AF13:AG13"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="K50:L50"/>
@@ -6130,6 +6143,14 @@
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
     <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="F59:H60"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="K61:L61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6138,10 +6159,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B530A311-2D6F-44F7-871F-14AF58E6CD82}">
-  <dimension ref="A1:AO111"/>
+  <dimension ref="A1:AP111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AO16" sqref="AO16:AO18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6149,41 +6170,43 @@
     <col min="1" max="1" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="13.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="15" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="3" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="3" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" style="3" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="32.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="32.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.85546875" style="3"/>
-    <col min="40" max="16384" width="10.85546875" style="2"/>
+    <col min="39" max="39" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6194,7 +6217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -6205,7 +6228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -6222,7 +6245,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6233,7 +6256,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -6245,7 +6268,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -6257,7 +6280,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -6272,7 +6295,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -6284,7 +6307,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -6295,7 +6318,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -6304,11 +6327,11 @@
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -6319,47 +6342,47 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="D13" s="35" t="s">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="D13" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="G13" s="33" t="s">
+      <c r="E13" s="34"/>
+      <c r="G13" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="L13" s="35" t="s">
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="L13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="35"/>
+      <c r="M13" s="34"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="33" t="s">
+      <c r="Z13" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="33"/>
-      <c r="AB13" s="33" t="s">
+      <c r="AA13" s="35"/>
+      <c r="AB13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="33"/>
-      <c r="AD13" s="33" t="s">
+      <c r="AC13" s="35"/>
+      <c r="AD13" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="33"/>
-      <c r="AF13" s="33" t="s">
+      <c r="AE13" s="35"/>
+      <c r="AF13" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="33"/>
-      <c r="AO13" s="2" t="s">
+      <c r="AG13" s="35"/>
+      <c r="AO13" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>62</v>
       </c>
@@ -6378,11 +6401,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -6473,14 +6496,17 @@
       <c r="AM14" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="AN14" s="16" t="s">
+      <c r="AN14" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AO14" s="16" t="s">
+      <c r="AO14" s="24" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP14" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
         <v>19</v>
@@ -6580,14 +6606,17 @@
         <v>31</v>
       </c>
       <c r="AM15" s="23"/>
-      <c r="AN15" s="2" t="s">
+      <c r="AN15" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AO15" s="2" t="s">
+      <c r="AO15" s="23" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP15" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>63</v>
       </c>
@@ -6729,16 +6758,20 @@
         <f>IFERROR(S16*AK16/Q16, 0)</f>
         <v>2.3524059815009852E-3</v>
       </c>
-      <c r="AN16" s="2">
+      <c r="AN16" s="7">
         <f>$B$4*F16/100*9.81</f>
         <v>1.2892792500000001</v>
       </c>
-      <c r="AO16" s="2">
+      <c r="AO16" s="37">
         <f>$B$2*9.81*K16*O16/(AN16*C16*2*PI()/60)*100</f>
         <v>37.010451746090069</v>
       </c>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP16" s="8">
+        <f>AO16*SQRT((Y16/K16)^2+(AI16/O16)^2)</f>
+        <v>0.88394101528140789</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -6880,16 +6913,20 @@
         <f t="shared" ref="AM17:AM49" si="21">IFERROR(S17*AK17/Q17, 0)</f>
         <v>2.0223797083059789E-3</v>
       </c>
-      <c r="AN17" s="2">
+      <c r="AN17" s="7">
         <f t="shared" ref="AN17:AN27" si="22">$B$4*F17/100*9.81</f>
         <v>1.2524427</v>
       </c>
-      <c r="AO17" s="2">
+      <c r="AO17" s="37">
         <f t="shared" ref="AO17:AO27" si="23">$B$2*9.81*K17*O17/(AN17*C17*2*PI()/60)*100</f>
         <v>39.406990455603598</v>
       </c>
-    </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP17" s="8">
+        <f t="shared" ref="AP17:AP27" si="24">AO17*SQRT((Y17/K17)^2+(AI17/O17)^2)</f>
+        <v>0.85152620176970306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>63</v>
       </c>
@@ -7001,7 +7038,7 @@
         <v>0.01</v>
       </c>
       <c r="AF18" s="15">
-        <f t="shared" ref="AF18:AF27" si="24">L18*AD18/D18</f>
+        <f t="shared" ref="AF18:AF27" si="25">L18*AD18/D18</f>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG18" s="15">
@@ -7031,16 +7068,20 @@
         <f t="shared" si="21"/>
         <v>4.2104856478026285E-4</v>
       </c>
-      <c r="AN18" s="2">
+      <c r="AN18" s="7">
         <f t="shared" si="22"/>
         <v>1.0682599500000001</v>
       </c>
-      <c r="AO18" s="2">
+      <c r="AO18" s="37">
         <f t="shared" si="23"/>
         <v>36.959072152593905</v>
       </c>
-    </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP18" s="8">
+        <f t="shared" si="24"/>
+        <v>0.38171822644471037</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>63</v>
       </c>
@@ -7151,7 +7192,7 @@
         <v>0.01</v>
       </c>
       <c r="AF19" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG19" s="15">
@@ -7181,16 +7222,19 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AN19" s="2">
+      <c r="AN19" s="22">
         <f t="shared" si="22"/>
         <v>0.66305789999999998</v>
       </c>
-      <c r="AO19" s="2">
+      <c r="AO19" s="25">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP19" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -7302,7 +7346,7 @@
         <v>0.01</v>
       </c>
       <c r="AF20" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG20" s="15">
@@ -7332,16 +7376,20 @@
         <f t="shared" si="21"/>
         <v>3.3433822934822006E-3</v>
       </c>
-      <c r="AN20" s="2">
+      <c r="AN20" s="7">
         <f t="shared" si="22"/>
         <v>2.4312123000000003</v>
       </c>
-      <c r="AO20" s="2">
+      <c r="AO20" s="37">
         <f t="shared" si="23"/>
         <v>40.916592886771006</v>
       </c>
-    </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP20" s="40">
+        <f t="shared" si="24"/>
+        <v>1.1995299740668006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -7453,7 +7501,7 @@
         <v>0.01</v>
       </c>
       <c r="AF21" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG21" s="15">
@@ -7483,16 +7531,20 @@
         <f t="shared" si="21"/>
         <v>2.6517015766541635E-3</v>
       </c>
-      <c r="AN21" s="2">
+      <c r="AN21" s="7">
         <f t="shared" si="22"/>
         <v>2.4312123000000003</v>
       </c>
-      <c r="AO21" s="2">
+      <c r="AO21" s="37">
         <f t="shared" si="23"/>
         <v>42.673982331632686</v>
       </c>
-    </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP21" s="40">
+        <f t="shared" si="24"/>
+        <v>1.0176801122282624</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -7604,7 +7656,7 @@
         <v>0.01</v>
       </c>
       <c r="AF22" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG22" s="15">
@@ -7634,16 +7686,20 @@
         <f t="shared" si="21"/>
         <v>6.251283419810062E-4</v>
       </c>
-      <c r="AN22" s="2">
+      <c r="AN22" s="7">
         <f t="shared" si="22"/>
         <v>2.1365199000000001</v>
       </c>
-      <c r="AO22" s="2">
+      <c r="AO22" s="37">
         <f t="shared" si="23"/>
         <v>49.917307149111032</v>
       </c>
-    </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP22" s="8">
+        <f t="shared" si="24"/>
+        <v>0.46801903534724748</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>63</v>
       </c>
@@ -7754,7 +7810,7 @@
         <v>0.01</v>
       </c>
       <c r="AF23" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG23" s="15">
@@ -7784,16 +7840,19 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AN23" s="2">
+      <c r="AN23" s="7">
         <f t="shared" si="22"/>
         <v>1.2524427</v>
       </c>
-      <c r="AO23" s="2">
+      <c r="AO23" s="25">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP23" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -7905,7 +7964,7 @@
         <v>0.01</v>
       </c>
       <c r="AF24" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG24" s="15">
@@ -7935,16 +7994,20 @@
         <f t="shared" si="21"/>
         <v>2.729034150603259E-3</v>
       </c>
-      <c r="AN24" s="2">
+      <c r="AN24" s="7">
         <f t="shared" si="22"/>
         <v>3.9046742999999999</v>
       </c>
-      <c r="AO24" s="2">
+      <c r="AO24" s="37">
         <f t="shared" si="23"/>
         <v>41.834907330788297</v>
       </c>
-    </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP24" s="40">
+        <f t="shared" si="24"/>
+        <v>0.99581938066018949</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -8056,7 +8119,7 @@
         <v>0.01</v>
       </c>
       <c r="AF25" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG25" s="15">
@@ -8086,16 +8149,20 @@
         <f t="shared" si="21"/>
         <v>8.1849299881077871E-3</v>
       </c>
-      <c r="AN25" s="2">
+      <c r="AN25" s="7">
         <f t="shared" si="22"/>
         <v>3.9046742999999999</v>
       </c>
-      <c r="AO25" s="2">
+      <c r="AO25" s="37">
         <f t="shared" si="23"/>
         <v>46.567659646009965</v>
       </c>
-    </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP25" s="40">
+        <f t="shared" si="24"/>
+        <v>3.3815067251001993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -8207,7 +8274,7 @@
         <v>0.01</v>
       </c>
       <c r="AF26" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG26" s="15">
@@ -8237,16 +8304,20 @@
         <f t="shared" si="21"/>
         <v>2.6005565417439914E-4</v>
       </c>
-      <c r="AN26" s="2">
+      <c r="AN26" s="7">
         <f t="shared" si="22"/>
         <v>2.9469240000000001</v>
       </c>
-      <c r="AO26" s="2">
+      <c r="AO26" s="37">
         <f t="shared" si="23"/>
         <v>44.898280449625048</v>
       </c>
-    </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP26" s="8">
+        <f t="shared" si="24"/>
+        <v>0.26971969939369633</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>63</v>
       </c>
@@ -8357,7 +8428,7 @@
         <v>0.01</v>
       </c>
       <c r="AF27" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG27" s="15">
@@ -8387,16 +8458,19 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AN27" s="2">
+      <c r="AN27" s="7">
         <f t="shared" si="22"/>
         <v>1.9155005999999999</v>
       </c>
-      <c r="AO27" s="2">
+      <c r="AO27" s="23">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP27" s="39" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
@@ -8455,7 +8529,7 @@
         <v>1.4974946581424107</v>
       </c>
       <c r="R28" s="22">
-        <f t="shared" ref="R28:R41" si="25">O28*9.81/P28^2</f>
+        <f t="shared" ref="R28:R41" si="26">O28*9.81/P28^2</f>
         <v>0.24428620768088338</v>
       </c>
       <c r="S28" s="25">
@@ -8506,7 +8580,7 @@
         <v>0.01</v>
       </c>
       <c r="AF28" s="15">
-        <f t="shared" ref="AF28:AF41" si="26">L28*AD28</f>
+        <f t="shared" ref="AF28:AF41" si="27">L28*AD28</f>
         <v>0</v>
       </c>
       <c r="AG28" s="15">
@@ -8517,7 +8591,7 @@
         <v>0</v>
       </c>
       <c r="AI28" s="15">
-        <f t="shared" ref="AI28:AI41" si="27">SQRT(AF28^2+(16*K28/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y28)^2)</f>
+        <f t="shared" ref="AI28:AI41" si="28">SQRT(AF28^2+(16*K28/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y28)^2)</f>
         <v>0</v>
       </c>
       <c r="AJ28" s="3">
@@ -8535,11 +8609,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO28" s="2">
+      <c r="AO28" s="23">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>63</v>
       </c>
@@ -8598,7 +8672,7 @@
         <v>1.2354330929674888</v>
       </c>
       <c r="R29" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.39199414720885933</v>
       </c>
       <c r="S29" s="25">
@@ -8649,7 +8723,7 @@
         <v>0.01</v>
       </c>
       <c r="AF29" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG29" s="15">
@@ -8660,7 +8734,7 @@
         <v>0</v>
       </c>
       <c r="AI29" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ29" s="3">
@@ -8678,11 +8752,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO29" s="2">
+      <c r="AO29" s="23">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>63</v>
       </c>
@@ -8741,7 +8815,7 @@
         <v>0.97337152779256686</v>
       </c>
       <c r="R30" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.46963550003766724</v>
       </c>
       <c r="S30" s="25">
@@ -8792,7 +8866,7 @@
         <v>0.01</v>
       </c>
       <c r="AF30" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG30" s="15">
@@ -8803,7 +8877,7 @@
         <v>0</v>
       </c>
       <c r="AI30" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ30" s="3">
@@ -8821,11 +8895,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO30" s="2">
+      <c r="AO30" s="23">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -8884,7 +8958,7 @@
         <v>0.74874732907120534</v>
       </c>
       <c r="R31" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.51129671375068619</v>
       </c>
       <c r="S31" s="25">
@@ -8935,7 +9009,7 @@
         <v>0.01</v>
       </c>
       <c r="AF31" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG31" s="15">
@@ -8946,7 +9020,7 @@
         <v>0</v>
       </c>
       <c r="AI31" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ31" s="3">
@@ -8964,11 +9038,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO31" s="2">
+      <c r="AO31" s="23">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -9027,7 +9101,7 @@
         <v>2.2462419872136161</v>
       </c>
       <c r="R32" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.24281333648900894</v>
       </c>
       <c r="S32" s="25">
@@ -9078,7 +9152,7 @@
         <v>0.01</v>
       </c>
       <c r="AF32" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG32" s="15">
@@ -9089,7 +9163,7 @@
         <v>0</v>
       </c>
       <c r="AI32" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ32" s="3">
@@ -9107,7 +9181,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO32" s="2">
+      <c r="AO32" s="23">
         <v>52</v>
       </c>
     </row>
@@ -9170,7 +9244,7 @@
         <v>1.8718683226780133</v>
       </c>
       <c r="R33" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.3837881505684162</v>
       </c>
       <c r="S33" s="25">
@@ -9221,7 +9295,7 @@
         <v>0.01</v>
       </c>
       <c r="AF33" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG33" s="15">
@@ -9232,7 +9306,7 @@
         <v>0</v>
       </c>
       <c r="AI33" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ33" s="3">
@@ -9250,7 +9324,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO33" s="2">
+      <c r="AO33" s="23">
         <v>71</v>
       </c>
     </row>
@@ -9313,7 +9387,7 @@
         <v>1.4974946581424107</v>
       </c>
       <c r="R34" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.46290237458909855</v>
       </c>
       <c r="S34" s="25">
@@ -9364,7 +9438,7 @@
         <v>0.01</v>
       </c>
       <c r="AF34" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG34" s="15">
@@ -9375,7 +9449,7 @@
         <v>0</v>
       </c>
       <c r="AI34" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ34" s="3">
@@ -9393,7 +9467,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO34" s="2">
+      <c r="AO34" s="23">
         <v>73</v>
       </c>
     </row>
@@ -9456,7 +9530,7 @@
         <v>1.1231209936068081</v>
       </c>
       <c r="R35" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.50919261204800836</v>
       </c>
       <c r="S35" s="25">
@@ -9507,7 +9581,7 @@
         <v>0.01</v>
       </c>
       <c r="AF35" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG35" s="15">
@@ -9518,7 +9592,7 @@
         <v>0</v>
       </c>
       <c r="AI35" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ35" s="3">
@@ -9536,7 +9610,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO35" s="2">
+      <c r="AO35" s="23">
         <v>69</v>
       </c>
     </row>
@@ -9599,7 +9673,7 @@
         <v>0.74874732907120534</v>
       </c>
       <c r="R36" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.53865003588549654</v>
       </c>
       <c r="S36" s="25">
@@ -9650,7 +9724,7 @@
         <v>0.01</v>
       </c>
       <c r="AF36" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG36" s="15">
@@ -9661,7 +9735,7 @@
         <v>0</v>
       </c>
       <c r="AI36" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ36" s="3">
@@ -9679,7 +9753,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO36" s="2">
+      <c r="AO36" s="23">
         <v>58</v>
       </c>
     </row>
@@ -9742,7 +9816,7 @@
         <v>2.9949893162848213</v>
       </c>
       <c r="R37" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.2438127847977809</v>
       </c>
       <c r="S37" s="25">
@@ -9793,7 +9867,7 @@
         <v>0.01</v>
       </c>
       <c r="AF37" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG37" s="15">
@@ -9804,7 +9878,7 @@
         <v>0</v>
       </c>
       <c r="AI37" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ37" s="3">
@@ -9822,7 +9896,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO37" s="3">
+      <c r="AO37" s="23">
         <v>52</v>
       </c>
     </row>
@@ -9885,7 +9959,7 @@
         <v>2.5083035523885377</v>
       </c>
       <c r="R38" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.38110542089750221</v>
       </c>
       <c r="S38" s="25">
@@ -9936,7 +10010,7 @@
         <v>0.01</v>
       </c>
       <c r="AF38" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG38" s="15">
@@ -9947,7 +10021,7 @@
         <v>0</v>
       </c>
       <c r="AI38" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ38" s="3">
@@ -9965,7 +10039,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO38" s="3">
+      <c r="AO38" s="23">
         <v>71</v>
       </c>
     </row>
@@ -10028,7 +10102,7 @@
         <v>2.0216177884922546</v>
       </c>
       <c r="R39" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.45448596777838768</v>
       </c>
       <c r="S39" s="25">
@@ -10079,7 +10153,7 @@
         <v>0.01</v>
       </c>
       <c r="AF39" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG39" s="15">
@@ -10090,7 +10164,7 @@
         <v>0</v>
       </c>
       <c r="AI39" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ39" s="3">
@@ -10108,7 +10182,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO39" s="3">
+      <c r="AO39" s="23">
         <v>73</v>
       </c>
     </row>
@@ -10171,7 +10245,7 @@
         <v>1.4974946581424107</v>
       </c>
       <c r="R40" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.51129671375068619</v>
       </c>
       <c r="S40" s="25">
@@ -10222,7 +10296,7 @@
         <v>0.01</v>
       </c>
       <c r="AF40" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG40" s="15">
@@ -10233,7 +10307,7 @@
         <v>0</v>
       </c>
       <c r="AI40" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ40" s="3">
@@ -10251,7 +10325,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO40" s="6">
+      <c r="AO40" s="38">
         <v>69</v>
       </c>
     </row>
@@ -10314,7 +10388,7 @@
         <v>1.0108088942461273</v>
       </c>
       <c r="R41" s="22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.5397020867368354</v>
       </c>
       <c r="S41" s="25">
@@ -10365,7 +10439,7 @@
         <v>0.01</v>
       </c>
       <c r="AF41" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG41" s="15">
@@ -10376,7 +10450,7 @@
         <v>0</v>
       </c>
       <c r="AI41" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AJ41" s="3">
@@ -10394,7 +10468,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO41" s="3">
+      <c r="AO41" s="23">
         <v>59</v>
       </c>
     </row>
@@ -10447,23 +10521,23 @@
         <v>9.8417294323611557</v>
       </c>
       <c r="O42" s="8">
-        <f t="shared" ref="O42:O49" si="28">N42+8*K42^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
+        <f t="shared" ref="O42:O49" si="29">N42+8*K42^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
         <v>11.256986832203168</v>
       </c>
       <c r="P42" s="8">
-        <f t="shared" ref="P42:P44" si="29">$B$7/2*2*PI()/60*C42</f>
+        <f t="shared" ref="P42:P44" si="30">$B$7/2*2*PI()/60*C42</f>
         <v>15.268140296446393</v>
       </c>
       <c r="Q42" s="8">
-        <f t="shared" ref="Q42:Q45" si="30">K42/($B$8*(2*PI()*$B$7/2-$B$10*$B$9))</f>
+        <f t="shared" ref="Q42:Q45" si="31">K42/($B$8*(2*PI()*$B$7/2-$B$10*$B$9))</f>
         <v>2.7202780690215822</v>
       </c>
       <c r="R42" s="22">
-        <f t="shared" ref="R42:R45" si="31">O42*9.81/P42^2</f>
+        <f t="shared" ref="R42:R45" si="32">O42*9.81/P42^2</f>
         <v>0.47371690321318732</v>
       </c>
       <c r="S42" s="25">
-        <f t="shared" ref="S42:S45" si="32">Q42/P42</f>
+        <f t="shared" ref="S42:S45" si="33">Q42/P42</f>
         <v>0.17816695525483989</v>
       </c>
       <c r="T42" s="19">
@@ -10510,11 +10584,11 @@
         <v>0.01</v>
       </c>
       <c r="AF42" s="15">
-        <f t="shared" ref="AF42:AG42" si="33">L42*AD42/D42</f>
+        <f t="shared" ref="AF42:AG42" si="34">L42*AD42/D42</f>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG42" s="15">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AH42" s="15">
@@ -10590,23 +10664,23 @@
         <v>10.633997454644252</v>
       </c>
       <c r="O43" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>11.692307952536082</v>
       </c>
       <c r="P43" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q43" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>2.352351058303686</v>
       </c>
       <c r="R43" s="22">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.49203610142326842</v>
       </c>
       <c r="S43" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.1540692587722152</v>
       </c>
       <c r="T43" s="19">
@@ -10653,19 +10727,19 @@
         <v>0.01</v>
       </c>
       <c r="AF43" s="15">
-        <f t="shared" ref="AF43:AF49" si="34">L43*AD43/D43</f>
+        <f t="shared" ref="AF43:AF49" si="35">L43*AD43/D43</f>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG43" s="15">
-        <f t="shared" ref="AG43:AG49" si="35">M43*AE43/E43</f>
+        <f t="shared" ref="AG43:AG49" si="36">M43*AE43/E43</f>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AH43" s="15">
-        <f t="shared" ref="AH43:AH45" si="36">SQRT((AF43/2)^2+(AG43/2)^2)</f>
+        <f t="shared" ref="AH43:AH45" si="37">SQRT((AF43/2)^2+(AG43/2)^2)</f>
         <v>2.4898581825494825E-2</v>
       </c>
       <c r="AI43" s="15">
-        <f t="shared" ref="AI43:AI49" si="37">SQRT(AH43^2+(16*K43/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y43)^2)</f>
+        <f t="shared" ref="AI43:AI49" si="38">SQRT(AH43^2+(16*K43/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y43)^2)</f>
         <v>4.1133546763215144E-2</v>
       </c>
       <c r="AJ43" s="3">
@@ -10717,7 +10791,7 @@
         <v>41.01</v>
       </c>
       <c r="K44" s="9">
-        <f t="shared" ref="K44:K48" si="38">$D$3/$B$2/J44</f>
+        <f t="shared" ref="K44:K48" si="39">$D$3/$B$2/J44</f>
         <v>2.2165398829846967E-3</v>
       </c>
       <c r="L44" s="8">
@@ -10733,19 +10807,19 @@
         <v>12.41219901576854</v>
       </c>
       <c r="O44" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>12.543894388300366</v>
       </c>
       <c r="P44" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q44" s="7">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.82981415858229679</v>
       </c>
       <c r="R44" s="22">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.52787259081264604</v>
       </c>
       <c r="S44" s="25">
@@ -10796,19 +10870,19 @@
         <v>0.01</v>
       </c>
       <c r="AF44" s="15">
-        <f t="shared" si="34"/>
-        <v>3.5211912101471038E-2</v>
-      </c>
-      <c r="AG44" s="15">
         <f t="shared" si="35"/>
         <v>3.5211912101471038E-2</v>
       </c>
+      <c r="AG44" s="15">
+        <f t="shared" si="36"/>
+        <v>3.5211912101471038E-2</v>
+      </c>
       <c r="AH44" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2.4898581825494828E-2</v>
       </c>
       <c r="AI44" s="15">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>2.4937819217776595E-2</v>
       </c>
       <c r="AJ44" s="3">
@@ -10875,7 +10949,7 @@
         <v>12.500228796022217</v>
       </c>
       <c r="O45" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>12.500228796022217</v>
       </c>
       <c r="P45" s="8">
@@ -10883,15 +10957,15 @@
         <v>15.268140296446393</v>
       </c>
       <c r="Q45" s="7">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="R45" s="22">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.52603505387142835</v>
       </c>
       <c r="S45" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="T45" s="19">
@@ -10938,19 +11012,19 @@
         <v>0.01</v>
       </c>
       <c r="AF45" s="15">
-        <f t="shared" si="34"/>
-        <v>3.5211912101471038E-2</v>
-      </c>
-      <c r="AG45" s="15">
         <f t="shared" si="35"/>
         <v>3.5211912101471038E-2</v>
       </c>
+      <c r="AG45" s="15">
+        <f t="shared" si="36"/>
+        <v>3.5211912101471038E-2</v>
+      </c>
       <c r="AH45" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2.4898581825494828E-2</v>
       </c>
       <c r="AI45" s="15">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>2.4898581825494828E-2</v>
       </c>
       <c r="AJ45" s="3">
@@ -11002,15 +11076,15 @@
         <v>16.28</v>
       </c>
       <c r="K46" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>5.5835565479854053E-3</v>
       </c>
       <c r="L46" s="7">
-        <f t="shared" ref="L46:L49" si="39">5*D46/($B$2*9.81)*6894.76</f>
+        <f t="shared" ref="L46:L49" si="40">5*D46/($B$2*9.81)*6894.76</f>
         <v>2.3944100229000305</v>
       </c>
       <c r="M46" s="7">
-        <f t="shared" ref="M46:M49" si="40">5*E46/($B$2*9.81)*6894.76</f>
+        <f t="shared" ref="M46:M49" si="41">5*E46/($B$2*9.81)*6894.76</f>
         <v>5.9156012330471341</v>
       </c>
       <c r="N46" s="7">
@@ -11018,11 +11092,11 @@
         <v>8.3100112559471651</v>
       </c>
       <c r="O46" s="7">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>9.1456936498984369</v>
       </c>
       <c r="P46" s="8">
-        <f t="shared" ref="P46:P49" si="41">$B$7/2*2*PI()/60*C46</f>
+        <f t="shared" ref="P46:P49" si="42">$B$7/2*2*PI()/60*C46</f>
         <v>15.268140296446393</v>
       </c>
       <c r="Q46" s="7">
@@ -11030,11 +11104,11 @@
         <v>2.0903365260110558</v>
       </c>
       <c r="R46" s="22">
-        <f t="shared" ref="R46:R49" si="42">O46*9.81/P46^2</f>
+        <f t="shared" ref="R46:R49" si="43">O46*9.81/P46^2</f>
         <v>0.38486939161840239</v>
       </c>
       <c r="S46" s="25">
-        <f t="shared" ref="S46:S49" si="43">Q46/P46</f>
+        <f t="shared" ref="S46:S49" si="44">Q46/P46</f>
         <v>0.13690839129226329</v>
       </c>
       <c r="T46" s="19">
@@ -11073,19 +11147,19 @@
         <v>0.01</v>
       </c>
       <c r="AD46" s="3">
-        <f t="shared" ref="AD46:AD49" si="44">SQRT(Z46^2+AB46^2)</f>
+        <f t="shared" ref="AD46:AD49" si="45">SQRT(Z46^2+AB46^2)</f>
         <v>0.01</v>
       </c>
       <c r="AE46" s="3">
-        <f t="shared" ref="AE46:AE49" si="45">SQRT(AA46^2+AC46^2)</f>
+        <f t="shared" ref="AE46:AE49" si="46">SQRT(AA46^2+AC46^2)</f>
         <v>0.01</v>
       </c>
       <c r="AF46" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG46" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AH46" s="15">
@@ -11093,7 +11167,7 @@
         <v>4.979716365098965E-2</v>
       </c>
       <c r="AI46" s="14">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>9.7683179625164276E-2</v>
       </c>
       <c r="AJ46" s="3">
@@ -11145,39 +11219,39 @@
         <v>16.683333333333334</v>
       </c>
       <c r="K47" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>5.4485694666055393E-3</v>
       </c>
       <c r="L47" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>3.1690720891323929</v>
       </c>
       <c r="M47" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>6.4789918266706712</v>
       </c>
       <c r="N47" s="7">
-        <f t="shared" ref="N47:N49" si="46">L47+M47</f>
+        <f t="shared" ref="N47:N49" si="47">L47+M47</f>
         <v>9.6480639158030641</v>
       </c>
       <c r="O47" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>10.443828120193732</v>
       </c>
       <c r="P47" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q47" s="7">
-        <f t="shared" ref="Q47:Q49" si="47">K47/($B$8*(2*PI()*$B$7/2-$B$10*$B$9))</f>
+        <f t="shared" ref="Q47:Q49" si="48">K47/($B$8*(2*PI()*$B$7/2-$B$10*$B$9))</f>
         <v>2.0398009176899095</v>
       </c>
       <c r="R47" s="22">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.43949753060346181</v>
       </c>
       <c r="S47" s="25">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.13359851809618661</v>
       </c>
       <c r="T47" s="19">
@@ -11216,27 +11290,27 @@
         <v>0.01</v>
       </c>
       <c r="AD47" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.01</v>
       </c>
       <c r="AE47" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.01</v>
       </c>
       <c r="AF47" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG47" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AH47" s="15">
-        <f t="shared" ref="AH47:AH49" si="48">SQRT(AF47^2+AG47^2)</f>
+        <f t="shared" ref="AH47:AH49" si="49">SQRT(AF47^2+AG47^2)</f>
         <v>4.979716365098965E-2</v>
       </c>
       <c r="AI47" s="15">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>5.7694103995025177E-2</v>
       </c>
       <c r="AJ47" s="3">
@@ -11288,39 +11362,39 @@
         <v>30.473333333333333</v>
       </c>
       <c r="K48" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>2.9829457646423892E-3</v>
       </c>
       <c r="L48" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>10.17624259732513</v>
       </c>
       <c r="M48" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>11.479083345079555</v>
       </c>
       <c r="N48" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>21.655325942404687</v>
       </c>
       <c r="O48" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>21.893837884806008</v>
       </c>
       <c r="P48" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q48" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>1.1167363370201266</v>
       </c>
       <c r="R48" s="22">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.92133723143140611</v>
       </c>
       <c r="S48" s="25">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>7.3141608299213956E-2</v>
       </c>
       <c r="T48" s="19">
@@ -11359,27 +11433,27 @@
         <v>0.01</v>
       </c>
       <c r="AD48" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.01</v>
       </c>
       <c r="AE48" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.01</v>
       </c>
       <c r="AF48" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG48" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AH48" s="15">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>4.979716365098965E-2</v>
       </c>
       <c r="AI48" s="15">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>5.0647966676196698E-2</v>
       </c>
       <c r="AJ48" s="3">
@@ -11434,35 +11508,35 @@
         <v>0</v>
       </c>
       <c r="L49" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>12.394593059717804</v>
       </c>
       <c r="M49" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>12.500228796022217</v>
       </c>
       <c r="N49" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>24.89482185574002</v>
       </c>
       <c r="O49" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>24.89482185574002</v>
       </c>
       <c r="P49" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q49" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="R49" s="22">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>1.0476247410904223</v>
       </c>
       <c r="S49" s="25">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="T49" s="19">
@@ -11501,27 +11575,27 @@
         <v>0.01</v>
       </c>
       <c r="AD49" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.01</v>
       </c>
       <c r="AE49" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.01</v>
       </c>
       <c r="AF49" s="15">
-        <f t="shared" si="34"/>
-        <v>3.5211912101471038E-2</v>
-      </c>
-      <c r="AG49" s="15">
         <f t="shared" si="35"/>
         <v>3.5211912101471038E-2</v>
       </c>
+      <c r="AG49" s="15">
+        <f t="shared" si="36"/>
+        <v>3.5211912101471038E-2</v>
+      </c>
       <c r="AH49" s="15">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>4.9797163650989656E-2</v>
       </c>
       <c r="AI49" s="15">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>4.9797163650989656E-2</v>
       </c>
       <c r="AJ49" s="3">
@@ -11559,16 +11633,16 @@
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C54" s="33" t="s">
+      <c r="C54" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33" t="s">
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
     </row>
     <row r="55" spans="1:39" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">
@@ -11630,7 +11704,7 @@
         <v>11</v>
       </c>
       <c r="C57" s="9">
-        <f t="shared" ref="C57:C58" si="49">K43</f>
+        <f t="shared" ref="C57:C58" si="50">K43</f>
         <v>6.2834309171338068E-3</v>
       </c>
       <c r="D57" s="8">
@@ -11638,19 +11712,19 @@
         <v>10.633997454644252</v>
       </c>
       <c r="E57" s="8">
-        <f t="shared" ref="E57" si="50">O43</f>
+        <f t="shared" ref="E57" si="51">O43</f>
         <v>11.692307952536082</v>
       </c>
       <c r="F57" s="9">
-        <f t="shared" ref="F57:F59" si="51">2*K21</f>
+        <f t="shared" ref="F57:F59" si="52">2*K21</f>
         <v>9.4984640126648291E-3</v>
       </c>
       <c r="G57" s="7">
-        <f t="shared" ref="G57:G59" si="52">N21</f>
+        <f t="shared" ref="G57:G59" si="53">N21</f>
         <v>5.7043297604383083</v>
       </c>
       <c r="H57" s="7">
-        <f t="shared" ref="H57:H59" si="53">G57+8*F57^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
+        <f t="shared" ref="H57:H59" si="54">G57+8*F57^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
         <v>8.1227188682608311</v>
       </c>
     </row>
@@ -11662,27 +11736,27 @@
         <v>12</v>
       </c>
       <c r="C58" s="9">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>2.2165398829846967E-3</v>
       </c>
       <c r="D58" s="8">
-        <f t="shared" ref="D58:E58" si="54">N44</f>
+        <f t="shared" ref="D58:E58" si="55">N44</f>
         <v>12.41219901576854</v>
       </c>
       <c r="E58" s="8">
+        <f t="shared" si="55"/>
+        <v>12.543894388300366</v>
+      </c>
+      <c r="F58" s="9">
+        <f t="shared" si="52"/>
+        <v>5.8225878467728668E-3</v>
+      </c>
+      <c r="G58" s="8">
+        <f t="shared" si="53"/>
+        <v>10.352302157832483</v>
+      </c>
+      <c r="H58" s="8">
         <f t="shared" si="54"/>
-        <v>12.543894388300366</v>
-      </c>
-      <c r="F58" s="9">
-        <f t="shared" si="51"/>
-        <v>5.8225878467728668E-3</v>
-      </c>
-      <c r="G58" s="8">
-        <f t="shared" si="52"/>
-        <v>10.352302157832483</v>
-      </c>
-      <c r="H58" s="8">
-        <f t="shared" si="53"/>
         <v>11.261066993909452</v>
       </c>
     </row>
@@ -11698,23 +11772,23 @@
         <v>0</v>
       </c>
       <c r="D59" s="8">
-        <f t="shared" ref="D59:E59" si="55">N45</f>
+        <f t="shared" ref="D59:E59" si="56">N45</f>
         <v>12.500228796022217</v>
       </c>
       <c r="E59" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>12.500228796022217</v>
       </c>
       <c r="F59" s="13">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="G59" s="8">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>12.394593059717804</v>
       </c>
       <c r="H59" s="8">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>12.394593059717804</v>
       </c>
     </row>
@@ -11726,7 +11800,7 @@
         <v>10</v>
       </c>
       <c r="C60" s="27">
-        <f t="shared" ref="C60:C63" si="56">K46</f>
+        <f t="shared" ref="C60:C63" si="57">K46</f>
         <v>5.5835565479854053E-3</v>
       </c>
       <c r="D60" s="7">
@@ -11734,7 +11808,7 @@
         <v>8.3100112559471651</v>
       </c>
       <c r="E60" s="8">
-        <f t="shared" ref="E60" si="57">O46</f>
+        <f t="shared" ref="E60" si="58">O46</f>
         <v>9.1456936498984369</v>
       </c>
       <c r="F60" s="9">
@@ -11758,27 +11832,27 @@
         <v>11</v>
       </c>
       <c r="C61" s="27">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>5.4485694666055393E-3</v>
       </c>
       <c r="D61" s="7">
-        <f t="shared" ref="D61:E61" si="58">N47</f>
+        <f t="shared" ref="D61:E61" si="59">N47</f>
         <v>9.6480639158030641</v>
       </c>
       <c r="E61" s="8">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>10.443828120193732</v>
       </c>
       <c r="F61" s="9">
-        <f t="shared" ref="F61:F63" si="59">K21</f>
+        <f t="shared" ref="F61:F63" si="60">K21</f>
         <v>4.7492320063324146E-3</v>
       </c>
       <c r="G61" s="8">
-        <f t="shared" ref="G61:G63" si="60">2*N21</f>
+        <f t="shared" ref="G61:G63" si="61">2*N21</f>
         <v>11.408659520876617</v>
       </c>
       <c r="H61" s="8">
-        <f t="shared" ref="H61:H63" si="61">G61+8*F61^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
+        <f t="shared" ref="H61:H63" si="62">G61+8*F61^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
         <v>12.013256797832247</v>
       </c>
     </row>
@@ -11790,27 +11864,27 @@
         <v>12</v>
       </c>
       <c r="C62" s="27">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>2.9829457646423892E-3</v>
       </c>
       <c r="D62" s="8">
-        <f t="shared" ref="D62:E62" si="62">N48</f>
+        <f t="shared" ref="D62:E62" si="63">N48</f>
         <v>21.655325942404687</v>
       </c>
       <c r="E62" s="8">
+        <f t="shared" si="63"/>
+        <v>21.893837884806008</v>
+      </c>
+      <c r="F62" s="9">
+        <f t="shared" si="60"/>
+        <v>2.9112939233864334E-3</v>
+      </c>
+      <c r="G62" s="3">
+        <f t="shared" si="61"/>
+        <v>20.704604315664966</v>
+      </c>
+      <c r="H62" s="8">
         <f t="shared" si="62"/>
-        <v>21.893837884806008</v>
-      </c>
-      <c r="F62" s="9">
-        <f t="shared" si="59"/>
-        <v>2.9112939233864334E-3</v>
-      </c>
-      <c r="G62" s="3">
-        <f t="shared" si="60"/>
-        <v>20.704604315664966</v>
-      </c>
-      <c r="H62" s="8">
-        <f t="shared" si="61"/>
         <v>20.931795524684208</v>
       </c>
     </row>
@@ -11822,27 +11896,27 @@
         <v>13</v>
       </c>
       <c r="C63" s="13">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="D63" s="8">
-        <f t="shared" ref="D63:E63" si="63">N49</f>
+        <f t="shared" ref="D63:E63" si="64">N49</f>
         <v>24.89482185574002</v>
       </c>
       <c r="E63" s="8">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>24.89482185574002</v>
       </c>
       <c r="F63" s="13">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="G63" s="8">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>24.789186119435609</v>
       </c>
       <c r="H63" s="8">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>24.789186119435609</v>
       </c>
     </row>
@@ -11966,11 +12040,11 @@
         <v>0.108</v>
       </c>
       <c r="C68" s="22">
-        <f t="shared" ref="C68:C86" si="64">$B$8</f>
+        <f t="shared" ref="C68:C86" si="65">$B$8</f>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D68" s="3">
-        <f t="shared" ref="D68:D86" si="65">$B$9</f>
+        <f t="shared" ref="D68:D86" si="66">$B$9</f>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E68" s="10">
@@ -11986,19 +12060,19 @@
         <v>71</v>
       </c>
       <c r="I68" s="8">
-        <f t="shared" ref="I68:I106" si="66">B68/2*F68*2*PI()/60</f>
+        <f t="shared" ref="I68:I106" si="67">B68/2*F68*2*PI()/60</f>
         <v>20.357520395261862</v>
       </c>
       <c r="J68" s="14">
-        <f t="shared" ref="J68:J106" si="67">E68/(C68*(2*PI()*B68/2-$B$10*D68))</f>
+        <f t="shared" ref="J68:J106" si="68">E68/(C68*(2*PI()*B68/2-$B$10*D68))</f>
         <v>2.5083035523885377</v>
       </c>
       <c r="K68" s="7">
-        <f t="shared" ref="K68:K106" si="68">G68*9.81/I68^2</f>
+        <f t="shared" ref="K68:K106" si="69">G68*9.81/I68^2</f>
         <v>0.38110542089750205</v>
       </c>
       <c r="L68" s="7">
-        <f t="shared" ref="L68:L106" si="69">J68/I68</f>
+        <f t="shared" ref="L68:L106" si="70">J68/I68</f>
         <v>0.123212626277036</v>
       </c>
     </row>
@@ -12010,11 +12084,11 @@
         <v>0.108</v>
       </c>
       <c r="C69" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D69" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E69" s="10">
@@ -12030,19 +12104,19 @@
         <v>73</v>
       </c>
       <c r="I69" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J69" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.0216177884922546</v>
       </c>
       <c r="K69" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.45922019660941232</v>
       </c>
       <c r="L69" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>9.9305698790446928E-2</v>
       </c>
       <c r="M69" s="8"/>
@@ -12056,11 +12130,11 @@
         <v>0.108</v>
       </c>
       <c r="C70" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D70" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E70" s="30">
@@ -12076,19 +12150,19 @@
         <v>69</v>
       </c>
       <c r="I70" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J70" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.4974946581424107</v>
       </c>
       <c r="K70" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.51129671375068597</v>
       </c>
       <c r="L70" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>7.3559776881812533E-2</v>
       </c>
       <c r="M70" s="8"/>
@@ -12102,11 +12176,11 @@
         <v>0.108</v>
       </c>
       <c r="C71" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D71" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E71" s="30">
@@ -12122,19 +12196,19 @@
         <v>59</v>
       </c>
       <c r="I71" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J71" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.0108088942461273</v>
       </c>
       <c r="K71" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.53970208673683517</v>
       </c>
       <c r="L71" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>4.9652849395223464E-2</v>
       </c>
       <c r="M71" s="8"/>
@@ -12148,11 +12222,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C72" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D72" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E72" s="10">
@@ -12168,19 +12242,19 @@
         <v>47</v>
       </c>
       <c r="I72" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J72" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>3.0381988876492994</v>
       </c>
       <c r="K72" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.2096493445655927</v>
       </c>
       <c r="L72" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.15802103629597514</v>
       </c>
       <c r="M72" s="8"/>
@@ -12194,11 +12268,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C73" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D73" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E73" s="10">
@@ -12214,19 +12288,19 @@
         <v>66</v>
       </c>
       <c r="I73" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J73" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.518506972656656</v>
       </c>
       <c r="K73" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.34499259232312718</v>
       </c>
       <c r="L73" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.13099112219271625</v>
       </c>
       <c r="M73" s="8"/>
@@ -12240,11 +12314,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C74" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D74" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E74" s="10">
@@ -12260,19 +12334,19 @@
         <v>69</v>
       </c>
       <c r="I74" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J74" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.9988150576640129</v>
       </c>
       <c r="K74" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.43256763498976725</v>
       </c>
       <c r="L74" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.10396120808945734</v>
       </c>
       <c r="M74" s="8"/>
@@ -12286,11 +12360,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C75" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D75" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E75" s="10">
@@ -12306,19 +12380,19 @@
         <v>64</v>
       </c>
       <c r="I75" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J75" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.5190994438246497</v>
       </c>
       <c r="K75" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.47768205090894539</v>
       </c>
       <c r="L75" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>7.9010518147987568E-2</v>
       </c>
       <c r="M75" s="8"/>
@@ -12332,11 +12406,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C76" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D76" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E76" s="10">
@@ -12352,19 +12426,19 @@
         <v>54</v>
       </c>
       <c r="I76" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J76" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>0.99940752883200645</v>
       </c>
       <c r="K76" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.50952752096954168</v>
       </c>
       <c r="L76" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>5.1980604044728672E-2</v>
       </c>
       <c r="M76" s="8"/>
@@ -12378,11 +12452,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C77" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D77" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E77" s="10">
@@ -12398,19 +12472,19 @@
         <v>45</v>
       </c>
       <c r="I77" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J77" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>3.0448109727843837</v>
       </c>
       <c r="K77" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.19922596561183958</v>
       </c>
       <c r="L77" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.16826274899273511</v>
       </c>
       <c r="M77" s="8"/>
@@ -12424,11 +12498,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C78" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D78" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E78" s="10">
@@ -12444,19 +12518,19 @@
         <v>62</v>
       </c>
       <c r="I78" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J78" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.5301950337222343</v>
       </c>
       <c r="K78" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.32954671003462188</v>
       </c>
       <c r="L78" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.13982397451508971</v>
       </c>
       <c r="M78" s="8"/>
@@ -12470,11 +12544,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C79" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D79" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E79" s="30">
@@ -12490,19 +12564,19 @@
         <v>65</v>
       </c>
       <c r="I79" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J79" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.0155790946600849</v>
       </c>
       <c r="K79" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.41642720631647673</v>
       </c>
       <c r="L79" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.11138520003744436</v>
       </c>
       <c r="M79" s="8"/>
@@ -12516,11 +12590,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C80" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D80" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E80" s="10">
@@ -12536,19 +12610,19 @@
         <v>60</v>
       </c>
       <c r="I80" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J80" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.5009631555979355</v>
       </c>
       <c r="K80" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.47334891077700236</v>
       </c>
       <c r="L80" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>8.2946425559798975E-2</v>
       </c>
       <c r="M80" s="8"/>
@@ -12562,11 +12636,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C81" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D81" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E81" s="10">
@@ -12582,19 +12656,19 @@
         <v>52</v>
       </c>
       <c r="I81" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J81" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.0292318781242986</v>
       </c>
       <c r="K81" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.50330770259833157</v>
       </c>
       <c r="L81" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>5.6877548955290728E-2</v>
       </c>
       <c r="M81" s="8"/>
@@ -12608,11 +12682,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C82" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D82" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E82" s="10">
@@ -12628,19 +12702,19 @@
         <v>24</v>
       </c>
       <c r="I82" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J82" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>3.0036608329602066</v>
       </c>
       <c r="K82" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.10300153568634084</v>
       </c>
       <c r="L82" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.19198693531611913</v>
       </c>
       <c r="M82" s="8"/>
@@ -12654,11 +12728,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C83" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D83" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E83" s="10">
@@ -12674,19 +12748,19 @@
         <v>43</v>
       </c>
       <c r="I83" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J83" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.4945657765262732</v>
       </c>
       <c r="K83" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.23846659040222878</v>
       </c>
       <c r="L83" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.15944677678796335</v>
       </c>
       <c r="M83" s="8"/>
@@ -12700,11 +12774,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C84" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D84" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E84" s="10">
@@ -12720,19 +12794,19 @@
         <v>53</v>
       </c>
       <c r="I84" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J84" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.98547072009234</v>
       </c>
       <c r="K84" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.33705950004752</v>
       </c>
       <c r="L84" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.12690661825980756</v>
       </c>
       <c r="M84" s="8"/>
@@ -12746,11 +12820,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C85" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D85" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E85" s="10">
@@ -12766,19 +12840,19 @@
         <v>51</v>
       </c>
       <c r="I85" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J85" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.4763756636584067</v>
       </c>
       <c r="K85" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.39717712788001464</v>
       </c>
       <c r="L85" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>9.4366459731651781E-2</v>
       </c>
       <c r="M85" s="8"/>
@@ -12792,11 +12866,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C86" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D86" s="3">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E86" s="10">
@@ -12812,19 +12886,19 @@
         <v>38</v>
       </c>
       <c r="I86" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J86" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.0181901128678668</v>
       </c>
       <c r="K86" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.42082339482746262</v>
       </c>
       <c r="L86" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>6.5080317056311579E-2</v>
       </c>
     </row>
@@ -12856,19 +12930,19 @@
         <v>52</v>
       </c>
       <c r="I87" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J87" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.9949893162848213</v>
       </c>
       <c r="K87" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.24381278479778079</v>
       </c>
       <c r="L87" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.14711955376362507</v>
       </c>
     </row>
@@ -12880,11 +12954,11 @@
         <v>0.108</v>
       </c>
       <c r="C88" s="22">
-        <f t="shared" ref="C88:C106" si="70">$B$8*B88/$B$7</f>
+        <f t="shared" ref="C88:C106" si="71">$B$8*B88/$B$7</f>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D88" s="3">
-        <f t="shared" ref="D88:D91" si="71">$B$9*B88/$B$7</f>
+        <f t="shared" ref="D88:D91" si="72">$B$9*B88/$B$7</f>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E88" s="10">
@@ -12900,19 +12974,19 @@
         <v>71</v>
       </c>
       <c r="I88" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J88" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.5083035523885377</v>
       </c>
       <c r="K88" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.38110542089750205</v>
       </c>
       <c r="L88" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.123212626277036</v>
       </c>
     </row>
@@ -12924,11 +12998,11 @@
         <v>0.108</v>
       </c>
       <c r="C89" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D89" s="3">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E89" s="10">
@@ -12944,19 +13018,19 @@
         <v>73</v>
       </c>
       <c r="I89" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J89" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.0216177884922546</v>
       </c>
       <c r="K89" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.45922019660941232</v>
       </c>
       <c r="L89" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>9.9305698790446928E-2</v>
       </c>
     </row>
@@ -12968,11 +13042,11 @@
         <v>0.108</v>
       </c>
       <c r="C90" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D90" s="3">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E90" s="30">
@@ -12992,15 +13066,15 @@
         <v>20.357520395261862</v>
       </c>
       <c r="J90" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.4974946581424107</v>
       </c>
       <c r="K90" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.51129671375068597</v>
       </c>
       <c r="L90" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>7.3559776881812533E-2</v>
       </c>
     </row>
@@ -13012,11 +13086,11 @@
         <v>0.108</v>
       </c>
       <c r="C91" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D91" s="3">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E91" s="30">
@@ -13032,19 +13106,19 @@
         <v>59</v>
       </c>
       <c r="I91" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J91" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.0108088942461273</v>
       </c>
       <c r="K91" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.53970208673683517</v>
       </c>
       <c r="L91" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>4.9652849395223464E-2</v>
       </c>
     </row>
@@ -13056,11 +13130,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C92" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D92" s="3">
-        <f t="shared" ref="D92:D106" si="72">$B$9*B92/$B$7</f>
+        <f t="shared" ref="D92:D106" si="73">$B$9*B92/$B$7</f>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E92" s="10">
@@ -13076,19 +13150,19 @@
         <v>47</v>
       </c>
       <c r="I92" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J92" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>3.1898190711158065</v>
       </c>
       <c r="K92" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.2096493445655927</v>
       </c>
       <c r="L92" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.16590701723427406</v>
       </c>
     </row>
@@ -13100,11 +13174,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C93" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D93" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E93" s="10">
@@ -13120,19 +13194,19 @@
         <v>66</v>
       </c>
       <c r="I93" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J93" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.6441921247407345</v>
       </c>
       <c r="K93" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.34499259232312718</v>
       </c>
       <c r="L93" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.13752818533893771</v>
       </c>
     </row>
@@ -13144,11 +13218,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C94" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D94" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E94" s="10">
@@ -13164,19 +13238,19 @@
         <v>69</v>
       </c>
       <c r="I94" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J94" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.0985651783656625</v>
       </c>
       <c r="K94" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.43256763498976725</v>
       </c>
       <c r="L94" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.10914935344360137</v>
       </c>
     </row>
@@ -13188,11 +13262,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C95" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D95" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E95" s="10">
@@ -13208,19 +13282,19 @@
         <v>64</v>
       </c>
       <c r="I95" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J95" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.5949095355579033</v>
       </c>
       <c r="K95" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.47768205090894539</v>
       </c>
       <c r="L95" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>8.2953508617137031E-2</v>
       </c>
     </row>
@@ -13232,11 +13306,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C96" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D96" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E96" s="10">
@@ -13252,19 +13326,19 @@
         <v>54</v>
       </c>
       <c r="I96" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J96" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.0492825891828312</v>
       </c>
       <c r="K96" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.50952752096954168</v>
       </c>
       <c r="L96" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>5.4574676721800684E-2</v>
       </c>
     </row>
@@ -13276,11 +13350,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C97" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D97" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E97" s="10">
@@ -13296,19 +13370,19 @@
         <v>45</v>
       </c>
       <c r="I97" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J97" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>3.3640983511628928</v>
       </c>
       <c r="K97" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.19922596561183958</v>
       </c>
       <c r="L97" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.18590725056766289</v>
       </c>
     </row>
@@ -13320,11 +13394,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C98" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D98" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E98" s="10">
@@ -13340,19 +13414,19 @@
         <v>62</v>
       </c>
       <c r="I98" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J98" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.7955183481494461</v>
       </c>
       <c r="K98" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.32954671003462188</v>
       </c>
       <c r="L98" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.15448630680974804</v>
       </c>
     </row>
@@ -13364,11 +13438,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C99" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D99" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E99" s="30">
@@ -13384,19 +13458,19 @@
         <v>65</v>
       </c>
       <c r="I99" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J99" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.2269383451359994</v>
       </c>
       <c r="K99" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.41642720631647673</v>
       </c>
       <c r="L99" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.12306536305183319</v>
       </c>
     </row>
@@ -13408,11 +13482,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C100" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D100" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E100" s="10">
@@ -13428,19 +13502,19 @@
         <v>60</v>
       </c>
       <c r="I100" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J100" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.6583583421225527</v>
       </c>
       <c r="K100" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.47334891077700236</v>
       </c>
       <c r="L100" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>9.1644419293918325E-2</v>
       </c>
     </row>
@@ -13452,11 +13526,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C101" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D101" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E101" s="10">
@@ -13472,19 +13546,19 @@
         <v>52</v>
       </c>
       <c r="I101" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J101" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.1371600060268932</v>
       </c>
       <c r="K101" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.50330770259833157</v>
       </c>
       <c r="L101" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>6.2841887515829697E-2</v>
       </c>
     </row>
@@ -13496,11 +13570,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C102" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D102" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E102" s="10">
@@ -13516,19 +13590,19 @@
         <v>24</v>
       </c>
       <c r="I102" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J102" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>3.7398021623668587</v>
       </c>
       <c r="K102" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.10300153568634084</v>
       </c>
       <c r="L102" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.23903935756082109</v>
       </c>
     </row>
@@ -13540,11 +13614,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C103" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D103" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E103" s="10">
@@ -13560,19 +13634,19 @@
         <v>43</v>
       </c>
       <c r="I103" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J103" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>3.1059373890843402</v>
       </c>
       <c r="K103" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.23846659040222878</v>
       </c>
       <c r="L103" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.19852421221152938</v>
       </c>
     </row>
@@ -13584,11 +13658,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C104" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D104" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E104" s="10">
@@ -13604,19 +13678,19 @@
         <v>53</v>
       </c>
       <c r="I104" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J104" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>2.4720726158018218</v>
       </c>
       <c r="K104" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.33705950004752</v>
       </c>
       <c r="L104" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.15800906686223767</v>
       </c>
     </row>
@@ -13628,11 +13702,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C105" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D105" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E105" s="10">
@@ -13648,19 +13722,19 @@
         <v>51</v>
       </c>
       <c r="I105" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J105" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.8382078425193034</v>
       </c>
       <c r="K105" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.39717712788001464</v>
       </c>
       <c r="L105" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.11749392151294595</v>
       </c>
     </row>
@@ -13672,11 +13746,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C106" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D106" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E106" s="10">
@@ -13692,19 +13766,19 @@
         <v>38</v>
       </c>
       <c r="I106" s="8">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J106" s="14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.2677295465650369</v>
       </c>
       <c r="K106" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.42082339482746262</v>
       </c>
       <c r="L106" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>8.1030290698583418E-2</v>
       </c>
     </row>
@@ -13712,7 +13786,7 @@
       <c r="A109" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B109" s="36">
+      <c r="B109" s="33">
         <f>I67^2/9.81</f>
         <v>42.245528709837174</v>
       </c>
@@ -13721,7 +13795,7 @@
       <c r="A110" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B110" s="36">
+      <c r="B110" s="33">
         <f>B109/2</f>
         <v>21.122764354918587</v>
       </c>
@@ -13730,7 +13804,7 @@
       <c r="A111" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B111" s="36">
+      <c r="B111" s="33">
         <f>N27</f>
         <v>21.760961678709098</v>
       </c>

</xml_diff>

<commit_message>
Changes (got a copy of a marked report) added more content to abstract added more to procedure added intro sentences to appendicies added more technical recommendations added more content to most of the questions added more to theory and reworded more
</commit_message>
<xml_diff>
--- a/Lab 1 - Pumps/data_and_analysis.xlsx
+++ b/Lab 1 - Pumps/data_and_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\LaTeX\MEC-E-403\Lab 1 - Pumps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73DA49B-7616-4D33-A38E-20070E2BDF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C39409-D381-4BEC-A56F-65F94C346794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="108">
   <si>
     <t>(V)</t>
   </si>
@@ -356,6 +356,12 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>average head</t>
+  </si>
+  <si>
+    <t>elevation err</t>
+  </si>
 </sst>
 </file>
 
@@ -423,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -518,8 +524,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,17 +539,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,41 +935,41 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="G13" s="35" t="s">
+      <c r="E13" s="39"/>
+      <c r="G13" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="L13" s="34" t="s">
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="L13" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="34"/>
+      <c r="M13" s="39"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="35" t="s">
+      <c r="Z13" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35" t="s">
+      <c r="AA13" s="37"/>
+      <c r="AB13" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35" t="s">
+      <c r="AC13" s="37"/>
+      <c r="AD13" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="35"/>
-      <c r="AF13" s="35" t="s">
+      <c r="AE13" s="37"/>
+      <c r="AF13" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="35"/>
+      <c r="AG13" s="37"/>
     </row>
     <row r="14" spans="1:39" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -987,11 +990,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -6007,8 +6010,8 @@
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="35"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
     </row>
@@ -6033,8 +6036,8 @@
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
-      <c r="K52" s="35"/>
-      <c r="L52" s="35"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
       <c r="M52" s="8"/>
       <c r="N52" s="8"/>
     </row>
@@ -6081,37 +6084,37 @@
       <c r="N58" s="8"/>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="34"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="35"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A60" s="34"/>
-      <c r="B60" s="35"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
-      <c r="H60" s="34"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="37"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
       <c r="M60" s="8"/>
       <c r="N60" s="8"/>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A61" s="34"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="35"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="35"/>
+      <c r="A61" s="39"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="37"/>
       <c r="M61" s="8"/>
       <c r="N61" s="8"/>
     </row>
@@ -6133,6 +6136,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="F59:H60"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="K61:L61"/>
     <mergeCell ref="AF13:AG13"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="K50:L50"/>
@@ -6143,14 +6154,6 @@
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
     <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="F59:H60"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="K61:L61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6159,10 +6162,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B530A311-2D6F-44F7-871F-14AF58E6CD82}">
-  <dimension ref="A1:AP111"/>
+  <dimension ref="A1:AR111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6206,7 +6209,7 @@
     <col min="43" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6217,7 +6220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -6228,7 +6231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -6245,7 +6248,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6256,7 +6259,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -6268,7 +6271,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -6280,7 +6283,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -6295,7 +6298,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -6306,8 +6309,12 @@
       <c r="C8" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="N8" s="22">
+        <f>(R38-R24)/R38*100</f>
+        <v>39.65641503161514</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -6317,8 +6324,9 @@
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="22"/>
+    </row>
+    <row r="10" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -6327,11 +6335,11 @@
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -6342,47 +6350,47 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="D13" s="34" t="s">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="D13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="G13" s="35" t="s">
+      <c r="E13" s="39"/>
+      <c r="G13" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="L13" s="34" t="s">
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="L13" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="34"/>
+      <c r="M13" s="39"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="35" t="s">
+      <c r="Z13" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35" t="s">
+      <c r="AA13" s="37"/>
+      <c r="AB13" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35" t="s">
+      <c r="AC13" s="37"/>
+      <c r="AD13" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="35"/>
-      <c r="AF13" s="35" t="s">
+      <c r="AE13" s="37"/>
+      <c r="AF13" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="35"/>
+      <c r="AG13" s="37"/>
       <c r="AO13" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:42" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" s="16" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>62</v>
       </c>
@@ -6401,11 +6409,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -6506,7 +6514,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
         <v>19</v>
@@ -6616,7 +6624,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>63</v>
       </c>
@@ -6697,15 +6705,15 @@
         <v>0.54726254786554984</v>
       </c>
       <c r="W16" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X16" s="15">
         <f>SQRT(V16^2+W16^2)</f>
-        <v>0.58266310703209379</v>
+        <v>0.54735390406600115</v>
       </c>
       <c r="Y16" s="21">
         <f>IFERROR(K16*(X16/J16), 0)</f>
-        <v>6.3959029818172578E-5</v>
+        <v>6.0083132514724753E-5</v>
       </c>
       <c r="Z16" s="15">
         <v>0</v>
@@ -6741,37 +6749,41 @@
       </c>
       <c r="AI16" s="15">
         <f t="shared" ref="AI16:AI26" si="2">SQRT(AH16^2+(16*K16/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y16)^2)</f>
-        <v>3.6840105816510794E-2</v>
+        <v>3.6652499942899805E-2</v>
       </c>
       <c r="AJ16" s="3">
         <v>0</v>
       </c>
       <c r="AK16" s="22">
         <f>IFERROR(Q16*Y16/K16, 0)</f>
-        <v>2.3944576373171149E-2</v>
+        <v>2.2493542496315726E-2</v>
       </c>
       <c r="AL16" s="22">
         <f>R16*AI16/O16</f>
-        <v>3.4881898218906493E-3</v>
+        <v>3.4704264391762748E-3</v>
       </c>
       <c r="AM16" s="28">
         <f>IFERROR(S16*AK16/Q16, 0)</f>
-        <v>2.3524059815009852E-3</v>
+        <v>2.2098509110717647E-3</v>
       </c>
       <c r="AN16" s="7">
         <f>$B$4*F16/100*9.81</f>
         <v>1.2892792500000001</v>
       </c>
-      <c r="AO16" s="37">
+      <c r="AO16" s="34">
         <f>$B$2*9.81*K16*O16/(AN16*C16*2*PI()/60)*100</f>
         <v>37.010451746090069</v>
       </c>
       <c r="AP16" s="8">
         <f>AO16*SQRT((Y16/K16)^2+(AI16/O16)^2)</f>
-        <v>0.88394101528140789</v>
-      </c>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+        <v>0.84446400040626601</v>
+      </c>
+      <c r="AR16" s="33">
+        <f>AO29-AO16</f>
+        <v>28.989548253909931</v>
+      </c>
+    </row>
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -6852,15 +6864,15 @@
         <v>0.51691557279860623</v>
       </c>
       <c r="W17" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X17" s="15">
         <f t="shared" ref="X17:X49" si="13">SQRT(V17^2+W17^2)</f>
-        <v>0.55425780048792384</v>
+        <v>0.51701229134490712</v>
       </c>
       <c r="Y17" s="21">
         <f t="shared" ref="Y17:Y49" si="14">IFERROR(K17*(X17/J17), 0)</f>
-        <v>5.4986020731283828E-5</v>
+        <v>5.1291021155125836E-5</v>
       </c>
       <c r="Z17" s="15">
         <v>0</v>
@@ -6896,37 +6908,41 @@
       </c>
       <c r="AI17" s="15">
         <f t="shared" si="2"/>
-        <v>3.6307594515548498E-2</v>
+        <v>3.6167160694871005E-2</v>
       </c>
       <c r="AJ17" s="3">
         <v>0</v>
       </c>
       <c r="AK17" s="22">
         <f t="shared" ref="AK17:AK49" si="19">IFERROR(Q17*Y17/K17, 0)</f>
-        <v>2.0585318079401348E-2</v>
+        <v>1.920200754761758E-2</v>
       </c>
       <c r="AL17" s="22">
         <f t="shared" ref="AL17:AL49" si="20">R17*AI17/O17</f>
-        <v>3.4377692148134039E-3</v>
+        <v>3.4244722979593569E-3</v>
       </c>
       <c r="AM17" s="28">
         <f t="shared" ref="AM17:AM49" si="21">IFERROR(S17*AK17/Q17, 0)</f>
-        <v>2.0223797083059789E-3</v>
+        <v>1.8864780361056916E-3</v>
       </c>
       <c r="AN17" s="7">
         <f t="shared" ref="AN17:AN27" si="22">$B$4*F17/100*9.81</f>
         <v>1.2524427</v>
       </c>
-      <c r="AO17" s="37">
+      <c r="AO17" s="34">
         <f t="shared" ref="AO17:AO27" si="23">$B$2*9.81*K17*O17/(AN17*C17*2*PI()/60)*100</f>
         <v>39.406990455603598</v>
       </c>
       <c r="AP17" s="8">
-        <f t="shared" ref="AP17:AP27" si="24">AO17*SQRT((Y17/K17)^2+(AI17/O17)^2)</f>
-        <v>0.85152620176970306</v>
-      </c>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+        <f t="shared" ref="AP17:AP26" si="24">AO17*SQRT((Y17/K17)^2+(AI17/O17)^2)</f>
+        <v>0.809873659825466</v>
+      </c>
+      <c r="AR17" s="33">
+        <f t="shared" ref="AR17:AR27" si="25">AO29-AO17</f>
+        <v>26.593009544396402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>63</v>
       </c>
@@ -7007,15 +7023,15 @@
         <v>0.42254688372518895</v>
       </c>
       <c r="W18" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X18" s="15">
         <f t="shared" si="13"/>
-        <v>0.46748889713646502</v>
+        <v>0.42266519722573365</v>
       </c>
       <c r="Y18" s="21">
         <f t="shared" si="14"/>
-        <v>1.1447793417230061E-5</v>
+        <v>1.035015781579207E-5</v>
       </c>
       <c r="Z18" s="15">
         <v>0</v>
@@ -7038,7 +7054,7 @@
         <v>0.01</v>
       </c>
       <c r="AF18" s="15">
-        <f t="shared" ref="AF18:AF27" si="25">L18*AD18/D18</f>
+        <f t="shared" ref="AF18:AF27" si="26">L18*AD18/D18</f>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG18" s="15">
@@ -7051,37 +7067,41 @@
       </c>
       <c r="AI18" s="15">
         <f t="shared" si="2"/>
-        <v>3.5223815341371312E-2</v>
+        <v>3.5221642462639861E-2</v>
       </c>
       <c r="AJ18" s="3">
         <v>0</v>
       </c>
       <c r="AK18" s="10">
         <f t="shared" si="19"/>
-        <v>4.2857523724549674E-3</v>
+        <v>3.8748265100198866E-3</v>
       </c>
       <c r="AL18" s="22">
         <f t="shared" si="20"/>
-        <v>3.3351520425563249E-3</v>
+        <v>3.33494630445359E-3</v>
       </c>
       <c r="AM18" s="28">
         <f t="shared" si="21"/>
-        <v>4.2104856478026285E-4</v>
+        <v>3.8067764981060653E-4</v>
       </c>
       <c r="AN18" s="7">
         <f t="shared" si="22"/>
         <v>1.0682599500000001</v>
       </c>
-      <c r="AO18" s="37">
+      <c r="AO18" s="34">
         <f t="shared" si="23"/>
         <v>36.959072152593905</v>
       </c>
       <c r="AP18" s="8">
         <f t="shared" si="24"/>
-        <v>0.38171822644471037</v>
-      </c>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+        <v>0.36196442368757586</v>
+      </c>
+      <c r="AR18" s="33">
+        <f t="shared" si="25"/>
+        <v>30.040927847406095</v>
+      </c>
+    </row>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>63</v>
       </c>
@@ -7192,7 +7212,7 @@
         <v>0.01</v>
       </c>
       <c r="AF19" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG19" s="15">
@@ -7233,8 +7253,9 @@
       <c r="AP19" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AR19" s="33"/>
+    </row>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -7315,15 +7336,15 @@
         <v>0.48573203778998497</v>
       </c>
       <c r="W20" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X20" s="15">
         <f t="shared" si="13"/>
-        <v>0.52529573816623654</v>
+        <v>0.48583496429920664</v>
       </c>
       <c r="Y20" s="21">
         <f t="shared" si="14"/>
-        <v>1.3635368819241931E-4</v>
+        <v>1.2611065428835632E-4</v>
       </c>
       <c r="Z20" s="15">
         <v>0</v>
@@ -7346,7 +7367,7 @@
         <v>0.01</v>
       </c>
       <c r="AF20" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG20" s="15">
@@ -7359,37 +7380,41 @@
       </c>
       <c r="AI20" s="15">
         <f>SQRT(AH20^2+(16*K20/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y20)^2)</f>
-        <v>5.0007214701646381E-2</v>
+        <v>4.8149818079246579E-2</v>
       </c>
       <c r="AJ20" s="3">
         <v>0</v>
       </c>
       <c r="AK20" s="22">
         <f t="shared" si="19"/>
-        <v>5.1047229921540947E-2</v>
+        <v>4.721250778291447E-2</v>
       </c>
       <c r="AL20" s="22">
         <f t="shared" si="20"/>
-        <v>2.1044053119980899E-3</v>
+        <v>2.0262422840833043E-3</v>
       </c>
       <c r="AM20" s="28">
         <f t="shared" si="21"/>
-        <v>3.3433822934822006E-3</v>
+        <v>3.0922238639569622E-3</v>
       </c>
       <c r="AN20" s="7">
         <f t="shared" si="22"/>
         <v>2.4312123000000003</v>
       </c>
-      <c r="AO20" s="37">
+      <c r="AO20" s="34">
         <f t="shared" si="23"/>
         <v>40.916592886771006</v>
       </c>
-      <c r="AP20" s="40">
+      <c r="AP20" s="36">
         <f t="shared" si="24"/>
-        <v>1.1995299740668006</v>
-      </c>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+        <v>1.1132806567892997</v>
+      </c>
+      <c r="AR20" s="33">
+        <f t="shared" si="25"/>
+        <v>11.083407113228994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -7470,15 +7495,15 @@
         <v>0.38723874567745109</v>
       </c>
       <c r="W21" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X21" s="15">
         <f t="shared" si="13"/>
-        <v>0.43583694904613773</v>
+        <v>0.38736784346902831</v>
       </c>
       <c r="Y21" s="21">
         <f t="shared" si="14"/>
-        <v>1.0814476426082482E-4</v>
+        <v>9.6118064808102085E-5</v>
       </c>
       <c r="Z21" s="15">
         <v>0</v>
@@ -7501,7 +7526,7 @@
         <v>0.01</v>
       </c>
       <c r="AF21" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG21" s="15">
@@ -7514,37 +7539,41 @@
       </c>
       <c r="AI21" s="15">
         <f t="shared" si="2"/>
-        <v>4.4699343234926324E-2</v>
+        <v>4.2881004764032275E-2</v>
       </c>
       <c r="AJ21" s="3">
         <v>0</v>
       </c>
       <c r="AK21" s="22">
         <f t="shared" si="19"/>
-        <v>4.0486551696663868E-2</v>
+        <v>3.5984072150279725E-2</v>
       </c>
       <c r="AL21" s="22">
         <f t="shared" si="20"/>
-        <v>1.8810392841836869E-3</v>
+        <v>1.8045199027306353E-3</v>
       </c>
       <c r="AM21" s="28">
         <f t="shared" si="21"/>
-        <v>2.6517015766541635E-3</v>
+        <v>2.3568078005318624E-3</v>
       </c>
       <c r="AN21" s="7">
         <f t="shared" si="22"/>
         <v>2.4312123000000003</v>
       </c>
-      <c r="AO21" s="37">
+      <c r="AO21" s="34">
         <f t="shared" si="23"/>
         <v>42.673982331632686</v>
       </c>
-      <c r="AP21" s="40">
+      <c r="AP21" s="36">
         <f t="shared" si="24"/>
-        <v>1.0176801122282624</v>
-      </c>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+        <v>0.91106770894828593</v>
+      </c>
+      <c r="AR21" s="33">
+        <f t="shared" si="25"/>
+        <v>28.326017668367314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -7625,15 +7654,15 @@
         <v>0.18644828495581278</v>
       </c>
       <c r="W22" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X22" s="15">
         <f t="shared" si="13"/>
-        <v>0.27342816783017065</v>
+        <v>0.1867162632524654</v>
       </c>
       <c r="Y22" s="21">
         <f t="shared" si="14"/>
-        <v>2.5494707915661208E-5</v>
+        <v>1.7409605720219627E-5</v>
       </c>
       <c r="Z22" s="15">
         <v>0</v>
@@ -7656,7 +7685,7 @@
         <v>0.01</v>
       </c>
       <c r="AF22" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG22" s="15">
@@ -7669,37 +7698,41 @@
       </c>
       <c r="AI22" s="15">
         <f t="shared" si="2"/>
-        <v>3.543602740374957E-2</v>
+        <v>3.531659701453306E-2</v>
       </c>
       <c r="AJ22" s="3">
         <v>0</v>
       </c>
       <c r="AK22" s="22">
         <f t="shared" si="19"/>
-        <v>9.5445472286509216E-3</v>
+        <v>6.5176978915986112E-3</v>
       </c>
       <c r="AL22" s="22">
         <f t="shared" si="20"/>
-        <v>1.491220111927277E-3</v>
+        <v>1.4861942382212385E-3</v>
       </c>
       <c r="AM22" s="29">
         <f t="shared" si="21"/>
-        <v>6.251283419810062E-4</v>
+        <v>4.2688223745989437E-4</v>
       </c>
       <c r="AN22" s="7">
         <f t="shared" si="22"/>
         <v>2.1365199000000001</v>
       </c>
-      <c r="AO22" s="37">
+      <c r="AO22" s="34">
         <f t="shared" si="23"/>
         <v>49.917307149111032</v>
       </c>
       <c r="AP22" s="8">
         <f t="shared" si="24"/>
-        <v>0.46801903534724748</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+        <v>0.34186738818208934</v>
+      </c>
+      <c r="AR22" s="33">
+        <f t="shared" si="25"/>
+        <v>23.082692850888968</v>
+      </c>
+    </row>
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>63</v>
       </c>
@@ -7810,7 +7843,7 @@
         <v>0.01</v>
       </c>
       <c r="AF23" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG23" s="15">
@@ -7851,8 +7884,9 @@
       <c r="AP23" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AR23" s="33"/>
+    </row>
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -7933,15 +7967,15 @@
         <v>0.25211244269310562</v>
       </c>
       <c r="W24" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X24" s="15">
         <f t="shared" si="13"/>
-        <v>0.321808458186985</v>
+        <v>0.25231068895448022</v>
       </c>
       <c r="Y24" s="21">
         <f t="shared" si="14"/>
-        <v>1.4839817445275611E-4</v>
+        <v>1.1635009796419436E-4</v>
       </c>
       <c r="Z24" s="15">
         <v>0</v>
@@ -7964,7 +7998,7 @@
         <v>0.01</v>
       </c>
       <c r="AF24" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG24" s="15">
@@ -7977,37 +8011,41 @@
       </c>
       <c r="AI24" s="15">
         <f>SQRT(AH24^2+(16*K24/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y24)^2)</f>
-        <v>6.2393678094612104E-2</v>
+        <v>5.3579698390235887E-2</v>
       </c>
       <c r="AJ24" s="3">
         <v>0</v>
       </c>
       <c r="AK24" s="22">
         <f t="shared" si="19"/>
-        <v>5.5556368380271962E-2</v>
+        <v>4.3558412543931807E-2</v>
       </c>
       <c r="AL24" s="22">
         <f t="shared" si="20"/>
-        <v>1.4769297485459881E-3</v>
+        <v>1.2682927643833583E-3</v>
       </c>
       <c r="AM24" s="28">
         <f t="shared" si="21"/>
-        <v>2.729034150603259E-3</v>
+        <v>2.1396718116057922E-3</v>
       </c>
       <c r="AN24" s="7">
         <f t="shared" si="22"/>
         <v>3.9046742999999999</v>
       </c>
-      <c r="AO24" s="37">
+      <c r="AO24" s="34">
         <f t="shared" si="23"/>
         <v>41.834907330788297</v>
       </c>
-      <c r="AP24" s="40">
+      <c r="AP24" s="36">
         <f t="shared" si="24"/>
-        <v>0.99581938066018949</v>
-      </c>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+        <v>0.78641419283448344</v>
+      </c>
+      <c r="AR24" s="33">
+        <f t="shared" si="25"/>
+        <v>16.165092669211703</v>
+      </c>
+    </row>
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -8088,15 +8126,15 @@
         <v>1.0195057737904283</v>
       </c>
       <c r="W25" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X25" s="15">
         <f t="shared" si="13"/>
-        <v>1.0389379301921842</v>
+        <v>1.0195548159819656</v>
       </c>
       <c r="Y25" s="21">
         <f t="shared" si="14"/>
-        <v>4.4507639011784382E-4</v>
+        <v>4.3677275016860246E-4</v>
       </c>
       <c r="Z25" s="15">
         <v>0</v>
@@ -8119,7 +8157,7 @@
         <v>0.01</v>
       </c>
       <c r="AF25" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG25" s="15">
@@ -8132,37 +8170,41 @@
       </c>
       <c r="AI25" s="14">
         <f>SQRT(AH25^2+(16*K25/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y25)^2)</f>
-        <v>0.15300495970901143</v>
+        <v>0.15030294209246406</v>
       </c>
       <c r="AJ25" s="3">
         <v>0</v>
       </c>
       <c r="AK25" s="7">
         <f t="shared" si="19"/>
-        <v>0.16662487916669469</v>
+        <v>0.16351621504991298</v>
       </c>
       <c r="AL25" s="22">
         <f t="shared" si="20"/>
-        <v>3.6218024577210038E-3</v>
+        <v>3.5578426092100256E-3</v>
       </c>
       <c r="AM25" s="28">
         <f t="shared" si="21"/>
-        <v>8.1849299881077871E-3</v>
+        <v>8.0322265126145133E-3</v>
       </c>
       <c r="AN25" s="7">
         <f t="shared" si="22"/>
         <v>3.9046742999999999</v>
       </c>
-      <c r="AO25" s="37">
+      <c r="AO25" s="34">
         <f t="shared" si="23"/>
         <v>46.567659646009965</v>
       </c>
-      <c r="AP25" s="40">
+      <c r="AP25" s="36">
         <f t="shared" si="24"/>
-        <v>3.3815067251001993</v>
-      </c>
-    </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+        <v>3.3185380503967217</v>
+      </c>
+      <c r="AR25" s="33">
+        <f t="shared" si="25"/>
+        <v>5.4323403539900355</v>
+      </c>
+    </row>
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -8243,15 +8285,15 @@
         <v>7.4524131352512762E-2</v>
       </c>
       <c r="W26" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X26" s="15">
         <f t="shared" si="13"/>
-        <v>0.21343347008809696</v>
+        <v>7.5192061774143254E-2</v>
       </c>
       <c r="Y26" s="21">
         <f t="shared" si="14"/>
-        <v>1.414118776310194E-5</v>
+        <v>4.9819040256620911E-6</v>
       </c>
       <c r="Z26" s="15">
         <v>0</v>
@@ -8274,7 +8316,7 @@
         <v>0.01</v>
       </c>
       <c r="AF26" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG26" s="15">
@@ -8287,37 +8329,41 @@
       </c>
       <c r="AI26" s="15">
         <f t="shared" si="2"/>
-        <v>3.526102967236603E-2</v>
+        <v>3.5218011977338856E-2</v>
       </c>
       <c r="AJ26" s="3">
         <v>0</v>
       </c>
       <c r="AK26" s="10">
         <f t="shared" si="19"/>
-        <v>5.2940882837584947E-3</v>
+        <v>1.8650936664517882E-3</v>
       </c>
       <c r="AL26" s="22">
         <f t="shared" si="20"/>
-        <v>8.3466891643269373E-4</v>
+        <v>8.3365063837248423E-4</v>
       </c>
       <c r="AM26" s="29">
         <f t="shared" si="21"/>
-        <v>2.6005565417439914E-4</v>
+        <v>9.1616937143576809E-5</v>
       </c>
       <c r="AN26" s="7">
         <f t="shared" si="22"/>
         <v>2.9469240000000001</v>
       </c>
-      <c r="AO26" s="37">
+      <c r="AO26" s="34">
         <f t="shared" si="23"/>
         <v>44.898280449625048</v>
       </c>
       <c r="AP26" s="8">
         <f t="shared" si="24"/>
-        <v>0.26971969939369633</v>
-      </c>
-    </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+        <v>0.11877930424820046</v>
+      </c>
+      <c r="AR26" s="33">
+        <f t="shared" si="25"/>
+        <v>26.101719550374952</v>
+      </c>
+    </row>
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>63</v>
       </c>
@@ -8428,7 +8474,7 @@
         <v>0.01</v>
       </c>
       <c r="AF27" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG27" s="15">
@@ -8466,11 +8512,12 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AP27" s="39" t="s">
+      <c r="AP27" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AR27" s="33"/>
+    </row>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
@@ -8529,7 +8576,7 @@
         <v>1.4974946581424107</v>
       </c>
       <c r="R28" s="22">
-        <f t="shared" ref="R28:R41" si="26">O28*9.81/P28^2</f>
+        <f t="shared" ref="R28:R41" si="27">O28*9.81/P28^2</f>
         <v>0.24428620768088338</v>
       </c>
       <c r="S28" s="25">
@@ -8580,7 +8627,7 @@
         <v>0.01</v>
       </c>
       <c r="AF28" s="15">
-        <f t="shared" ref="AF28:AF41" si="27">L28*AD28</f>
+        <f t="shared" ref="AF28:AF41" si="28">L28*AD28</f>
         <v>0</v>
       </c>
       <c r="AG28" s="15">
@@ -8591,7 +8638,7 @@
         <v>0</v>
       </c>
       <c r="AI28" s="15">
-        <f t="shared" ref="AI28:AI41" si="28">SQRT(AF28^2+(16*K28/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y28)^2)</f>
+        <f t="shared" ref="AI28:AI41" si="29">SQRT(AF28^2+(16*K28/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y28)^2)</f>
         <v>0</v>
       </c>
       <c r="AJ28" s="3">
@@ -8613,7 +8660,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>63</v>
       </c>
@@ -8672,7 +8719,7 @@
         <v>1.2354330929674888</v>
       </c>
       <c r="R29" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.39199414720885933</v>
       </c>
       <c r="S29" s="25">
@@ -8723,7 +8770,7 @@
         <v>0.01</v>
       </c>
       <c r="AF29" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG29" s="15">
@@ -8734,7 +8781,7 @@
         <v>0</v>
       </c>
       <c r="AI29" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ29" s="3">
@@ -8756,7 +8803,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>63</v>
       </c>
@@ -8815,7 +8862,7 @@
         <v>0.97337152779256686</v>
       </c>
       <c r="R30" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.46963550003766724</v>
       </c>
       <c r="S30" s="25">
@@ -8866,7 +8913,7 @@
         <v>0.01</v>
       </c>
       <c r="AF30" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG30" s="15">
@@ -8877,7 +8924,7 @@
         <v>0</v>
       </c>
       <c r="AI30" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ30" s="3">
@@ -8899,7 +8946,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -8958,7 +9005,7 @@
         <v>0.74874732907120534</v>
       </c>
       <c r="R31" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.51129671375068619</v>
       </c>
       <c r="S31" s="25">
@@ -9009,7 +9056,7 @@
         <v>0.01</v>
       </c>
       <c r="AF31" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG31" s="15">
@@ -9020,7 +9067,7 @@
         <v>0</v>
       </c>
       <c r="AI31" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ31" s="3">
@@ -9042,7 +9089,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -9101,7 +9148,7 @@
         <v>2.2462419872136161</v>
       </c>
       <c r="R32" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.24281333648900894</v>
       </c>
       <c r="S32" s="25">
@@ -9152,7 +9199,7 @@
         <v>0.01</v>
       </c>
       <c r="AF32" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG32" s="15">
@@ -9163,7 +9210,7 @@
         <v>0</v>
       </c>
       <c r="AI32" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ32" s="3">
@@ -9244,7 +9291,7 @@
         <v>1.8718683226780133</v>
       </c>
       <c r="R33" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.3837881505684162</v>
       </c>
       <c r="S33" s="25">
@@ -9295,7 +9342,7 @@
         <v>0.01</v>
       </c>
       <c r="AF33" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG33" s="15">
@@ -9306,7 +9353,7 @@
         <v>0</v>
       </c>
       <c r="AI33" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ33" s="3">
@@ -9387,7 +9434,7 @@
         <v>1.4974946581424107</v>
       </c>
       <c r="R34" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.46290237458909855</v>
       </c>
       <c r="S34" s="25">
@@ -9438,7 +9485,7 @@
         <v>0.01</v>
       </c>
       <c r="AF34" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG34" s="15">
@@ -9449,7 +9496,7 @@
         <v>0</v>
       </c>
       <c r="AI34" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ34" s="3">
@@ -9530,7 +9577,7 @@
         <v>1.1231209936068081</v>
       </c>
       <c r="R35" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.50919261204800836</v>
       </c>
       <c r="S35" s="25">
@@ -9581,7 +9628,7 @@
         <v>0.01</v>
       </c>
       <c r="AF35" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG35" s="15">
@@ -9592,7 +9639,7 @@
         <v>0</v>
       </c>
       <c r="AI35" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ35" s="3">
@@ -9673,7 +9720,7 @@
         <v>0.74874732907120534</v>
       </c>
       <c r="R36" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.53865003588549654</v>
       </c>
       <c r="S36" s="25">
@@ -9724,7 +9771,7 @@
         <v>0.01</v>
       </c>
       <c r="AF36" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG36" s="15">
@@ -9735,7 +9782,7 @@
         <v>0</v>
       </c>
       <c r="AI36" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ36" s="3">
@@ -9816,7 +9863,7 @@
         <v>2.9949893162848213</v>
       </c>
       <c r="R37" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.2438127847977809</v>
       </c>
       <c r="S37" s="25">
@@ -9867,7 +9914,7 @@
         <v>0.01</v>
       </c>
       <c r="AF37" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG37" s="15">
@@ -9878,7 +9925,7 @@
         <v>0</v>
       </c>
       <c r="AI37" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ37" s="3">
@@ -9959,7 +10006,7 @@
         <v>2.5083035523885377</v>
       </c>
       <c r="R38" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.38110542089750221</v>
       </c>
       <c r="S38" s="25">
@@ -10010,7 +10057,7 @@
         <v>0.01</v>
       </c>
       <c r="AF38" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG38" s="15">
@@ -10021,7 +10068,7 @@
         <v>0</v>
       </c>
       <c r="AI38" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ38" s="3">
@@ -10102,7 +10149,7 @@
         <v>2.0216177884922546</v>
       </c>
       <c r="R39" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.45448596777838768</v>
       </c>
       <c r="S39" s="25">
@@ -10153,7 +10200,7 @@
         <v>0.01</v>
       </c>
       <c r="AF39" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG39" s="15">
@@ -10164,7 +10211,7 @@
         <v>0</v>
       </c>
       <c r="AI39" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ39" s="3">
@@ -10245,7 +10292,7 @@
         <v>1.4974946581424107</v>
       </c>
       <c r="R40" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.51129671375068619</v>
       </c>
       <c r="S40" s="25">
@@ -10296,7 +10343,7 @@
         <v>0.01</v>
       </c>
       <c r="AF40" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG40" s="15">
@@ -10307,7 +10354,7 @@
         <v>0</v>
       </c>
       <c r="AI40" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ40" s="3">
@@ -10325,7 +10372,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AO40" s="38">
+      <c r="AO40" s="35">
         <v>69</v>
       </c>
     </row>
@@ -10388,7 +10435,7 @@
         <v>1.0108088942461273</v>
       </c>
       <c r="R41" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.5397020867368354</v>
       </c>
       <c r="S41" s="25">
@@ -10439,7 +10486,7 @@
         <v>0.01</v>
       </c>
       <c r="AF41" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG41" s="15">
@@ -10450,7 +10497,7 @@
         <v>0</v>
       </c>
       <c r="AI41" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AJ41" s="3">
@@ -10521,23 +10568,23 @@
         <v>9.8417294323611557</v>
       </c>
       <c r="O42" s="8">
-        <f t="shared" ref="O42:O49" si="29">N42+8*K42^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
+        <f t="shared" ref="O42:O49" si="30">N42+8*K42^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
         <v>11.256986832203168</v>
       </c>
       <c r="P42" s="8">
-        <f t="shared" ref="P42:P44" si="30">$B$7/2*2*PI()/60*C42</f>
+        <f t="shared" ref="P42:P44" si="31">$B$7/2*2*PI()/60*C42</f>
         <v>15.268140296446393</v>
       </c>
       <c r="Q42" s="8">
-        <f t="shared" ref="Q42:Q45" si="31">K42/($B$8*(2*PI()*$B$7/2-$B$10*$B$9))</f>
+        <f t="shared" ref="Q42:Q45" si="32">K42/($B$8*(2*PI()*$B$7/2-$B$10*$B$9))</f>
         <v>2.7202780690215822</v>
       </c>
       <c r="R42" s="22">
-        <f t="shared" ref="R42:R45" si="32">O42*9.81/P42^2</f>
+        <f t="shared" ref="R42:R45" si="33">O42*9.81/P42^2</f>
         <v>0.47371690321318732</v>
       </c>
       <c r="S42" s="25">
-        <f t="shared" ref="S42:S45" si="33">Q42/P42</f>
+        <f t="shared" ref="S42:S45" si="34">Q42/P42</f>
         <v>0.17816695525483989</v>
       </c>
       <c r="T42" s="19">
@@ -10553,15 +10600,15 @@
         <v>0.64252307152031252</v>
       </c>
       <c r="W42" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X42" s="15">
         <f>SQRT(V42^2+W42^2)</f>
-        <v>0.67293082663517256</v>
+        <v>0.64260088502576518</v>
       </c>
       <c r="Y42" s="21">
         <f t="shared" si="14"/>
-        <v>3.9085990631924716E-4</v>
+        <v>3.7324329898473399E-4</v>
       </c>
       <c r="Z42" s="15">
         <v>0</v>
@@ -10584,11 +10631,11 @@
         <v>0.01</v>
       </c>
       <c r="AF42" s="15">
-        <f t="shared" ref="AF42:AG42" si="34">L42*AD42/D42</f>
+        <f t="shared" ref="AF42:AG42" si="35">L42*AD42/D42</f>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG42" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AH42" s="15">
@@ -10597,22 +10644,22 @@
       </c>
       <c r="AI42" s="14">
         <f>SQRT(AH42^2+(16*K42/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y42)^2)</f>
-        <v>0.15427984182058216</v>
+        <v>0.14751149877945924</v>
       </c>
       <c r="AJ42" s="3">
         <v>0</v>
       </c>
       <c r="AK42" s="7">
         <f t="shared" si="19"/>
-        <v>0.14632765544877893</v>
+        <v>0.13973246160427244</v>
       </c>
       <c r="AL42" s="22">
         <f t="shared" si="20"/>
-        <v>6.4924095572707263E-3</v>
+        <v>6.2075839149280535E-3</v>
       </c>
       <c r="AM42" s="19">
         <f t="shared" si="21"/>
-        <v>9.5838558336299937E-3</v>
+        <v>9.1518979319828945E-3</v>
       </c>
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.25">
@@ -10664,23 +10711,23 @@
         <v>10.633997454644252</v>
       </c>
       <c r="O43" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>11.692307952536082</v>
       </c>
       <c r="P43" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q43" s="8">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2.352351058303686</v>
       </c>
       <c r="R43" s="22">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.49203610142326842</v>
       </c>
       <c r="S43" s="25">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.1540692587722152</v>
       </c>
       <c r="T43" s="19">
@@ -10696,15 +10743,15 @@
         <v>0.10039523036082122</v>
       </c>
       <c r="W43" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X43" s="15">
         <f t="shared" si="13"/>
-        <v>0.22378382935145777</v>
+        <v>0.10089203278357692</v>
       </c>
       <c r="Y43" s="21">
         <f t="shared" si="14"/>
-        <v>9.7197942311166743E-5</v>
+        <v>4.3821298485124759E-5</v>
       </c>
       <c r="Z43" s="15">
         <v>0</v>
@@ -10727,35 +10774,35 @@
         <v>0.01</v>
       </c>
       <c r="AF43" s="15">
-        <f t="shared" ref="AF43:AF49" si="35">L43*AD43/D43</f>
+        <f t="shared" ref="AF43:AF49" si="36">L43*AD43/D43</f>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG43" s="15">
-        <f t="shared" ref="AG43:AG49" si="36">M43*AE43/E43</f>
+        <f t="shared" ref="AG43:AG49" si="37">M43*AE43/E43</f>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AH43" s="15">
-        <f t="shared" ref="AH43:AH45" si="37">SQRT((AF43/2)^2+(AG43/2)^2)</f>
+        <f t="shared" ref="AH43:AH45" si="38">SQRT((AF43/2)^2+(AG43/2)^2)</f>
         <v>2.4898581825494825E-2</v>
       </c>
       <c r="AI43" s="15">
-        <f t="shared" ref="AI43:AI49" si="38">SQRT(AH43^2+(16*K43/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y43)^2)</f>
-        <v>4.1133546763215144E-2</v>
+        <f t="shared" ref="AI43:AI49" si="39">SQRT(AH43^2+(16*K43/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^(4))*Y43)^2)</f>
+        <v>2.8945505162947846E-2</v>
       </c>
       <c r="AJ43" s="3">
         <v>0</v>
       </c>
       <c r="AK43" s="22">
         <f t="shared" si="19"/>
-        <v>3.6388349848351598E-2</v>
+        <v>1.6405540098584609E-2</v>
       </c>
       <c r="AL43" s="22">
         <f t="shared" si="20"/>
-        <v>1.7309833156330925E-3</v>
+        <v>1.2180857339645064E-3</v>
       </c>
       <c r="AM43" s="19">
         <f t="shared" si="21"/>
-        <v>2.3832863165935709E-3</v>
+        <v>1.0744949797456957E-3</v>
       </c>
     </row>
     <row r="44" spans="1:41" x14ac:dyDescent="0.25">
@@ -10791,7 +10838,7 @@
         <v>41.01</v>
       </c>
       <c r="K44" s="9">
-        <f t="shared" ref="K44:K48" si="39">$D$3/$B$2/J44</f>
+        <f t="shared" ref="K44:K48" si="40">$D$3/$B$2/J44</f>
         <v>2.2165398829846967E-3</v>
       </c>
       <c r="L44" s="8">
@@ -10807,19 +10854,19 @@
         <v>12.41219901576854</v>
       </c>
       <c r="O44" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12.543894388300366</v>
       </c>
       <c r="P44" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q44" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.82981415858229679</v>
       </c>
       <c r="R44" s="22">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.52787259081264604</v>
       </c>
       <c r="S44" s="25">
@@ -10839,15 +10886,15 @@
         <v>8.6053054594982345E-2</v>
       </c>
       <c r="W44" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X44" s="15">
         <f t="shared" si="13"/>
-        <v>0.21772718756537277</v>
+        <v>8.6632143025132488E-2</v>
       </c>
       <c r="Y44" s="21">
         <f t="shared" si="14"/>
-        <v>1.1767885755882431E-5</v>
+        <v>4.682360403892726E-6</v>
       </c>
       <c r="Z44" s="15">
         <v>0</v>
@@ -10870,35 +10917,35 @@
         <v>0.01</v>
       </c>
       <c r="AF44" s="15">
-        <f t="shared" si="35"/>
-        <v>3.5211912101471038E-2</v>
-      </c>
-      <c r="AG44" s="15">
         <f t="shared" si="36"/>
         <v>3.5211912101471038E-2</v>
       </c>
+      <c r="AG44" s="15">
+        <f t="shared" si="37"/>
+        <v>3.5211912101471038E-2</v>
+      </c>
       <c r="AH44" s="15">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>2.4898581825494828E-2</v>
       </c>
       <c r="AI44" s="15">
-        <f t="shared" si="38"/>
-        <v>2.4937819217776595E-2</v>
+        <f t="shared" si="39"/>
+        <v>2.4904797965426013E-2</v>
       </c>
       <c r="AJ44" s="3">
         <v>0</v>
       </c>
       <c r="AK44" s="10">
         <f t="shared" si="19"/>
-        <v>4.405586514266026E-3</v>
+        <v>1.7529524230817245E-3</v>
       </c>
       <c r="AL44" s="22">
         <f t="shared" si="20"/>
-        <v>1.0494341575438583E-3</v>
+        <v>1.0480445560779501E-3</v>
       </c>
       <c r="AM44" s="20">
         <f t="shared" si="21"/>
-        <v>2.885476835244572E-4</v>
+        <v>1.1481112886352755E-4</v>
       </c>
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.25">
@@ -10949,7 +10996,7 @@
         <v>12.500228796022217</v>
       </c>
       <c r="O45" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>12.500228796022217</v>
       </c>
       <c r="P45" s="8">
@@ -10957,15 +11004,15 @@
         <v>15.268140296446393</v>
       </c>
       <c r="Q45" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R45" s="22">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.52603505387142835</v>
       </c>
       <c r="S45" s="25">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="T45" s="19">
@@ -11012,19 +11059,19 @@
         <v>0.01</v>
       </c>
       <c r="AF45" s="15">
-        <f t="shared" si="35"/>
-        <v>3.5211912101471038E-2</v>
-      </c>
-      <c r="AG45" s="15">
         <f t="shared" si="36"/>
         <v>3.5211912101471038E-2</v>
       </c>
+      <c r="AG45" s="15">
+        <f t="shared" si="37"/>
+        <v>3.5211912101471038E-2</v>
+      </c>
       <c r="AH45" s="15">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>2.4898581825494828E-2</v>
       </c>
       <c r="AI45" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>2.4898581825494828E-2</v>
       </c>
       <c r="AJ45" s="3">
@@ -11076,15 +11123,15 @@
         <v>16.28</v>
       </c>
       <c r="K46" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>5.5835565479854053E-3</v>
       </c>
       <c r="L46" s="7">
-        <f t="shared" ref="L46:L49" si="40">5*D46/($B$2*9.81)*6894.76</f>
+        <f t="shared" ref="L46:L49" si="41">5*D46/($B$2*9.81)*6894.76</f>
         <v>2.3944100229000305</v>
       </c>
       <c r="M46" s="7">
-        <f t="shared" ref="M46:M49" si="41">5*E46/($B$2*9.81)*6894.76</f>
+        <f t="shared" ref="M46:M49" si="42">5*E46/($B$2*9.81)*6894.76</f>
         <v>5.9156012330471341</v>
       </c>
       <c r="N46" s="7">
@@ -11092,11 +11139,11 @@
         <v>8.3100112559471651</v>
       </c>
       <c r="O46" s="7">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>9.1456936498984369</v>
       </c>
       <c r="P46" s="8">
-        <f t="shared" ref="P46:P49" si="42">$B$7/2*2*PI()/60*C46</f>
+        <f t="shared" ref="P46:P49" si="43">$B$7/2*2*PI()/60*C46</f>
         <v>15.268140296446393</v>
       </c>
       <c r="Q46" s="7">
@@ -11104,11 +11151,11 @@
         <v>2.0903365260110558</v>
       </c>
       <c r="R46" s="22">
-        <f t="shared" ref="R46:R49" si="43">O46*9.81/P46^2</f>
+        <f t="shared" ref="R46:R49" si="44">O46*9.81/P46^2</f>
         <v>0.38486939161840239</v>
       </c>
       <c r="S46" s="25">
-        <f t="shared" ref="S46:S49" si="44">Q46/P46</f>
+        <f t="shared" ref="S46:S49" si="45">Q46/P46</f>
         <v>0.13690839129226329</v>
       </c>
       <c r="T46" s="19">
@@ -11124,15 +11171,15 @@
         <v>0.7937587740951213</v>
       </c>
       <c r="W46" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X46" s="15">
         <f t="shared" si="13"/>
-        <v>0.81856764622906386</v>
+        <v>0.7938217630255483</v>
       </c>
       <c r="Y46" s="21">
         <f t="shared" si="14"/>
-        <v>2.8074439441469842E-4</v>
+        <v>2.7225729133136477E-4</v>
       </c>
       <c r="Z46" s="15">
         <v>0</v>
@@ -11147,19 +11194,19 @@
         <v>0.01</v>
       </c>
       <c r="AD46" s="3">
-        <f t="shared" ref="AD46:AD49" si="45">SQRT(Z46^2+AB46^2)</f>
+        <f t="shared" ref="AD46:AD49" si="46">SQRT(Z46^2+AB46^2)</f>
         <v>0.01</v>
       </c>
       <c r="AE46" s="3">
-        <f t="shared" ref="AE46:AE49" si="46">SQRT(AA46^2+AC46^2)</f>
+        <f t="shared" ref="AE46:AE49" si="47">SQRT(AA46^2+AC46^2)</f>
         <v>0.01</v>
       </c>
       <c r="AF46" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG46" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AH46" s="15">
@@ -11167,23 +11214,23 @@
         <v>4.979716365098965E-2</v>
       </c>
       <c r="AI46" s="14">
-        <f t="shared" si="38"/>
-        <v>9.7683179625164276E-2</v>
+        <f t="shared" si="39"/>
+        <v>9.5506357265650266E-2</v>
       </c>
       <c r="AJ46" s="3">
         <v>0</v>
       </c>
       <c r="AK46" s="7">
         <f t="shared" si="19"/>
-        <v>0.10510330773485922</v>
+        <v>0.1019259598522602</v>
       </c>
       <c r="AL46" s="22">
         <f t="shared" si="20"/>
-        <v>4.1107068914456356E-3</v>
+        <v>4.0191017787840283E-3</v>
       </c>
       <c r="AM46" s="19">
         <f t="shared" si="21"/>
-        <v>6.8838316713215981E-3</v>
+        <v>6.6757285349272758E-3</v>
       </c>
     </row>
     <row r="47" spans="1:41" x14ac:dyDescent="0.25">
@@ -11219,39 +11266,39 @@
         <v>16.683333333333334</v>
       </c>
       <c r="K47" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>5.4485694666055393E-3</v>
       </c>
       <c r="L47" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3.1690720891323929</v>
       </c>
       <c r="M47" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>6.4789918266706712</v>
       </c>
       <c r="N47" s="7">
-        <f t="shared" ref="N47:N49" si="47">L47+M47</f>
+        <f t="shared" ref="N47:N49" si="48">L47+M47</f>
         <v>9.6480639158030641</v>
       </c>
       <c r="O47" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>10.443828120193732</v>
       </c>
       <c r="P47" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q47" s="7">
-        <f t="shared" ref="Q47:Q49" si="48">K47/($B$8*(2*PI()*$B$7/2-$B$10*$B$9))</f>
+        <f t="shared" ref="Q47:Q49" si="49">K47/($B$8*(2*PI()*$B$7/2-$B$10*$B$9))</f>
         <v>2.0398009176899095</v>
       </c>
       <c r="R47" s="22">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.43949753060346181</v>
       </c>
       <c r="S47" s="25">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.13359851809618661</v>
       </c>
       <c r="T47" s="19">
@@ -11267,15 +11314,15 @@
         <v>0.23081547494868154</v>
       </c>
       <c r="W47" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X47" s="15">
         <f t="shared" si="13"/>
-        <v>0.3054108437429579</v>
+        <v>0.23103199664935037</v>
       </c>
       <c r="Y47" s="21">
         <f t="shared" si="14"/>
-        <v>9.9743388490796157E-5</v>
+        <v>7.5452180784369458E-5</v>
       </c>
       <c r="Z47" s="15">
         <v>0</v>
@@ -11290,43 +11337,43 @@
         <v>0.01</v>
       </c>
       <c r="AD47" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.01</v>
       </c>
       <c r="AE47" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.01</v>
       </c>
       <c r="AF47" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AG47" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AH47" s="15">
-        <f t="shared" ref="AH47:AH49" si="49">SQRT(AF47^2+AG47^2)</f>
+        <f t="shared" ref="AH47:AH49" si="50">SQRT(AF47^2+AG47^2)</f>
         <v>4.979716365098965E-2</v>
       </c>
       <c r="AI47" s="15">
-        <f t="shared" si="38"/>
-        <v>5.7694103995025177E-2</v>
+        <f t="shared" si="39"/>
+        <v>5.4456417954920247E-2</v>
       </c>
       <c r="AJ47" s="3">
         <v>0</v>
       </c>
       <c r="AK47" s="22">
         <f t="shared" si="19"/>
-        <v>3.7341297862497604E-2</v>
+        <v>2.8247309417447172E-2</v>
       </c>
       <c r="AL47" s="22">
         <f t="shared" si="20"/>
-        <v>2.4278852490079591E-3</v>
+        <v>2.2916368348135457E-3</v>
       </c>
       <c r="AM47" s="19">
         <f t="shared" si="21"/>
-        <v>2.4457004676063047E-3</v>
+        <v>1.8500818612481335E-3</v>
       </c>
     </row>
     <row r="48" spans="1:41" x14ac:dyDescent="0.25">
@@ -11362,39 +11409,39 @@
         <v>30.473333333333333</v>
       </c>
       <c r="K48" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>2.9829457646423892E-3</v>
       </c>
       <c r="L48" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>10.17624259732513</v>
       </c>
       <c r="M48" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>11.479083345079555</v>
       </c>
       <c r="N48" s="8">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>21.655325942404687</v>
       </c>
       <c r="O48" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>21.893837884806008</v>
       </c>
       <c r="P48" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q48" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1.1167363370201266</v>
       </c>
       <c r="R48" s="22">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.92133723143140611</v>
       </c>
       <c r="S48" s="25">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>7.3141608299213956E-2</v>
       </c>
       <c r="T48" s="19">
@@ -11410,15 +11457,15 @@
         <v>0.55565520473825125</v>
       </c>
       <c r="W48" s="3">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="X48" s="15">
         <f t="shared" si="13"/>
-        <v>0.59055288209669077</v>
+        <v>0.55574518131307982</v>
       </c>
       <c r="Y48" s="21">
         <f t="shared" si="14"/>
-        <v>5.7807500058444974E-5</v>
+        <v>5.440027569957126E-5</v>
       </c>
       <c r="Z48" s="15">
         <v>0</v>
@@ -11433,43 +11480,43 @@
         <v>0.01</v>
       </c>
       <c r="AD48" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.01</v>
       </c>
       <c r="AE48" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.01</v>
       </c>
       <c r="AF48" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3.5211912101471038E-2</v>
       </c>
       <c r="AG48" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>3.5211912101471031E-2</v>
       </c>
       <c r="AH48" s="15">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>4.979716365098965E-2</v>
       </c>
       <c r="AI48" s="15">
-        <f t="shared" si="38"/>
-        <v>5.0647966676196698E-2</v>
+        <f t="shared" si="39"/>
+        <v>5.0551353663437527E-2</v>
       </c>
       <c r="AJ48" s="3">
         <v>0</v>
       </c>
       <c r="AK48" s="22">
         <f t="shared" si="19"/>
-        <v>2.1641605634522113E-2</v>
+        <v>2.0366030565395588E-2</v>
       </c>
       <c r="AL48" s="22">
         <f t="shared" si="20"/>
-        <v>2.1313694584109985E-3</v>
+        <v>2.1273037863180507E-3</v>
       </c>
       <c r="AM48" s="19">
         <f t="shared" si="21"/>
-        <v>1.4174356021315262E-3</v>
+        <v>1.3338907142565167E-3</v>
       </c>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
@@ -11508,35 +11555,35 @@
         <v>0</v>
       </c>
       <c r="L49" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>12.394593059717804</v>
       </c>
       <c r="M49" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>12.500228796022217</v>
       </c>
       <c r="N49" s="8">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>24.89482185574002</v>
       </c>
       <c r="O49" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>24.89482185574002</v>
       </c>
       <c r="P49" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>15.268140296446393</v>
       </c>
       <c r="Q49" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="R49" s="22">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>1.0476247410904223</v>
       </c>
       <c r="S49" s="25">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="T49" s="19">
@@ -11575,27 +11622,27 @@
         <v>0.01</v>
       </c>
       <c r="AD49" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>0.01</v>
       </c>
       <c r="AE49" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.01</v>
       </c>
       <c r="AF49" s="15">
-        <f t="shared" si="35"/>
-        <v>3.5211912101471038E-2</v>
-      </c>
-      <c r="AG49" s="15">
         <f t="shared" si="36"/>
         <v>3.5211912101471038E-2</v>
       </c>
+      <c r="AG49" s="15">
+        <f t="shared" si="37"/>
+        <v>3.5211912101471038E-2</v>
+      </c>
       <c r="AH49" s="15">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>4.9797163650989656E-2</v>
       </c>
       <c r="AI49" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>4.9797163650989656E-2</v>
       </c>
       <c r="AJ49" s="3">
@@ -11622,6 +11669,13 @@
         <f>180-147</f>
         <v>33</v>
       </c>
+      <c r="K51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L51" s="3">
+        <f>0.2/L52</f>
+        <v>2.1630832257659448E-2</v>
+      </c>
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
@@ -11631,18 +11685,25 @@
         <f>_xlfn.COT(RADIANS(B51))</f>
         <v>1.5398649638145827</v>
       </c>
+      <c r="K52" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L52" s="7">
+        <f>AVERAGE(N16:N27)</f>
+        <v>9.2460612526446031</v>
+      </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35" t="s">
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
     </row>
     <row r="55" spans="1:39" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">
@@ -11704,7 +11765,7 @@
         <v>11</v>
       </c>
       <c r="C57" s="9">
-        <f t="shared" ref="C57:C58" si="50">K43</f>
+        <f t="shared" ref="C57:C58" si="51">K43</f>
         <v>6.2834309171338068E-3</v>
       </c>
       <c r="D57" s="8">
@@ -11712,19 +11773,19 @@
         <v>10.633997454644252</v>
       </c>
       <c r="E57" s="8">
-        <f t="shared" ref="E57" si="51">O43</f>
+        <f t="shared" ref="E57" si="52">O43</f>
         <v>11.692307952536082</v>
       </c>
       <c r="F57" s="9">
-        <f t="shared" ref="F57:F59" si="52">2*K21</f>
+        <f t="shared" ref="F57:F59" si="53">2*K21</f>
         <v>9.4984640126648291E-3</v>
       </c>
       <c r="G57" s="7">
-        <f t="shared" ref="G57:G59" si="53">N21</f>
+        <f t="shared" ref="G57:G59" si="54">N21</f>
         <v>5.7043297604383083</v>
       </c>
       <c r="H57" s="7">
-        <f t="shared" ref="H57:H59" si="54">G57+8*F57^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
+        <f t="shared" ref="H57:H59" si="55">G57+8*F57^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
         <v>8.1227188682608311</v>
       </c>
     </row>
@@ -11736,27 +11797,27 @@
         <v>12</v>
       </c>
       <c r="C58" s="9">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>2.2165398829846967E-3</v>
       </c>
       <c r="D58" s="8">
-        <f t="shared" ref="D58:E58" si="55">N44</f>
+        <f t="shared" ref="D58:E58" si="56">N44</f>
         <v>12.41219901576854</v>
       </c>
       <c r="E58" s="8">
+        <f t="shared" si="56"/>
+        <v>12.543894388300366</v>
+      </c>
+      <c r="F58" s="9">
+        <f t="shared" si="53"/>
+        <v>5.8225878467728668E-3</v>
+      </c>
+      <c r="G58" s="8">
+        <f t="shared" si="54"/>
+        <v>10.352302157832483</v>
+      </c>
+      <c r="H58" s="8">
         <f t="shared" si="55"/>
-        <v>12.543894388300366</v>
-      </c>
-      <c r="F58" s="9">
-        <f t="shared" si="52"/>
-        <v>5.8225878467728668E-3</v>
-      </c>
-      <c r="G58" s="8">
-        <f t="shared" si="53"/>
-        <v>10.352302157832483</v>
-      </c>
-      <c r="H58" s="8">
-        <f t="shared" si="54"/>
         <v>11.261066993909452</v>
       </c>
     </row>
@@ -11772,23 +11833,23 @@
         <v>0</v>
       </c>
       <c r="D59" s="8">
-        <f t="shared" ref="D59:E59" si="56">N45</f>
+        <f t="shared" ref="D59:E59" si="57">N45</f>
         <v>12.500228796022217</v>
       </c>
       <c r="E59" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>12.500228796022217</v>
       </c>
       <c r="F59" s="13">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="G59" s="8">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>12.394593059717804</v>
       </c>
       <c r="H59" s="8">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>12.394593059717804</v>
       </c>
     </row>
@@ -11800,7 +11861,7 @@
         <v>10</v>
       </c>
       <c r="C60" s="27">
-        <f t="shared" ref="C60:C63" si="57">K46</f>
+        <f t="shared" ref="C60:C63" si="58">K46</f>
         <v>5.5835565479854053E-3</v>
       </c>
       <c r="D60" s="7">
@@ -11808,7 +11869,7 @@
         <v>8.3100112559471651</v>
       </c>
       <c r="E60" s="8">
-        <f t="shared" ref="E60" si="58">O46</f>
+        <f t="shared" ref="E60" si="59">O46</f>
         <v>9.1456936498984369</v>
       </c>
       <c r="F60" s="9">
@@ -11832,27 +11893,27 @@
         <v>11</v>
       </c>
       <c r="C61" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>5.4485694666055393E-3</v>
       </c>
       <c r="D61" s="7">
-        <f t="shared" ref="D61:E61" si="59">N47</f>
+        <f t="shared" ref="D61:E61" si="60">N47</f>
         <v>9.6480639158030641</v>
       </c>
       <c r="E61" s="8">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>10.443828120193732</v>
       </c>
       <c r="F61" s="9">
-        <f t="shared" ref="F61:F63" si="60">K21</f>
+        <f t="shared" ref="F61:F63" si="61">K21</f>
         <v>4.7492320063324146E-3</v>
       </c>
       <c r="G61" s="8">
-        <f t="shared" ref="G61:G63" si="61">2*N21</f>
+        <f t="shared" ref="G61:G63" si="62">2*N21</f>
         <v>11.408659520876617</v>
       </c>
       <c r="H61" s="8">
-        <f t="shared" ref="H61:H63" si="62">G61+8*F61^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
+        <f t="shared" ref="H61:H63" si="63">G61+8*F61^2/(PI()^2*$B$6^4*9.81)*(1-($B$6/$B$5)^4)</f>
         <v>12.013256797832247</v>
       </c>
     </row>
@@ -11864,27 +11925,27 @@
         <v>12</v>
       </c>
       <c r="C62" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>2.9829457646423892E-3</v>
       </c>
       <c r="D62" s="8">
-        <f t="shared" ref="D62:E62" si="63">N48</f>
+        <f t="shared" ref="D62:E62" si="64">N48</f>
         <v>21.655325942404687</v>
       </c>
       <c r="E62" s="8">
+        <f t="shared" si="64"/>
+        <v>21.893837884806008</v>
+      </c>
+      <c r="F62" s="9">
+        <f t="shared" si="61"/>
+        <v>2.9112939233864334E-3</v>
+      </c>
+      <c r="G62" s="3">
+        <f t="shared" si="62"/>
+        <v>20.704604315664966</v>
+      </c>
+      <c r="H62" s="8">
         <f t="shared" si="63"/>
-        <v>21.893837884806008</v>
-      </c>
-      <c r="F62" s="9">
-        <f t="shared" si="60"/>
-        <v>2.9112939233864334E-3</v>
-      </c>
-      <c r="G62" s="3">
-        <f t="shared" si="61"/>
-        <v>20.704604315664966</v>
-      </c>
-      <c r="H62" s="8">
-        <f t="shared" si="62"/>
         <v>20.931795524684208</v>
       </c>
     </row>
@@ -11896,27 +11957,27 @@
         <v>13</v>
       </c>
       <c r="C63" s="13">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="D63" s="8">
-        <f t="shared" ref="D63:E63" si="64">N49</f>
+        <f t="shared" ref="D63:E63" si="65">N49</f>
         <v>24.89482185574002</v>
       </c>
       <c r="E63" s="8">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>24.89482185574002</v>
       </c>
       <c r="F63" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="G63" s="8">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>24.789186119435609</v>
       </c>
       <c r="H63" s="8">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>24.789186119435609</v>
       </c>
     </row>
@@ -12040,11 +12101,11 @@
         <v>0.108</v>
       </c>
       <c r="C68" s="22">
-        <f t="shared" ref="C68:C86" si="65">$B$8</f>
+        <f t="shared" ref="C68:C86" si="66">$B$8</f>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D68" s="3">
-        <f t="shared" ref="D68:D86" si="66">$B$9</f>
+        <f t="shared" ref="D68:D86" si="67">$B$9</f>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E68" s="10">
@@ -12060,19 +12121,19 @@
         <v>71</v>
       </c>
       <c r="I68" s="8">
-        <f t="shared" ref="I68:I106" si="67">B68/2*F68*2*PI()/60</f>
+        <f t="shared" ref="I68:I106" si="68">B68/2*F68*2*PI()/60</f>
         <v>20.357520395261862</v>
       </c>
       <c r="J68" s="14">
-        <f t="shared" ref="J68:J106" si="68">E68/(C68*(2*PI()*B68/2-$B$10*D68))</f>
+        <f t="shared" ref="J68:J106" si="69">E68/(C68*(2*PI()*B68/2-$B$10*D68))</f>
         <v>2.5083035523885377</v>
       </c>
       <c r="K68" s="7">
-        <f t="shared" ref="K68:K106" si="69">G68*9.81/I68^2</f>
+        <f t="shared" ref="K68:K106" si="70">G68*9.81/I68^2</f>
         <v>0.38110542089750205</v>
       </c>
       <c r="L68" s="7">
-        <f t="shared" ref="L68:L106" si="70">J68/I68</f>
+        <f t="shared" ref="L68:L106" si="71">J68/I68</f>
         <v>0.123212626277036</v>
       </c>
     </row>
@@ -12084,11 +12145,11 @@
         <v>0.108</v>
       </c>
       <c r="C69" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D69" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E69" s="10">
@@ -12104,19 +12165,19 @@
         <v>73</v>
       </c>
       <c r="I69" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J69" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.0216177884922546</v>
       </c>
       <c r="K69" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.45922019660941232</v>
       </c>
       <c r="L69" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>9.9305698790446928E-2</v>
       </c>
       <c r="M69" s="8"/>
@@ -12130,11 +12191,11 @@
         <v>0.108</v>
       </c>
       <c r="C70" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D70" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E70" s="30">
@@ -12150,19 +12211,19 @@
         <v>69</v>
       </c>
       <c r="I70" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J70" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.4974946581424107</v>
       </c>
       <c r="K70" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.51129671375068597</v>
       </c>
       <c r="L70" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>7.3559776881812533E-2</v>
       </c>
       <c r="M70" s="8"/>
@@ -12176,11 +12237,11 @@
         <v>0.108</v>
       </c>
       <c r="C71" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D71" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E71" s="30">
@@ -12196,19 +12257,19 @@
         <v>59</v>
       </c>
       <c r="I71" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J71" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.0108088942461273</v>
       </c>
       <c r="K71" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.53970208673683517</v>
       </c>
       <c r="L71" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>4.9652849395223464E-2</v>
       </c>
       <c r="M71" s="8"/>
@@ -12222,11 +12283,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C72" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D72" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E72" s="10">
@@ -12242,19 +12303,19 @@
         <v>47</v>
       </c>
       <c r="I72" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J72" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>3.0381988876492994</v>
       </c>
       <c r="K72" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.2096493445655927</v>
       </c>
       <c r="L72" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.15802103629597514</v>
       </c>
       <c r="M72" s="8"/>
@@ -12268,11 +12329,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C73" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D73" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E73" s="10">
@@ -12288,19 +12349,19 @@
         <v>66</v>
       </c>
       <c r="I73" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J73" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.518506972656656</v>
       </c>
       <c r="K73" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.34499259232312718</v>
       </c>
       <c r="L73" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.13099112219271625</v>
       </c>
       <c r="M73" s="8"/>
@@ -12314,11 +12375,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C74" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D74" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E74" s="10">
@@ -12334,19 +12395,19 @@
         <v>69</v>
       </c>
       <c r="I74" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J74" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.9988150576640129</v>
       </c>
       <c r="K74" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.43256763498976725</v>
       </c>
       <c r="L74" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.10396120808945734</v>
       </c>
       <c r="M74" s="8"/>
@@ -12360,11 +12421,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C75" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D75" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E75" s="10">
@@ -12380,19 +12441,19 @@
         <v>64</v>
       </c>
       <c r="I75" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J75" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.5190994438246497</v>
       </c>
       <c r="K75" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.47768205090894539</v>
       </c>
       <c r="L75" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>7.9010518147987568E-2</v>
       </c>
       <c r="M75" s="8"/>
@@ -12406,11 +12467,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C76" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D76" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E76" s="10">
@@ -12426,19 +12487,19 @@
         <v>54</v>
       </c>
       <c r="I76" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J76" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.99940752883200645</v>
       </c>
       <c r="K76" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.50952752096954168</v>
       </c>
       <c r="L76" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>5.1980604044728672E-2</v>
       </c>
       <c r="M76" s="8"/>
@@ -12452,11 +12513,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C77" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D77" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E77" s="10">
@@ -12472,19 +12533,19 @@
         <v>45</v>
       </c>
       <c r="I77" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J77" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>3.0448109727843837</v>
       </c>
       <c r="K77" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.19922596561183958</v>
       </c>
       <c r="L77" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.16826274899273511</v>
       </c>
       <c r="M77" s="8"/>
@@ -12498,11 +12559,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C78" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D78" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E78" s="10">
@@ -12518,19 +12579,19 @@
         <v>62</v>
       </c>
       <c r="I78" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J78" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.5301950337222343</v>
       </c>
       <c r="K78" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.32954671003462188</v>
       </c>
       <c r="L78" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.13982397451508971</v>
       </c>
       <c r="M78" s="8"/>
@@ -12544,11 +12605,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C79" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D79" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E79" s="30">
@@ -12564,19 +12625,19 @@
         <v>65</v>
       </c>
       <c r="I79" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J79" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.0155790946600849</v>
       </c>
       <c r="K79" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.41642720631647673</v>
       </c>
       <c r="L79" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.11138520003744436</v>
       </c>
       <c r="M79" s="8"/>
@@ -12590,11 +12651,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C80" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D80" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E80" s="10">
@@ -12610,19 +12671,19 @@
         <v>60</v>
       </c>
       <c r="I80" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J80" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.5009631555979355</v>
       </c>
       <c r="K80" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.47334891077700236</v>
       </c>
       <c r="L80" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.2946425559798975E-2</v>
       </c>
       <c r="M80" s="8"/>
@@ -12636,11 +12697,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C81" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D81" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E81" s="10">
@@ -12656,19 +12717,19 @@
         <v>52</v>
       </c>
       <c r="I81" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J81" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.0292318781242986</v>
       </c>
       <c r="K81" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.50330770259833157</v>
       </c>
       <c r="L81" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>5.6877548955290728E-2</v>
       </c>
       <c r="M81" s="8"/>
@@ -12682,11 +12743,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C82" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D82" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E82" s="10">
@@ -12702,19 +12763,19 @@
         <v>24</v>
       </c>
       <c r="I82" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J82" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>3.0036608329602066</v>
       </c>
       <c r="K82" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.10300153568634084</v>
       </c>
       <c r="L82" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.19198693531611913</v>
       </c>
       <c r="M82" s="8"/>
@@ -12728,11 +12789,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C83" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D83" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E83" s="10">
@@ -12748,19 +12809,19 @@
         <v>43</v>
       </c>
       <c r="I83" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J83" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.4945657765262732</v>
       </c>
       <c r="K83" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.23846659040222878</v>
       </c>
       <c r="L83" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.15944677678796335</v>
       </c>
       <c r="M83" s="8"/>
@@ -12774,11 +12835,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C84" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D84" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E84" s="10">
@@ -12794,19 +12855,19 @@
         <v>53</v>
       </c>
       <c r="I84" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J84" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.98547072009234</v>
       </c>
       <c r="K84" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.33705950004752</v>
       </c>
       <c r="L84" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.12690661825980756</v>
       </c>
       <c r="M84" s="8"/>
@@ -12820,11 +12881,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C85" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D85" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E85" s="10">
@@ -12840,19 +12901,19 @@
         <v>51</v>
       </c>
       <c r="I85" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J85" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.4763756636584067</v>
       </c>
       <c r="K85" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.39717712788001464</v>
       </c>
       <c r="L85" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>9.4366459731651781E-2</v>
       </c>
       <c r="M85" s="8"/>
@@ -12866,11 +12927,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C86" s="22">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D86" s="3">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E86" s="10">
@@ -12886,19 +12947,19 @@
         <v>38</v>
       </c>
       <c r="I86" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J86" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.0181901128678668</v>
       </c>
       <c r="K86" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.42082339482746262</v>
       </c>
       <c r="L86" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>6.5080317056311579E-2</v>
       </c>
     </row>
@@ -12930,19 +12991,19 @@
         <v>52</v>
       </c>
       <c r="I87" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J87" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.9949893162848213</v>
       </c>
       <c r="K87" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.24381278479778079</v>
       </c>
       <c r="L87" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.14711955376362507</v>
       </c>
     </row>
@@ -12954,11 +13015,11 @@
         <v>0.108</v>
       </c>
       <c r="C88" s="22">
-        <f t="shared" ref="C88:C106" si="71">$B$8*B88/$B$7</f>
+        <f t="shared" ref="C88:C106" si="72">$B$8*B88/$B$7</f>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D88" s="3">
-        <f t="shared" ref="D88:D91" si="72">$B$9*B88/$B$7</f>
+        <f t="shared" ref="D88:D91" si="73">$B$9*B88/$B$7</f>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E88" s="10">
@@ -12974,19 +13035,19 @@
         <v>71</v>
       </c>
       <c r="I88" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J88" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.5083035523885377</v>
       </c>
       <c r="K88" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.38110542089750205</v>
       </c>
       <c r="L88" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.123212626277036</v>
       </c>
     </row>
@@ -12998,11 +13059,11 @@
         <v>0.108</v>
       </c>
       <c r="C89" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D89" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E89" s="10">
@@ -13018,19 +13079,19 @@
         <v>73</v>
       </c>
       <c r="I89" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J89" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.0216177884922546</v>
       </c>
       <c r="K89" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.45922019660941232</v>
       </c>
       <c r="L89" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>9.9305698790446928E-2</v>
       </c>
     </row>
@@ -13042,11 +13103,11 @@
         <v>0.108</v>
       </c>
       <c r="C90" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D90" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E90" s="30">
@@ -13066,15 +13127,15 @@
         <v>20.357520395261862</v>
       </c>
       <c r="J90" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.4974946581424107</v>
       </c>
       <c r="K90" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.51129671375068597</v>
       </c>
       <c r="L90" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>7.3559776881812533E-2</v>
       </c>
     </row>
@@ -13086,11 +13147,11 @@
         <v>0.108</v>
       </c>
       <c r="C91" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="D91" s="3">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="E91" s="30">
@@ -13106,19 +13167,19 @@
         <v>59</v>
       </c>
       <c r="I91" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>20.357520395261862</v>
       </c>
       <c r="J91" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.0108088942461273</v>
       </c>
       <c r="K91" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.53970208673683517</v>
       </c>
       <c r="L91" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>4.9652849395223464E-2</v>
       </c>
     </row>
@@ -13130,11 +13191,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C92" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D92" s="3">
-        <f t="shared" ref="D92:D106" si="73">$B$9*B92/$B$7</f>
+        <f t="shared" ref="D92:D106" si="74">$B$9*B92/$B$7</f>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E92" s="10">
@@ -13150,19 +13211,19 @@
         <v>47</v>
       </c>
       <c r="I92" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J92" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>3.1898190711158065</v>
       </c>
       <c r="K92" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.2096493445655927</v>
       </c>
       <c r="L92" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.16590701723427406</v>
       </c>
     </row>
@@ -13174,11 +13235,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C93" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D93" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E93" s="10">
@@ -13194,19 +13255,19 @@
         <v>66</v>
       </c>
       <c r="I93" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J93" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.6441921247407345</v>
       </c>
       <c r="K93" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.34499259232312718</v>
       </c>
       <c r="L93" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.13752818533893771</v>
       </c>
     </row>
@@ -13218,11 +13279,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C94" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D94" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E94" s="10">
@@ -13238,19 +13299,19 @@
         <v>69</v>
       </c>
       <c r="I94" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J94" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.0985651783656625</v>
       </c>
       <c r="K94" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.43256763498976725</v>
       </c>
       <c r="L94" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.10914935344360137</v>
       </c>
     </row>
@@ -13262,11 +13323,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C95" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D95" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E95" s="10">
@@ -13282,19 +13343,19 @@
         <v>64</v>
       </c>
       <c r="I95" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J95" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.5949095355579033</v>
       </c>
       <c r="K95" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.47768205090894539</v>
       </c>
       <c r="L95" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.2953508617137031E-2</v>
       </c>
     </row>
@@ -13306,11 +13367,11 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C96" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="D96" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>8.0277777777777778E-3</v>
       </c>
       <c r="E96" s="10">
@@ -13326,19 +13387,19 @@
         <v>54</v>
       </c>
       <c r="I96" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
       <c r="J96" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.0492825891828312</v>
       </c>
       <c r="K96" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.50952752096954168</v>
       </c>
       <c r="L96" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>5.4574676721800684E-2</v>
       </c>
     </row>
@@ -13350,11 +13411,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C97" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D97" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E97" s="10">
@@ -13370,19 +13431,19 @@
         <v>45</v>
       </c>
       <c r="I97" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J97" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>3.3640983511628928</v>
       </c>
       <c r="K97" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.19922596561183958</v>
       </c>
       <c r="L97" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.18590725056766289</v>
       </c>
     </row>
@@ -13394,11 +13455,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C98" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D98" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E98" s="10">
@@ -13414,19 +13475,19 @@
         <v>62</v>
       </c>
       <c r="I98" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J98" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.7955183481494461</v>
       </c>
       <c r="K98" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.32954671003462188</v>
       </c>
       <c r="L98" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.15448630680974804</v>
       </c>
     </row>
@@ -13438,11 +13499,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C99" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D99" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E99" s="30">
@@ -13458,19 +13519,19 @@
         <v>65</v>
       </c>
       <c r="I99" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J99" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.2269383451359994</v>
       </c>
       <c r="K99" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.41642720631647673</v>
       </c>
       <c r="L99" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.12306536305183319</v>
       </c>
     </row>
@@ -13482,11 +13543,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C100" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D100" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E100" s="10">
@@ -13502,19 +13563,19 @@
         <v>60</v>
       </c>
       <c r="I100" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J100" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.6583583421225527</v>
       </c>
       <c r="K100" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.47334891077700236</v>
       </c>
       <c r="L100" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>9.1644419293918325E-2</v>
       </c>
     </row>
@@ -13526,11 +13587,11 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C101" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D101" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>7.5555555555555567E-3</v>
       </c>
       <c r="E101" s="10">
@@ -13546,19 +13607,19 @@
         <v>52</v>
       </c>
       <c r="I101" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>18.095573684677209</v>
       </c>
       <c r="J101" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1371600060268932</v>
       </c>
       <c r="K101" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.50330770259833157</v>
       </c>
       <c r="L101" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>6.2841887515829697E-2</v>
       </c>
     </row>
@@ -13570,11 +13631,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C102" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D102" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E102" s="10">
@@ -13590,19 +13651,19 @@
         <v>24</v>
       </c>
       <c r="I102" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J102" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>3.7398021623668587</v>
       </c>
       <c r="K102" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.10300153568634084</v>
       </c>
       <c r="L102" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.23903935756082109</v>
       </c>
     </row>
@@ -13614,11 +13675,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C103" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D103" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E103" s="10">
@@ -13634,19 +13695,19 @@
         <v>43</v>
       </c>
       <c r="I103" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J103" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>3.1059373890843402</v>
       </c>
       <c r="K103" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.23846659040222878</v>
       </c>
       <c r="L103" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.19852421221152938</v>
       </c>
     </row>
@@ -13658,11 +13719,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C104" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D104" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E104" s="10">
@@ -13678,19 +13739,19 @@
         <v>53</v>
       </c>
       <c r="I104" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J104" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>2.4720726158018218</v>
       </c>
       <c r="K104" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.33705950004752</v>
       </c>
       <c r="L104" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.15800906686223767</v>
       </c>
     </row>
@@ -13702,11 +13763,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C105" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D105" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E105" s="10">
@@ -13722,19 +13783,19 @@
         <v>51</v>
       </c>
       <c r="I105" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J105" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.8382078425193034</v>
       </c>
       <c r="K105" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.39717712788001464</v>
       </c>
       <c r="L105" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.11749392151294595</v>
       </c>
     </row>
@@ -13746,11 +13807,11 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="C106" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>6.9166666666666682E-3</v>
       </c>
       <c r="D106" s="3">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>6.5324074074074078E-3</v>
       </c>
       <c r="E106" s="10">
@@ -13766,19 +13827,19 @@
         <v>38</v>
       </c>
       <c r="I106" s="8">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>15.64513141487717</v>
       </c>
       <c r="J106" s="14">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.2677295465650369</v>
       </c>
       <c r="K106" s="7">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.42082339482746262</v>
       </c>
       <c r="L106" s="7">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>8.1030290698583418E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add table of contents to bibliography in main.tex
</commit_message>
<xml_diff>
--- a/Lab 1 - Pumps/data_and_analysis.xlsx
+++ b/Lab 1 - Pumps/data_and_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\LaTeX\MEC-E-403\Lab 1 - Pumps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C39409-D381-4BEC-A56F-65F94C346794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D42F7C7-9DEF-47AA-BEE5-2566452A6C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,13 +534,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -935,41 +935,41 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="G13" s="37" t="s">
+      <c r="E13" s="37"/>
+      <c r="G13" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="L13" s="39" t="s">
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="L13" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="39"/>
+      <c r="M13" s="37"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="37" t="s">
+      <c r="Z13" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="37" t="s">
+      <c r="AA13" s="38"/>
+      <c r="AB13" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="37"/>
-      <c r="AD13" s="37" t="s">
+      <c r="AC13" s="38"/>
+      <c r="AD13" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="37"/>
-      <c r="AF13" s="37" t="s">
+      <c r="AE13" s="38"/>
+      <c r="AF13" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="37"/>
+      <c r="AG13" s="38"/>
     </row>
     <row r="14" spans="1:39" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -990,11 +990,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -6010,8 +6010,8 @@
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
-      <c r="K50" s="37"/>
-      <c r="L50" s="37"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38"/>
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
     </row>
@@ -6036,8 +6036,8 @@
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="37"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
       <c r="M52" s="8"/>
       <c r="N52" s="8"/>
     </row>
@@ -6084,37 +6084,37 @@
       <c r="N58" s="8"/>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A59" s="39"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="K59" s="37"/>
-      <c r="L59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="K59" s="38"/>
+      <c r="L59" s="38"/>
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A60" s="39"/>
-      <c r="B60" s="37"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="38"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
       <c r="M60" s="8"/>
       <c r="N60" s="8"/>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A61" s="39"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="K61" s="37"/>
-      <c r="L61" s="37"/>
+      <c r="A61" s="37"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+      <c r="K61" s="38"/>
+      <c r="L61" s="38"/>
       <c r="M61" s="8"/>
       <c r="N61" s="8"/>
     </row>
@@ -6136,14 +6136,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="F59:H60"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="K61:L61"/>
     <mergeCell ref="AF13:AG13"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="K50:L50"/>
@@ -6154,6 +6146,14 @@
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
     <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="F59:H60"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="K61:L61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6164,8 +6164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B530A311-2D6F-44F7-871F-14AF58E6CD82}">
   <dimension ref="A1:AR111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N35" sqref="N34:N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6351,41 +6351,41 @@
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="G13" s="37" t="s">
+      <c r="E13" s="37"/>
+      <c r="G13" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="L13" s="39" t="s">
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="L13" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="39"/>
+      <c r="M13" s="37"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="37" t="s">
+      <c r="Z13" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="37" t="s">
+      <c r="AA13" s="38"/>
+      <c r="AB13" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="37"/>
-      <c r="AD13" s="37" t="s">
+      <c r="AC13" s="38"/>
+      <c r="AD13" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="37"/>
-      <c r="AF13" s="37" t="s">
+      <c r="AE13" s="38"/>
+      <c r="AF13" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="37"/>
+      <c r="AG13" s="38"/>
       <c r="AO13" s="3" t="s">
         <v>83</v>
       </c>
@@ -6409,11 +6409,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>0.809873659825466</v>
       </c>
       <c r="AR17" s="33">
-        <f t="shared" ref="AR17:AR27" si="25">AO29-AO17</f>
+        <f t="shared" ref="AR17:AR26" si="25">AO29-AO17</f>
         <v>26.593009544396402</v>
       </c>
     </row>
@@ -11694,16 +11694,16 @@
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C54" s="37" t="s">
+      <c r="C54" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37" t="s">
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
     </row>
     <row r="55" spans="1:39" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">

</xml_diff>

<commit_message>
Update pump diagrams and improve documentation
</commit_message>
<xml_diff>
--- a/Lab 1 - Pumps/data_and_analysis.xlsx
+++ b/Lab 1 - Pumps/data_and_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\LaTeX\MEC-E-403\Lab 1 - Pumps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDD71B6-9DED-4B6C-846E-72F66594169E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543E12A2-95D4-4204-A576-D94244FC2FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alex analysis" sheetId="5" r:id="rId1"/>
@@ -531,15 +531,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -555,6 +546,15 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,45 +773,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B530A311-2D6F-44F7-871F-14AF58E6CD82}">
   <dimension ref="A1:AR111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K81" sqref="K81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="13.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="14" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="3" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="3" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" style="3" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" style="3" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="21.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="22" style="3" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="3" hidden="1" customWidth="1"/>
-    <col min="30" max="31" width="14" style="3" hidden="1" customWidth="1"/>
-    <col min="32" max="33" width="13.5703125" style="3" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="8.28515625" style="3" hidden="1" customWidth="1"/>
+    <col min="26" max="27" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11" style="3" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="19.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -962,41 +960,41 @@
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="G13" s="35" t="s">
+      <c r="E13" s="43"/>
+      <c r="G13" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="L13" s="37" t="s">
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="L13" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="37"/>
+      <c r="M13" s="43"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="35" t="s">
+      <c r="Z13" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35" t="s">
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35" t="s">
+      <c r="AC13" s="42"/>
+      <c r="AD13" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="35"/>
-      <c r="AF13" s="35" t="s">
+      <c r="AE13" s="42"/>
+      <c r="AF13" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="35"/>
+      <c r="AG13" s="42"/>
       <c r="AO13" s="3" t="s">
         <v>83</v>
       </c>
@@ -1020,11 +1018,11 @@
       <c r="F14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="17" t="s">
         <v>23</v>
       </c>
@@ -6305,16 +6303,16 @@
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35" t="s">
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:39" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C55" s="16" t="s">
@@ -6886,78 +6884,78 @@
       <c r="M71" s="7"/>
       <c r="N71" s="7"/>
     </row>
-    <row r="72" spans="1:41" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="38" t="s">
+    <row r="72" spans="1:41" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B72" s="39">
+      <c r="B72" s="36">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C72" s="40">
+      <c r="C72" s="37">
         <f t="shared" si="66"/>
         <v>9.0000000000000011E-3</v>
       </c>
-      <c r="D72" s="39">
+      <c r="D72" s="36">
         <f t="shared" si="67"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="E72" s="40">
+      <c r="E72" s="37">
         <v>7.6E-3</v>
       </c>
-      <c r="F72" s="39">
+      <c r="F72" s="36">
         <v>3600</v>
       </c>
-      <c r="G72" s="41">
+      <c r="G72" s="38">
         <v>7.9</v>
       </c>
-      <c r="H72" s="39">
+      <c r="H72" s="36">
         <v>47</v>
       </c>
-      <c r="I72" s="41">
+      <c r="I72" s="38">
         <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J72" s="42">
+      <c r="J72" s="39">
         <f t="shared" si="69"/>
         <v>3.0381988876492994</v>
       </c>
-      <c r="K72" s="43">
+      <c r="K72" s="40">
         <f t="shared" si="70"/>
         <v>0.2096493445655927</v>
       </c>
-      <c r="L72" s="43">
+      <c r="L72" s="40">
         <f t="shared" si="71"/>
         <v>0.15802103629597514</v>
       </c>
-      <c r="M72" s="41"/>
-      <c r="N72" s="41"/>
-      <c r="O72" s="39"/>
-      <c r="P72" s="39"/>
-      <c r="Q72" s="39"/>
-      <c r="R72" s="39"/>
-      <c r="S72" s="39"/>
-      <c r="T72" s="39"/>
-      <c r="U72" s="39"/>
-      <c r="V72" s="39"/>
-      <c r="W72" s="39"/>
-      <c r="X72" s="39"/>
-      <c r="Y72" s="39"/>
-      <c r="Z72" s="39"/>
-      <c r="AA72" s="39"/>
-      <c r="AB72" s="39"/>
-      <c r="AC72" s="39"/>
-      <c r="AD72" s="39"/>
-      <c r="AE72" s="39"/>
-      <c r="AF72" s="39"/>
-      <c r="AG72" s="39"/>
-      <c r="AH72" s="39"/>
-      <c r="AI72" s="39"/>
-      <c r="AJ72" s="39"/>
-      <c r="AK72" s="39"/>
-      <c r="AL72" s="39"/>
-      <c r="AM72" s="39"/>
-      <c r="AN72" s="39"/>
-      <c r="AO72" s="39"/>
+      <c r="M72" s="38"/>
+      <c r="N72" s="38"/>
+      <c r="O72" s="36"/>
+      <c r="P72" s="36"/>
+      <c r="Q72" s="36"/>
+      <c r="R72" s="36"/>
+      <c r="S72" s="36"/>
+      <c r="T72" s="36"/>
+      <c r="U72" s="36"/>
+      <c r="V72" s="36"/>
+      <c r="W72" s="36"/>
+      <c r="X72" s="36"/>
+      <c r="Y72" s="36"/>
+      <c r="Z72" s="36"/>
+      <c r="AA72" s="36"/>
+      <c r="AB72" s="36"/>
+      <c r="AC72" s="36"/>
+      <c r="AD72" s="36"/>
+      <c r="AE72" s="36"/>
+      <c r="AF72" s="36"/>
+      <c r="AG72" s="36"/>
+      <c r="AH72" s="36"/>
+      <c r="AI72" s="36"/>
+      <c r="AJ72" s="36"/>
+      <c r="AK72" s="36"/>
+      <c r="AL72" s="36"/>
+      <c r="AM72" s="36"/>
+      <c r="AN72" s="36"/>
+      <c r="AO72" s="36"/>
     </row>
     <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
@@ -7821,78 +7819,78 @@
         <v>4.9652849395223464E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:41" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="38" t="s">
+    <row r="92" spans="1:41" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="39">
+      <c r="B92" s="36">
         <v>0.10199999999999999</v>
       </c>
-      <c r="C92" s="40">
+      <c r="C92" s="37">
         <f t="shared" si="72"/>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="D92" s="39">
+      <c r="D92" s="36">
         <f t="shared" ref="D92:D106" si="74">$B$9*B92/$B$7</f>
         <v>8.0277777777777778E-3</v>
       </c>
-      <c r="E92" s="40">
+      <c r="E92" s="37">
         <v>7.6E-3</v>
       </c>
-      <c r="F92" s="39">
+      <c r="F92" s="36">
         <v>3600</v>
       </c>
-      <c r="G92" s="41">
+      <c r="G92" s="38">
         <v>7.9</v>
       </c>
-      <c r="H92" s="39">
+      <c r="H92" s="36">
         <v>47</v>
       </c>
-      <c r="I92" s="41">
+      <c r="I92" s="38">
         <f t="shared" si="68"/>
         <v>19.226547039969535</v>
       </c>
-      <c r="J92" s="42">
-        <f t="shared" si="69"/>
+      <c r="J92" s="39">
+        <f>E92/(C92*(2*PI()*B92/2-$B$10*D92))</f>
         <v>3.1898190711158065</v>
       </c>
-      <c r="K92" s="43">
-        <f t="shared" si="70"/>
+      <c r="K92" s="40">
+        <f>G92*9.81/I92^2</f>
         <v>0.2096493445655927</v>
       </c>
-      <c r="L92" s="43">
-        <f t="shared" si="71"/>
+      <c r="L92" s="40">
+        <f>J92/I92</f>
         <v>0.16590701723427406</v>
       </c>
-      <c r="M92" s="39"/>
-      <c r="N92" s="39"/>
-      <c r="O92" s="39"/>
-      <c r="P92" s="39"/>
-      <c r="Q92" s="39"/>
-      <c r="R92" s="39"/>
-      <c r="S92" s="39"/>
-      <c r="T92" s="39"/>
-      <c r="U92" s="39"/>
-      <c r="V92" s="39"/>
-      <c r="W92" s="39"/>
-      <c r="X92" s="39"/>
-      <c r="Y92" s="39"/>
-      <c r="Z92" s="39"/>
-      <c r="AA92" s="39"/>
-      <c r="AB92" s="39"/>
-      <c r="AC92" s="39"/>
-      <c r="AD92" s="39"/>
-      <c r="AE92" s="39"/>
-      <c r="AF92" s="39"/>
-      <c r="AG92" s="39"/>
-      <c r="AH92" s="39"/>
-      <c r="AI92" s="39"/>
-      <c r="AJ92" s="39"/>
-      <c r="AK92" s="39"/>
-      <c r="AL92" s="39"/>
-      <c r="AM92" s="39"/>
-      <c r="AN92" s="39"/>
-      <c r="AO92" s="39"/>
+      <c r="M92" s="36"/>
+      <c r="N92" s="36"/>
+      <c r="O92" s="36"/>
+      <c r="P92" s="36"/>
+      <c r="Q92" s="36"/>
+      <c r="R92" s="36"/>
+      <c r="S92" s="36"/>
+      <c r="T92" s="36"/>
+      <c r="U92" s="36"/>
+      <c r="V92" s="36"/>
+      <c r="W92" s="36"/>
+      <c r="X92" s="36"/>
+      <c r="Y92" s="36"/>
+      <c r="Z92" s="36"/>
+      <c r="AA92" s="36"/>
+      <c r="AB92" s="36"/>
+      <c r="AC92" s="36"/>
+      <c r="AD92" s="36"/>
+      <c r="AE92" s="36"/>
+      <c r="AF92" s="36"/>
+      <c r="AG92" s="36"/>
+      <c r="AH92" s="36"/>
+      <c r="AI92" s="36"/>
+      <c r="AJ92" s="36"/>
+      <c r="AK92" s="36"/>
+      <c r="AL92" s="36"/>
+      <c r="AM92" s="36"/>
+      <c r="AN92" s="36"/>
+      <c r="AO92" s="36"/>
     </row>
     <row r="93" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">

</xml_diff>